<commit_message>
Plantilla Report add file type option "PDF"
</commit_message>
<xml_diff>
--- a/public/CSC_PLANTILLA.xlsx
+++ b/public/CSC_PLANTILLA.xlsx
@@ -598,7 +598,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="000\-000\-000"/>
   </numFmts>
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="25">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1369,23 +1369,40 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="164" fontId="13" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -1416,35 +1433,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" indent="7"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1479,13 +1475,19 @@
     <xf numFmtId="0" fontId="5" fillId="11" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="23" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -3123,11 +3125,11 @@
   </sheetPr>
   <dimension ref="A1:AB70"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="70" zoomScaleNormal="130" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <selection activeCell="AL49" sqref="AL49"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A2" zoomScale="145" zoomScaleNormal="130" zoomScaleSheetLayoutView="145" workbookViewId="0">
+      <selection activeCell="P15" sqref="P15:AB25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="4.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="19.5703125" style="1" hidden="1" customWidth="1"/>
@@ -3177,135 +3179,135 @@
     <col min="54" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="120" t="s">
+    <row r="1" spans="1:28" ht="15">
+      <c r="A1" s="125" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="120"/>
-      <c r="C1" s="120"/>
-      <c r="D1" s="120"/>
-      <c r="E1" s="120"/>
-      <c r="F1" s="120"/>
-      <c r="G1" s="120"/>
-      <c r="H1" s="120"/>
-      <c r="I1" s="120"/>
-      <c r="J1" s="120"/>
-      <c r="K1" s="120"/>
-      <c r="L1" s="120"/>
-      <c r="M1" s="120"/>
-      <c r="N1" s="120"/>
-      <c r="O1" s="120"/>
-      <c r="P1" s="120"/>
-      <c r="Q1" s="120"/>
-      <c r="R1" s="120"/>
-      <c r="S1" s="120"/>
-      <c r="T1" s="120"/>
-      <c r="U1" s="120"/>
-      <c r="V1" s="120"/>
-      <c r="W1" s="120"/>
-      <c r="X1" s="120"/>
-      <c r="Y1" s="120"/>
-      <c r="Z1" s="120"/>
-      <c r="AA1" s="120"/>
-      <c r="AB1" s="120"/>
-    </row>
-    <row r="2" spans="1:28" ht="15" x14ac:dyDescent="0.2">
-      <c r="A2" s="120" t="s">
+      <c r="B1" s="125"/>
+      <c r="C1" s="125"/>
+      <c r="D1" s="125"/>
+      <c r="E1" s="125"/>
+      <c r="F1" s="125"/>
+      <c r="G1" s="125"/>
+      <c r="H1" s="125"/>
+      <c r="I1" s="125"/>
+      <c r="J1" s="125"/>
+      <c r="K1" s="125"/>
+      <c r="L1" s="125"/>
+      <c r="M1" s="125"/>
+      <c r="N1" s="125"/>
+      <c r="O1" s="125"/>
+      <c r="P1" s="125"/>
+      <c r="Q1" s="125"/>
+      <c r="R1" s="125"/>
+      <c r="S1" s="125"/>
+      <c r="T1" s="125"/>
+      <c r="U1" s="125"/>
+      <c r="V1" s="125"/>
+      <c r="W1" s="125"/>
+      <c r="X1" s="125"/>
+      <c r="Y1" s="125"/>
+      <c r="Z1" s="125"/>
+      <c r="AA1" s="125"/>
+      <c r="AB1" s="125"/>
+    </row>
+    <row r="2" spans="1:28" ht="15">
+      <c r="A2" s="125" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="120"/>
-      <c r="C2" s="120"/>
-      <c r="D2" s="120"/>
-      <c r="E2" s="120"/>
-      <c r="F2" s="120"/>
-      <c r="G2" s="120"/>
-      <c r="H2" s="120"/>
-      <c r="I2" s="120"/>
-      <c r="J2" s="120"/>
-      <c r="K2" s="120"/>
-      <c r="L2" s="120"/>
-      <c r="M2" s="120"/>
-      <c r="N2" s="120"/>
-      <c r="O2" s="120"/>
-      <c r="P2" s="120"/>
-      <c r="Q2" s="120"/>
-      <c r="R2" s="120"/>
-      <c r="S2" s="120"/>
-      <c r="T2" s="120"/>
-      <c r="U2" s="120"/>
-      <c r="V2" s="120"/>
-      <c r="W2" s="120"/>
-      <c r="X2" s="120"/>
-      <c r="Y2" s="120"/>
-      <c r="Z2" s="120"/>
-      <c r="AA2" s="120"/>
-      <c r="AB2" s="120"/>
-    </row>
-    <row r="3" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A3" s="121" t="s">
+      <c r="B2" s="125"/>
+      <c r="C2" s="125"/>
+      <c r="D2" s="125"/>
+      <c r="E2" s="125"/>
+      <c r="F2" s="125"/>
+      <c r="G2" s="125"/>
+      <c r="H2" s="125"/>
+      <c r="I2" s="125"/>
+      <c r="J2" s="125"/>
+      <c r="K2" s="125"/>
+      <c r="L2" s="125"/>
+      <c r="M2" s="125"/>
+      <c r="N2" s="125"/>
+      <c r="O2" s="125"/>
+      <c r="P2" s="125"/>
+      <c r="Q2" s="125"/>
+      <c r="R2" s="125"/>
+      <c r="S2" s="125"/>
+      <c r="T2" s="125"/>
+      <c r="U2" s="125"/>
+      <c r="V2" s="125"/>
+      <c r="W2" s="125"/>
+      <c r="X2" s="125"/>
+      <c r="Y2" s="125"/>
+      <c r="Z2" s="125"/>
+      <c r="AA2" s="125"/>
+      <c r="AB2" s="125"/>
+    </row>
+    <row r="3" spans="1:28" ht="14.25">
+      <c r="A3" s="126" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="121"/>
-      <c r="C3" s="121"/>
-      <c r="D3" s="121"/>
-      <c r="E3" s="121"/>
-      <c r="F3" s="121"/>
-      <c r="G3" s="121"/>
-      <c r="H3" s="121"/>
-      <c r="I3" s="121"/>
-      <c r="J3" s="121"/>
-      <c r="K3" s="121"/>
-      <c r="L3" s="121"/>
-      <c r="M3" s="121"/>
-      <c r="N3" s="121"/>
-      <c r="O3" s="121"/>
-      <c r="P3" s="121"/>
-      <c r="Q3" s="121"/>
-      <c r="R3" s="121"/>
-      <c r="S3" s="121"/>
-      <c r="T3" s="121"/>
-      <c r="U3" s="121"/>
-      <c r="V3" s="121"/>
-      <c r="W3" s="121"/>
-      <c r="X3" s="121"/>
-      <c r="Y3" s="121"/>
-      <c r="Z3" s="121"/>
-      <c r="AA3" s="121"/>
-      <c r="AB3" s="121"/>
-    </row>
-    <row r="4" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="120" t="s">
+      <c r="B3" s="126"/>
+      <c r="C3" s="126"/>
+      <c r="D3" s="126"/>
+      <c r="E3" s="126"/>
+      <c r="F3" s="126"/>
+      <c r="G3" s="126"/>
+      <c r="H3" s="126"/>
+      <c r="I3" s="126"/>
+      <c r="J3" s="126"/>
+      <c r="K3" s="126"/>
+      <c r="L3" s="126"/>
+      <c r="M3" s="126"/>
+      <c r="N3" s="126"/>
+      <c r="O3" s="126"/>
+      <c r="P3" s="126"/>
+      <c r="Q3" s="126"/>
+      <c r="R3" s="126"/>
+      <c r="S3" s="126"/>
+      <c r="T3" s="126"/>
+      <c r="U3" s="126"/>
+      <c r="V3" s="126"/>
+      <c r="W3" s="126"/>
+      <c r="X3" s="126"/>
+      <c r="Y3" s="126"/>
+      <c r="Z3" s="126"/>
+      <c r="AA3" s="126"/>
+      <c r="AB3" s="126"/>
+    </row>
+    <row r="4" spans="1:28" ht="12.75" customHeight="1">
+      <c r="A4" s="125" t="s">
         <v>159</v>
       </c>
-      <c r="B4" s="120"/>
-      <c r="C4" s="120"/>
-      <c r="D4" s="120"/>
-      <c r="E4" s="120"/>
-      <c r="F4" s="120"/>
-      <c r="G4" s="120"/>
-      <c r="H4" s="120"/>
-      <c r="I4" s="120"/>
-      <c r="J4" s="120"/>
-      <c r="K4" s="120"/>
-      <c r="L4" s="120"/>
-      <c r="M4" s="120"/>
-      <c r="N4" s="120"/>
-      <c r="O4" s="120"/>
-      <c r="P4" s="120"/>
-      <c r="Q4" s="120"/>
-      <c r="R4" s="120"/>
-      <c r="S4" s="120"/>
-      <c r="T4" s="120"/>
-      <c r="U4" s="120"/>
-      <c r="V4" s="120"/>
-      <c r="W4" s="120"/>
-      <c r="X4" s="120"/>
-      <c r="Y4" s="120"/>
-      <c r="Z4" s="120"/>
-      <c r="AA4" s="120"/>
-      <c r="AB4" s="120"/>
-    </row>
-    <row r="5" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="125"/>
+      <c r="C4" s="125"/>
+      <c r="D4" s="125"/>
+      <c r="E4" s="125"/>
+      <c r="F4" s="125"/>
+      <c r="G4" s="125"/>
+      <c r="H4" s="125"/>
+      <c r="I4" s="125"/>
+      <c r="J4" s="125"/>
+      <c r="K4" s="125"/>
+      <c r="L4" s="125"/>
+      <c r="M4" s="125"/>
+      <c r="N4" s="125"/>
+      <c r="O4" s="125"/>
+      <c r="P4" s="125"/>
+      <c r="Q4" s="125"/>
+      <c r="R4" s="125"/>
+      <c r="S4" s="125"/>
+      <c r="T4" s="125"/>
+      <c r="U4" s="125"/>
+      <c r="V4" s="125"/>
+      <c r="W4" s="125"/>
+      <c r="X4" s="125"/>
+      <c r="Y4" s="125"/>
+      <c r="Z4" s="125"/>
+      <c r="AA4" s="125"/>
+      <c r="AB4" s="125"/>
+    </row>
+    <row r="5" spans="1:28" ht="15" customHeight="1">
       <c r="B5" s="44"/>
       <c r="C5" s="44"/>
       <c r="D5" s="44"/>
@@ -3334,7 +3336,7 @@
       <c r="AA5" s="44"/>
       <c r="AB5" s="44"/>
     </row>
-    <row r="7" spans="1:28" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:28" ht="15">
       <c r="A7" s="3" t="s">
         <v>3</v>
       </c>
@@ -3368,7 +3370,7 @@
       <c r="AA7" s="6"/>
       <c r="AB7" s="9"/>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:28">
       <c r="A8" s="10"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
@@ -3398,7 +3400,7 @@
       <c r="AA8" s="12"/>
       <c r="AB8" s="13"/>
     </row>
-    <row r="9" spans="1:28" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:28" ht="15">
       <c r="A9" s="14"/>
       <c r="B9" s="14"/>
       <c r="C9" s="14"/>
@@ -3406,23 +3408,23 @@
       <c r="E9" s="14"/>
       <c r="F9" s="14"/>
       <c r="G9" s="15"/>
-      <c r="H9" s="122" t="s">
+      <c r="H9" s="127" t="s">
         <v>5</v>
       </c>
-      <c r="I9" s="123"/>
-      <c r="J9" s="123"/>
-      <c r="K9" s="124"/>
+      <c r="I9" s="128"/>
+      <c r="J9" s="128"/>
+      <c r="K9" s="129"/>
       <c r="L9" s="14"/>
-      <c r="M9" s="125" t="s">
+      <c r="M9" s="130" t="s">
         <v>6</v>
       </c>
-      <c r="N9" s="126"/>
+      <c r="N9" s="131"/>
       <c r="O9" s="14"/>
-      <c r="P9" s="127" t="s">
+      <c r="P9" s="132" t="s">
         <v>7</v>
       </c>
-      <c r="Q9" s="128"/>
-      <c r="R9" s="129"/>
+      <c r="Q9" s="133"/>
+      <c r="R9" s="134"/>
       <c r="S9" s="15"/>
       <c r="T9" s="107"/>
       <c r="U9" s="15"/>
@@ -3434,7 +3436,7 @@
       <c r="AA9" s="16"/>
       <c r="AB9" s="15"/>
     </row>
-    <row r="10" spans="1:28" ht="15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:28" ht="15">
       <c r="A10" s="17" t="s">
         <v>8</v>
       </c>
@@ -3478,7 +3480,7 @@
       </c>
       <c r="AB10" s="17"/>
     </row>
-    <row r="11" spans="1:28" ht="15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:28" ht="15">
       <c r="A11" s="17" t="s">
         <v>14</v>
       </c>
@@ -3536,7 +3538,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:28" ht="15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:28" ht="15">
       <c r="A12" s="18"/>
       <c r="B12" s="18"/>
       <c r="C12" s="18"/>
@@ -3586,7 +3588,7 @@
       </c>
       <c r="AB12" s="19"/>
     </row>
-    <row r="13" spans="1:28" ht="15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:28" ht="15">
       <c r="A13" s="18"/>
       <c r="B13" s="18"/>
       <c r="C13" s="18"/>
@@ -3628,7 +3630,7 @@
       <c r="AA13" s="19"/>
       <c r="AB13" s="19"/>
     </row>
-    <row r="14" spans="1:28" ht="15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:28" ht="15">
       <c r="A14" s="26" t="s">
         <v>42</v>
       </c>
@@ -3704,7 +3706,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:28" ht="15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:28" ht="15">
       <c r="A15" s="28"/>
       <c r="B15" s="55"/>
       <c r="C15" s="55"/>
@@ -3720,20 +3722,20 @@
       <c r="M15" s="66"/>
       <c r="N15" s="66"/>
       <c r="O15" s="66"/>
-      <c r="P15" s="64"/>
-      <c r="Q15" s="55"/>
-      <c r="R15" s="55"/>
-      <c r="S15" s="58"/>
-      <c r="U15" s="111"/>
-      <c r="V15" s="116"/>
-      <c r="W15" s="117"/>
-      <c r="X15" s="118"/>
-      <c r="Y15" s="119"/>
-      <c r="Z15" s="58"/>
+      <c r="P15" s="149"/>
+      <c r="Q15" s="66"/>
+      <c r="R15" s="66"/>
+      <c r="S15" s="60"/>
+      <c r="U15" s="150"/>
+      <c r="V15" s="151"/>
+      <c r="W15" s="114"/>
+      <c r="X15" s="152"/>
+      <c r="Y15" s="152"/>
+      <c r="Z15" s="60"/>
       <c r="AA15" s="60"/>
       <c r="AB15" s="66"/>
     </row>
-    <row r="16" spans="1:28" ht="15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:28" ht="15">
       <c r="A16" s="28"/>
       <c r="B16" s="55"/>
       <c r="C16" s="55"/>
@@ -3749,23 +3751,23 @@
       <c r="M16" s="66"/>
       <c r="N16" s="66"/>
       <c r="O16" s="66"/>
-      <c r="P16" s="55"/>
+      <c r="P16" s="66"/>
       <c r="Q16" s="66"/>
       <c r="R16" s="66"/>
       <c r="S16" s="60"/>
-      <c r="T16" s="114" t="s">
+      <c r="T16" s="153" t="s">
         <v>146</v>
       </c>
-      <c r="U16" s="114"/>
-      <c r="V16" s="111"/>
-      <c r="W16" s="111"/>
-      <c r="X16" s="111"/>
-      <c r="Y16" s="111"/>
+      <c r="U16" s="153"/>
+      <c r="V16" s="150"/>
+      <c r="W16" s="150"/>
+      <c r="X16" s="150"/>
+      <c r="Y16" s="150"/>
       <c r="Z16" s="60"/>
       <c r="AA16" s="68"/>
       <c r="AB16" s="66"/>
     </row>
-    <row r="17" spans="1:28" ht="15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:28" ht="15">
       <c r="A17" s="28"/>
       <c r="B17" s="29"/>
       <c r="C17" s="29"/>
@@ -3781,23 +3783,23 @@
       <c r="M17" s="30"/>
       <c r="N17" s="30"/>
       <c r="O17" s="30"/>
-      <c r="P17" s="29"/>
+      <c r="P17" s="30"/>
       <c r="Q17" s="30"/>
       <c r="R17" s="30"/>
       <c r="S17" s="30"/>
-      <c r="T17" s="115" t="s">
+      <c r="T17" s="153" t="s">
         <v>144</v>
       </c>
-      <c r="U17" s="114"/>
-      <c r="V17" s="111"/>
-      <c r="W17" s="111"/>
-      <c r="X17" s="111"/>
-      <c r="Y17" s="111"/>
+      <c r="U17" s="153"/>
+      <c r="V17" s="150"/>
+      <c r="W17" s="150"/>
+      <c r="X17" s="150"/>
+      <c r="Y17" s="150"/>
       <c r="Z17" s="30"/>
       <c r="AA17" s="35"/>
       <c r="AB17" s="30"/>
     </row>
-    <row r="18" spans="1:28" ht="15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:28" ht="15">
       <c r="A18" s="28"/>
       <c r="B18" s="29"/>
       <c r="C18" s="29"/>
@@ -3813,23 +3815,23 @@
       <c r="M18" s="30"/>
       <c r="N18" s="30"/>
       <c r="O18" s="30"/>
-      <c r="P18" s="29"/>
+      <c r="P18" s="30"/>
       <c r="Q18" s="30"/>
       <c r="R18" s="30"/>
       <c r="S18" s="30"/>
-      <c r="T18" s="115" t="s">
+      <c r="T18" s="153" t="s">
         <v>147</v>
       </c>
-      <c r="U18" s="114"/>
-      <c r="V18" s="111"/>
-      <c r="W18" s="111"/>
-      <c r="X18" s="111"/>
-      <c r="Y18" s="111"/>
+      <c r="U18" s="153"/>
+      <c r="V18" s="150"/>
+      <c r="W18" s="150"/>
+      <c r="X18" s="150"/>
+      <c r="Y18" s="150"/>
       <c r="Z18" s="30"/>
       <c r="AA18" s="35"/>
       <c r="AB18" s="30"/>
     </row>
-    <row r="19" spans="1:28" ht="15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:28" ht="15">
       <c r="A19" s="28"/>
       <c r="B19" s="29"/>
       <c r="C19" s="29"/>
@@ -3845,23 +3847,23 @@
       <c r="M19" s="30"/>
       <c r="N19" s="30"/>
       <c r="O19" s="30"/>
-      <c r="P19" s="29"/>
+      <c r="P19" s="30"/>
       <c r="Q19" s="30"/>
       <c r="R19" s="30"/>
       <c r="S19" s="30"/>
-      <c r="T19" s="115" t="s">
+      <c r="T19" s="153" t="s">
         <v>148</v>
       </c>
-      <c r="U19" s="114"/>
-      <c r="V19" s="111"/>
-      <c r="W19" s="111"/>
-      <c r="X19" s="111"/>
-      <c r="Y19" s="111"/>
+      <c r="U19" s="153"/>
+      <c r="V19" s="150"/>
+      <c r="W19" s="150"/>
+      <c r="X19" s="150"/>
+      <c r="Y19" s="150"/>
       <c r="Z19" s="30"/>
       <c r="AA19" s="35"/>
       <c r="AB19" s="30"/>
     </row>
-    <row r="20" spans="1:28" ht="15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:28" ht="15">
       <c r="A20" s="28"/>
       <c r="B20" s="29"/>
       <c r="C20" s="29"/>
@@ -3877,23 +3879,23 @@
       <c r="M20" s="30"/>
       <c r="N20" s="30"/>
       <c r="O20" s="30"/>
-      <c r="P20" s="29"/>
+      <c r="P20" s="30"/>
       <c r="Q20" s="36"/>
       <c r="R20" s="30"/>
       <c r="S20" s="31"/>
-      <c r="T20" s="114" t="s">
+      <c r="T20" s="153" t="s">
         <v>149</v>
       </c>
-      <c r="U20" s="114"/>
-      <c r="V20" s="111"/>
-      <c r="W20" s="111"/>
-      <c r="X20" s="111"/>
-      <c r="Y20" s="111"/>
+      <c r="U20" s="153"/>
+      <c r="V20" s="150"/>
+      <c r="W20" s="150"/>
+      <c r="X20" s="150"/>
+      <c r="Y20" s="150"/>
       <c r="Z20" s="31"/>
       <c r="AA20" s="30"/>
       <c r="AB20" s="30"/>
     </row>
-    <row r="21" spans="1:28" ht="15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:28" ht="15">
       <c r="A21" s="28"/>
       <c r="B21" s="29"/>
       <c r="C21" s="29"/>
@@ -3909,23 +3911,23 @@
       <c r="M21" s="30"/>
       <c r="N21" s="30"/>
       <c r="O21" s="30"/>
-      <c r="P21" s="29"/>
+      <c r="P21" s="30"/>
       <c r="Q21" s="30"/>
       <c r="R21" s="30"/>
       <c r="S21" s="30"/>
-      <c r="T21" s="115" t="s">
+      <c r="T21" s="153" t="s">
         <v>150</v>
       </c>
-      <c r="U21" s="114"/>
-      <c r="V21" s="111"/>
-      <c r="W21" s="111"/>
-      <c r="X21" s="111"/>
-      <c r="Y21" s="111"/>
+      <c r="U21" s="153"/>
+      <c r="V21" s="150"/>
+      <c r="W21" s="150"/>
+      <c r="X21" s="150"/>
+      <c r="Y21" s="150"/>
       <c r="Z21" s="30"/>
       <c r="AA21" s="30"/>
       <c r="AB21" s="30"/>
     </row>
-    <row r="22" spans="1:28" ht="15" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:28" ht="15">
       <c r="A22" s="28"/>
       <c r="B22" s="29"/>
       <c r="C22" s="29"/>
@@ -3941,23 +3943,23 @@
       <c r="M22" s="30"/>
       <c r="N22" s="30"/>
       <c r="O22" s="30"/>
-      <c r="P22" s="29"/>
+      <c r="P22" s="30"/>
       <c r="Q22" s="30"/>
       <c r="R22" s="30"/>
       <c r="S22" s="30"/>
-      <c r="T22" s="115" t="s">
+      <c r="T22" s="153" t="s">
         <v>151</v>
       </c>
-      <c r="U22" s="114"/>
-      <c r="V22" s="111"/>
-      <c r="W22" s="111"/>
-      <c r="X22" s="111"/>
-      <c r="Y22" s="111"/>
+      <c r="U22" s="153"/>
+      <c r="V22" s="150"/>
+      <c r="W22" s="150"/>
+      <c r="X22" s="150"/>
+      <c r="Y22" s="150"/>
       <c r="Z22" s="30"/>
       <c r="AA22" s="30"/>
       <c r="AB22" s="30"/>
     </row>
-    <row r="23" spans="1:28" ht="15" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:28" ht="15">
       <c r="A23" s="28"/>
       <c r="B23" s="29"/>
       <c r="C23" s="29"/>
@@ -3973,23 +3975,23 @@
       <c r="M23" s="30"/>
       <c r="N23" s="30"/>
       <c r="O23" s="30"/>
-      <c r="P23" s="29"/>
+      <c r="P23" s="30"/>
       <c r="Q23" s="30"/>
       <c r="R23" s="30"/>
       <c r="S23" s="30"/>
-      <c r="T23" s="114" t="s">
+      <c r="T23" s="153" t="s">
         <v>152</v>
       </c>
-      <c r="U23" s="114"/>
-      <c r="V23" s="111"/>
-      <c r="W23" s="111"/>
-      <c r="X23" s="111"/>
-      <c r="Y23" s="111"/>
+      <c r="U23" s="153"/>
+      <c r="V23" s="150"/>
+      <c r="W23" s="150"/>
+      <c r="X23" s="150"/>
+      <c r="Y23" s="150"/>
       <c r="Z23" s="30"/>
       <c r="AA23" s="30"/>
       <c r="AB23" s="30"/>
     </row>
-    <row r="24" spans="1:28" ht="17.25" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:28" ht="17.25">
       <c r="A24" s="28"/>
       <c r="B24" s="29"/>
       <c r="C24" s="29"/>
@@ -4005,23 +4007,23 @@
       <c r="M24" s="30"/>
       <c r="N24" s="30"/>
       <c r="O24" s="30"/>
-      <c r="P24" s="29"/>
+      <c r="P24" s="30"/>
       <c r="Q24" s="30"/>
       <c r="R24" s="30"/>
       <c r="S24" s="30"/>
-      <c r="T24" s="115" t="s">
+      <c r="T24" s="153" t="s">
         <v>153</v>
       </c>
-      <c r="U24" s="114"/>
-      <c r="V24" s="111"/>
-      <c r="W24" s="111"/>
-      <c r="X24" s="111"/>
-      <c r="Y24" s="111"/>
+      <c r="U24" s="153"/>
+      <c r="V24" s="150"/>
+      <c r="W24" s="150"/>
+      <c r="X24" s="150"/>
+      <c r="Y24" s="150"/>
       <c r="Z24" s="30"/>
       <c r="AA24" s="37"/>
       <c r="AB24" s="30"/>
     </row>
-    <row r="25" spans="1:28" ht="15" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:28" ht="15">
       <c r="A25" s="28"/>
       <c r="B25" s="29"/>
       <c r="C25" s="29"/>
@@ -4037,23 +4039,23 @@
       <c r="M25" s="30"/>
       <c r="N25" s="30"/>
       <c r="O25" s="30"/>
-      <c r="P25" s="29"/>
+      <c r="P25" s="30"/>
       <c r="Q25" s="30"/>
       <c r="R25" s="30"/>
       <c r="S25" s="30"/>
-      <c r="T25" s="115" t="s">
+      <c r="T25" s="153" t="s">
         <v>145</v>
       </c>
-      <c r="U25" s="114"/>
-      <c r="V25" s="111"/>
-      <c r="W25" s="111"/>
-      <c r="X25" s="111"/>
-      <c r="Y25" s="111"/>
+      <c r="U25" s="153"/>
+      <c r="V25" s="150"/>
+      <c r="W25" s="150"/>
+      <c r="X25" s="150"/>
+      <c r="Y25" s="150"/>
       <c r="Z25" s="30"/>
       <c r="AA25" s="31"/>
       <c r="AB25" s="30"/>
     </row>
-    <row r="26" spans="1:28" ht="15" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:28" ht="15">
       <c r="A26" s="38" t="s">
         <v>117</v>
       </c>
@@ -4062,7 +4064,7 @@
       <c r="X26" s="111"/>
       <c r="Y26" s="111"/>
     </row>
-    <row r="27" spans="1:28" ht="15" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:28" ht="15">
       <c r="V27" s="111"/>
       <c r="W27" s="111"/>
       <c r="X27" s="111"/>
@@ -4071,12 +4073,12 @@
         <v>64</v>
       </c>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:28">
       <c r="A28" s="38" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="29" spans="1:28" ht="15" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:28" ht="15">
       <c r="A29" s="38" t="s">
         <v>66</v>
       </c>
@@ -4084,7 +4086,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="30" spans="1:28" ht="15" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:28" ht="15">
       <c r="A30" s="38" t="s">
         <v>68</v>
       </c>
@@ -4092,21 +4094,21 @@
         <v>69</v>
       </c>
     </row>
-    <row r="31" spans="1:28" ht="15" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:28" ht="15">
       <c r="AB31" s="42" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="32" spans="1:28" ht="15" x14ac:dyDescent="0.2">
-      <c r="F32" s="136" t="s">
+    <row r="32" spans="1:28" ht="15">
+      <c r="F32" s="117" t="s">
         <v>70</v>
       </c>
-      <c r="G32" s="136"/>
-      <c r="H32" s="136"/>
-      <c r="I32" s="136"/>
-      <c r="J32" s="136"/>
-      <c r="K32" s="136"/>
-      <c r="L32" s="136"/>
+      <c r="G32" s="117"/>
+      <c r="H32" s="117"/>
+      <c r="I32" s="117"/>
+      <c r="J32" s="117"/>
+      <c r="K32" s="117"/>
+      <c r="L32" s="117"/>
       <c r="Q32" s="43" t="s">
         <v>71</v>
       </c>
@@ -4114,28 +4116,28 @@
         <v>73</v>
       </c>
     </row>
-    <row r="33" spans="1:28" ht="15" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:28" ht="15">
       <c r="AB33" s="42" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="34" spans="1:28" ht="15" x14ac:dyDescent="0.2">
-      <c r="A34" s="137" t="s">
+    <row r="34" spans="1:28" ht="15">
+      <c r="A34" s="118" t="s">
         <v>142</v>
       </c>
-      <c r="B34" s="137"/>
-      <c r="C34" s="137"/>
-      <c r="D34" s="137"/>
-      <c r="E34" s="137"/>
-      <c r="F34" s="137"/>
-      <c r="G34" s="137"/>
-      <c r="K34" s="138"/>
-      <c r="L34" s="139"/>
-      <c r="Q34" s="130" t="s">
+      <c r="B34" s="118"/>
+      <c r="C34" s="118"/>
+      <c r="D34" s="118"/>
+      <c r="E34" s="118"/>
+      <c r="F34" s="118"/>
+      <c r="G34" s="118"/>
+      <c r="K34" s="119"/>
+      <c r="L34" s="120"/>
+      <c r="Q34" s="121" t="s">
         <v>143</v>
       </c>
-      <c r="R34" s="130"/>
-      <c r="S34" s="130"/>
+      <c r="R34" s="121"/>
+      <c r="S34" s="121"/>
       <c r="T34" s="112"/>
       <c r="U34" s="39"/>
       <c r="V34" s="39"/>
@@ -4146,30 +4148,30 @@
         <v>76</v>
       </c>
     </row>
-    <row r="35" spans="1:28" ht="15" x14ac:dyDescent="0.2">
-      <c r="A35" s="131" t="s">
+    <row r="35" spans="1:28" ht="15">
+      <c r="A35" s="122" t="s">
         <v>141</v>
       </c>
-      <c r="B35" s="131"/>
-      <c r="C35" s="131"/>
-      <c r="D35" s="131"/>
-      <c r="E35" s="131"/>
-      <c r="F35" s="131"/>
-      <c r="G35" s="131"/>
+      <c r="B35" s="122"/>
+      <c r="C35" s="122"/>
+      <c r="D35" s="122"/>
+      <c r="E35" s="122"/>
+      <c r="F35" s="122"/>
+      <c r="G35" s="122"/>
       <c r="H35" s="43"/>
       <c r="I35" s="43"/>
       <c r="J35" s="43"/>
-      <c r="K35" s="132" t="s">
+      <c r="K35" s="123" t="s">
         <v>78</v>
       </c>
-      <c r="L35" s="132"/>
+      <c r="L35" s="123"/>
       <c r="M35" s="44"/>
       <c r="N35" s="44"/>
-      <c r="Q35" s="133" t="s">
+      <c r="Q35" s="124" t="s">
         <v>86</v>
       </c>
-      <c r="R35" s="133"/>
-      <c r="S35" s="133"/>
+      <c r="R35" s="124"/>
+      <c r="S35" s="124"/>
       <c r="T35" s="113"/>
       <c r="U35" s="42"/>
       <c r="V35" s="42"/>
@@ -4180,15 +4182,15 @@
         <v>79</v>
       </c>
     </row>
-    <row r="36" spans="1:28" ht="15" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:28" ht="15">
       <c r="H36" s="44"/>
       <c r="I36" s="44"/>
       <c r="J36" s="44"/>
     </row>
-    <row r="37" spans="1:28" ht="15" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:28" ht="15">
       <c r="O37" s="44"/>
     </row>
-    <row r="38" spans="1:28" ht="15" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:28" ht="15">
       <c r="B38" s="44"/>
       <c r="C38" s="44"/>
       <c r="D38" s="46"/>
@@ -4197,17 +4199,17 @@
       <c r="O38" s="44"/>
       <c r="AA38" s="45"/>
     </row>
-    <row r="40" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:28" ht="14.25">
       <c r="D40" s="46"/>
       <c r="E40" s="46"/>
       <c r="F40" s="46"/>
     </row>
-    <row r="41" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:28" ht="14.25">
       <c r="D41" s="46"/>
       <c r="E41" s="46"/>
       <c r="F41" s="46"/>
     </row>
-    <row r="42" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:28" ht="14.25">
       <c r="B42" s="46"/>
       <c r="C42" s="46"/>
       <c r="D42" s="46"/>
@@ -4226,7 +4228,7 @@
       <c r="Q42" s="49"/>
       <c r="R42" s="50"/>
     </row>
-    <row r="43" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:28" ht="14.25">
       <c r="B43" s="46"/>
       <c r="C43" s="46"/>
       <c r="D43" s="46"/>
@@ -4245,7 +4247,7 @@
       <c r="Q43" s="49"/>
       <c r="R43" s="50"/>
     </row>
-    <row r="44" spans="1:28" ht="15" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:28" ht="15">
       <c r="B44" s="42"/>
       <c r="C44" s="42"/>
       <c r="D44" s="46"/>
@@ -4264,7 +4266,7 @@
       <c r="Q44" s="45"/>
       <c r="R44" s="50"/>
     </row>
-    <row r="45" spans="1:28" ht="15" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:28" ht="15">
       <c r="B45" s="42"/>
       <c r="C45" s="42"/>
       <c r="D45" s="42"/>
@@ -4283,7 +4285,7 @@
       <c r="Q45" s="45"/>
       <c r="R45" s="50"/>
     </row>
-    <row r="46" spans="1:28" ht="15" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:28" ht="15">
       <c r="B46" s="42"/>
       <c r="C46" s="42"/>
       <c r="D46" s="46"/>
@@ -4302,7 +4304,7 @@
       <c r="Q46" s="45"/>
       <c r="R46" s="50"/>
     </row>
-    <row r="47" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:28" ht="14.25">
       <c r="B47" s="46"/>
       <c r="C47" s="46"/>
       <c r="D47" s="46"/>
@@ -4321,7 +4323,7 @@
       <c r="Q47" s="49"/>
       <c r="R47" s="50"/>
     </row>
-    <row r="48" spans="1:28" ht="15" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:28" ht="15">
       <c r="B48" s="42"/>
       <c r="C48" s="42"/>
       <c r="D48" s="46"/>
@@ -4340,7 +4342,7 @@
       <c r="Q48" s="45"/>
       <c r="R48" s="50"/>
     </row>
-    <row r="49" spans="2:28" ht="15" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:28" ht="15">
       <c r="B49" s="42"/>
       <c r="C49" s="42"/>
       <c r="D49" s="46"/>
@@ -4359,13 +4361,13 @@
       <c r="Q49" s="49"/>
       <c r="R49" s="50"/>
     </row>
-    <row r="50" spans="2:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="B50" s="134"/>
-      <c r="C50" s="134"/>
-      <c r="D50" s="134"/>
-      <c r="E50" s="134"/>
-      <c r="F50" s="134"/>
-      <c r="G50" s="135"/>
+    <row r="50" spans="2:28" ht="14.25">
+      <c r="B50" s="115"/>
+      <c r="C50" s="115"/>
+      <c r="D50" s="115"/>
+      <c r="E50" s="115"/>
+      <c r="F50" s="115"/>
+      <c r="G50" s="116"/>
       <c r="H50" s="47"/>
       <c r="I50" s="47"/>
       <c r="J50" s="47"/>
@@ -4378,7 +4380,7 @@
       <c r="Q50" s="49"/>
       <c r="R50" s="50"/>
     </row>
-    <row r="51" spans="2:28" ht="15" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:28" ht="15">
       <c r="B51" s="51"/>
       <c r="C51" s="51"/>
       <c r="D51" s="46"/>
@@ -4397,7 +4399,7 @@
       <c r="Q51" s="49"/>
       <c r="R51" s="50"/>
     </row>
-    <row r="52" spans="2:28" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:28" ht="14.25">
       <c r="B52" s="46"/>
       <c r="C52" s="46"/>
       <c r="D52" s="46"/>
@@ -4416,7 +4418,7 @@
       <c r="Q52" s="49"/>
       <c r="R52" s="50"/>
     </row>
-    <row r="53" spans="2:28" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:28" ht="14.25">
       <c r="B53" s="46"/>
       <c r="C53" s="46"/>
       <c r="D53" s="46"/>
@@ -4435,7 +4437,7 @@
       <c r="Q53" s="49"/>
       <c r="R53" s="50"/>
     </row>
-    <row r="54" spans="2:28" ht="15" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:28" ht="15">
       <c r="B54" s="42"/>
       <c r="C54" s="42"/>
       <c r="D54" s="46"/>
@@ -4454,7 +4456,7 @@
       <c r="Q54" s="45"/>
       <c r="R54" s="50"/>
     </row>
-    <row r="55" spans="2:28" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:28" ht="14.25">
       <c r="B55" s="46"/>
       <c r="C55" s="46"/>
       <c r="D55" s="46"/>
@@ -4473,7 +4475,7 @@
       <c r="Q55" s="49"/>
       <c r="R55" s="50"/>
     </row>
-    <row r="56" spans="2:28" ht="15" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:28" ht="15">
       <c r="B56" s="42"/>
       <c r="C56" s="42"/>
       <c r="D56" s="46"/>
@@ -4492,7 +4494,7 @@
       <c r="Q56" s="45"/>
       <c r="R56" s="50"/>
     </row>
-    <row r="57" spans="2:28" ht="15" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:28" ht="15">
       <c r="B57" s="42"/>
       <c r="C57" s="42"/>
       <c r="D57" s="46"/>
@@ -4511,7 +4513,7 @@
       <c r="Q57" s="45"/>
       <c r="R57" s="50"/>
     </row>
-    <row r="58" spans="2:28" ht="15" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:28" ht="15">
       <c r="B58" s="42"/>
       <c r="C58" s="42"/>
       <c r="D58" s="42"/>
@@ -4530,13 +4532,13 @@
       <c r="Q58" s="45"/>
       <c r="R58" s="50"/>
     </row>
-    <row r="59" spans="2:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="B59" s="134"/>
-      <c r="C59" s="134"/>
-      <c r="D59" s="134"/>
-      <c r="E59" s="134"/>
-      <c r="F59" s="134"/>
-      <c r="G59" s="135"/>
+    <row r="59" spans="2:28" ht="14.25">
+      <c r="B59" s="115"/>
+      <c r="C59" s="115"/>
+      <c r="D59" s="115"/>
+      <c r="E59" s="115"/>
+      <c r="F59" s="115"/>
+      <c r="G59" s="116"/>
       <c r="H59" s="47"/>
       <c r="I59" s="47"/>
       <c r="J59" s="47"/>
@@ -4549,7 +4551,7 @@
       <c r="Q59" s="49"/>
       <c r="R59" s="50"/>
     </row>
-    <row r="60" spans="2:28" ht="15" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:28" ht="15">
       <c r="B60" s="42"/>
       <c r="C60" s="42"/>
       <c r="D60" s="46"/>
@@ -4568,7 +4570,7 @@
       <c r="Q60" s="45"/>
       <c r="R60" s="50"/>
     </row>
-    <row r="61" spans="2:28" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:28">
       <c r="G61" s="1"/>
       <c r="H61" s="1"/>
       <c r="I61" s="1"/>
@@ -4587,7 +4589,7 @@
       <c r="AA61" s="1"/>
       <c r="AB61" s="1"/>
     </row>
-    <row r="62" spans="2:28" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:28">
       <c r="G62" s="1"/>
       <c r="H62" s="1"/>
       <c r="I62" s="1"/>
@@ -4606,7 +4608,7 @@
       <c r="AA62" s="1"/>
       <c r="AB62" s="1"/>
     </row>
-    <row r="63" spans="2:28" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:28">
       <c r="G63" s="1"/>
       <c r="H63" s="1"/>
       <c r="I63" s="1"/>
@@ -4625,7 +4627,7 @@
       <c r="AA63" s="1"/>
       <c r="AB63" s="1"/>
     </row>
-    <row r="64" spans="2:28" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:28">
       <c r="G64" s="1"/>
       <c r="H64" s="1"/>
       <c r="I64" s="1"/>
@@ -4644,7 +4646,7 @@
       <c r="AA64" s="1"/>
       <c r="AB64" s="1"/>
     </row>
-    <row r="65" spans="2:28" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:28">
       <c r="G65" s="1"/>
       <c r="H65" s="1"/>
       <c r="I65" s="1"/>
@@ -4663,7 +4665,7 @@
       <c r="AA65" s="1"/>
       <c r="AB65" s="1"/>
     </row>
-    <row r="66" spans="2:28" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:28">
       <c r="G66" s="1"/>
       <c r="H66" s="1"/>
       <c r="I66" s="1"/>
@@ -4682,7 +4684,7 @@
       <c r="AA66" s="1"/>
       <c r="AB66" s="1"/>
     </row>
-    <row r="67" spans="2:28" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:28">
       <c r="G67" s="1"/>
       <c r="H67" s="1"/>
       <c r="I67" s="1"/>
@@ -4701,7 +4703,7 @@
       <c r="AA67" s="1"/>
       <c r="AB67" s="1"/>
     </row>
-    <row r="68" spans="2:28" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:28">
       <c r="G68" s="1"/>
       <c r="H68" s="1"/>
       <c r="I68" s="1"/>
@@ -4720,7 +4722,7 @@
       <c r="AA68" s="1"/>
       <c r="AB68" s="1"/>
     </row>
-    <row r="69" spans="2:28" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:28" ht="14.25">
       <c r="B69" s="46"/>
       <c r="C69" s="46"/>
       <c r="D69" s="46"/>
@@ -4739,7 +4741,7 @@
       <c r="Q69" s="49"/>
       <c r="R69" s="50"/>
     </row>
-    <row r="70" spans="2:28" ht="15" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:28" ht="15">
       <c r="B70" s="53"/>
       <c r="C70" s="53"/>
       <c r="D70" s="53"/>
@@ -4760,22 +4762,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="B50:G50"/>
-    <mergeCell ref="B59:G59"/>
-    <mergeCell ref="F32:L32"/>
-    <mergeCell ref="A34:G34"/>
-    <mergeCell ref="K34:L34"/>
-    <mergeCell ref="Q34:S34"/>
-    <mergeCell ref="A35:G35"/>
-    <mergeCell ref="K35:L35"/>
-    <mergeCell ref="Q35:S35"/>
-    <mergeCell ref="A4:AB4"/>
     <mergeCell ref="A1:AB1"/>
     <mergeCell ref="A2:AB2"/>
     <mergeCell ref="A3:AB3"/>
     <mergeCell ref="H9:K9"/>
     <mergeCell ref="M9:N9"/>
     <mergeCell ref="P9:R9"/>
+    <mergeCell ref="Q34:S34"/>
+    <mergeCell ref="A35:G35"/>
+    <mergeCell ref="K35:L35"/>
+    <mergeCell ref="Q35:S35"/>
+    <mergeCell ref="A4:AB4"/>
+    <mergeCell ref="B50:G50"/>
+    <mergeCell ref="B59:G59"/>
+    <mergeCell ref="F32:L32"/>
+    <mergeCell ref="A34:G34"/>
+    <mergeCell ref="K34:L34"/>
   </mergeCells>
   <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="V15">
@@ -4796,7 +4798,7 @@
       <selection activeCell="B23" sqref="B23:AN23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="4.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="19.5703125" style="1" customWidth="1"/>
@@ -4838,73 +4840,73 @@
     <col min="43" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="120" t="s">
+    <row r="1" spans="1:40" ht="15">
+      <c r="A1" s="125" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="120"/>
-      <c r="C1" s="120"/>
-      <c r="D1" s="120"/>
-      <c r="E1" s="120"/>
-      <c r="F1" s="120"/>
-      <c r="G1" s="120"/>
-      <c r="H1" s="120"/>
-      <c r="I1" s="120"/>
-      <c r="J1" s="120"/>
-      <c r="K1" s="120"/>
-      <c r="L1" s="120"/>
-      <c r="M1" s="120"/>
-      <c r="N1" s="120"/>
-      <c r="O1" s="120"/>
-      <c r="P1" s="120"/>
-      <c r="Q1" s="120"/>
-      <c r="R1" s="120"/>
-    </row>
-    <row r="2" spans="1:40" ht="15" x14ac:dyDescent="0.2">
-      <c r="A2" s="120" t="s">
+      <c r="B1" s="125"/>
+      <c r="C1" s="125"/>
+      <c r="D1" s="125"/>
+      <c r="E1" s="125"/>
+      <c r="F1" s="125"/>
+      <c r="G1" s="125"/>
+      <c r="H1" s="125"/>
+      <c r="I1" s="125"/>
+      <c r="J1" s="125"/>
+      <c r="K1" s="125"/>
+      <c r="L1" s="125"/>
+      <c r="M1" s="125"/>
+      <c r="N1" s="125"/>
+      <c r="O1" s="125"/>
+      <c r="P1" s="125"/>
+      <c r="Q1" s="125"/>
+      <c r="R1" s="125"/>
+    </row>
+    <row r="2" spans="1:40" ht="15">
+      <c r="A2" s="125" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="120"/>
-      <c r="C2" s="120"/>
-      <c r="D2" s="120"/>
-      <c r="E2" s="120"/>
-      <c r="F2" s="120"/>
-      <c r="G2" s="120"/>
-      <c r="H2" s="120"/>
-      <c r="I2" s="120"/>
-      <c r="J2" s="120"/>
-      <c r="K2" s="120"/>
-      <c r="L2" s="120"/>
-      <c r="M2" s="120"/>
-      <c r="N2" s="120"/>
-      <c r="O2" s="120"/>
-      <c r="P2" s="120"/>
-      <c r="Q2" s="120"/>
-      <c r="R2" s="120"/>
-    </row>
-    <row r="3" spans="1:40" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A3" s="121" t="s">
+      <c r="B2" s="125"/>
+      <c r="C2" s="125"/>
+      <c r="D2" s="125"/>
+      <c r="E2" s="125"/>
+      <c r="F2" s="125"/>
+      <c r="G2" s="125"/>
+      <c r="H2" s="125"/>
+      <c r="I2" s="125"/>
+      <c r="J2" s="125"/>
+      <c r="K2" s="125"/>
+      <c r="L2" s="125"/>
+      <c r="M2" s="125"/>
+      <c r="N2" s="125"/>
+      <c r="O2" s="125"/>
+      <c r="P2" s="125"/>
+      <c r="Q2" s="125"/>
+      <c r="R2" s="125"/>
+    </row>
+    <row r="3" spans="1:40" ht="14.25">
+      <c r="A3" s="126" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="121"/>
-      <c r="C3" s="121"/>
-      <c r="D3" s="121"/>
-      <c r="E3" s="121"/>
-      <c r="F3" s="121"/>
-      <c r="G3" s="121"/>
-      <c r="H3" s="121"/>
-      <c r="I3" s="121"/>
-      <c r="J3" s="121"/>
-      <c r="K3" s="121"/>
-      <c r="L3" s="121"/>
-      <c r="M3" s="121"/>
-      <c r="N3" s="121"/>
-      <c r="O3" s="121"/>
-      <c r="P3" s="121"/>
-      <c r="Q3" s="121"/>
-      <c r="R3" s="121"/>
-    </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="B3" s="126"/>
+      <c r="C3" s="126"/>
+      <c r="D3" s="126"/>
+      <c r="E3" s="126"/>
+      <c r="F3" s="126"/>
+      <c r="G3" s="126"/>
+      <c r="H3" s="126"/>
+      <c r="I3" s="126"/>
+      <c r="J3" s="126"/>
+      <c r="K3" s="126"/>
+      <c r="L3" s="126"/>
+      <c r="M3" s="126"/>
+      <c r="N3" s="126"/>
+      <c r="O3" s="126"/>
+      <c r="P3" s="126"/>
+      <c r="Q3" s="126"/>
+      <c r="R3" s="126"/>
+    </row>
+    <row r="4" spans="1:40">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -4914,38 +4916,38 @@
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
     </row>
-    <row r="5" spans="1:40" ht="15" x14ac:dyDescent="0.2">
-      <c r="A5" s="120" t="s">
+    <row r="5" spans="1:40" ht="15">
+      <c r="A5" s="125" t="s">
         <v>129</v>
       </c>
-      <c r="B5" s="120"/>
-      <c r="C5" s="120"/>
-      <c r="D5" s="120"/>
-      <c r="E5" s="120"/>
-      <c r="F5" s="120"/>
-      <c r="G5" s="120"/>
-      <c r="H5" s="120"/>
-      <c r="I5" s="120"/>
-      <c r="J5" s="120"/>
-      <c r="K5" s="120"/>
-      <c r="L5" s="120"/>
-      <c r="M5" s="120"/>
-      <c r="N5" s="120"/>
-      <c r="O5" s="120"/>
-      <c r="P5" s="120"/>
-      <c r="Q5" s="120"/>
-      <c r="R5" s="120"/>
-    </row>
-    <row r="7" spans="1:40" ht="15" x14ac:dyDescent="0.2">
-      <c r="A7" s="152" t="s">
+      <c r="B5" s="125"/>
+      <c r="C5" s="125"/>
+      <c r="D5" s="125"/>
+      <c r="E5" s="125"/>
+      <c r="F5" s="125"/>
+      <c r="G5" s="125"/>
+      <c r="H5" s="125"/>
+      <c r="I5" s="125"/>
+      <c r="J5" s="125"/>
+      <c r="K5" s="125"/>
+      <c r="L5" s="125"/>
+      <c r="M5" s="125"/>
+      <c r="N5" s="125"/>
+      <c r="O5" s="125"/>
+      <c r="P5" s="125"/>
+      <c r="Q5" s="125"/>
+      <c r="R5" s="125"/>
+    </row>
+    <row r="7" spans="1:40" ht="15">
+      <c r="A7" s="135" t="s">
         <v>89</v>
       </c>
-      <c r="B7" s="153"/>
-      <c r="C7" s="153"/>
-      <c r="D7" s="153"/>
-      <c r="E7" s="153"/>
-      <c r="F7" s="153"/>
-      <c r="G7" s="153"/>
+      <c r="B7" s="136"/>
+      <c r="C7" s="136"/>
+      <c r="D7" s="136"/>
+      <c r="E7" s="136"/>
+      <c r="F7" s="136"/>
+      <c r="G7" s="136"/>
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
       <c r="J7" s="7"/>
@@ -4960,7 +4962,7 @@
       <c r="Q7" s="6"/>
       <c r="R7" s="9"/>
     </row>
-    <row r="8" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:40">
       <c r="A8" s="10"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
@@ -4980,33 +4982,33 @@
       <c r="Q8" s="12"/>
       <c r="R8" s="13"/>
     </row>
-    <row r="9" spans="1:40" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:40" ht="15">
       <c r="A9" s="14"/>
       <c r="B9" s="14"/>
       <c r="C9" s="14"/>
       <c r="D9" s="15"/>
-      <c r="E9" s="122" t="s">
+      <c r="E9" s="127" t="s">
         <v>5</v>
       </c>
-      <c r="F9" s="123"/>
-      <c r="G9" s="124"/>
+      <c r="F9" s="128"/>
+      <c r="G9" s="129"/>
       <c r="H9" s="14"/>
-      <c r="I9" s="125" t="s">
+      <c r="I9" s="130" t="s">
         <v>6</v>
       </c>
-      <c r="J9" s="126"/>
+      <c r="J9" s="131"/>
       <c r="K9" s="14"/>
-      <c r="L9" s="127" t="s">
+      <c r="L9" s="132" t="s">
         <v>7</v>
       </c>
-      <c r="M9" s="128"/>
-      <c r="N9" s="129"/>
+      <c r="M9" s="133"/>
+      <c r="N9" s="134"/>
       <c r="O9" s="15"/>
       <c r="P9" s="15"/>
       <c r="Q9" s="16"/>
       <c r="R9" s="15"/>
     </row>
-    <row r="10" spans="1:40" ht="15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:40" ht="15">
       <c r="A10" s="17" t="s">
         <v>8</v>
       </c>
@@ -5040,7 +5042,7 @@
       </c>
       <c r="R10" s="17"/>
     </row>
-    <row r="11" spans="1:40" ht="15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:40" ht="15">
       <c r="A11" s="17" t="s">
         <v>14</v>
       </c>
@@ -5086,7 +5088,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:40" ht="15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:40" ht="15">
       <c r="A12" s="18"/>
       <c r="B12" s="18"/>
       <c r="C12" s="18"/>
@@ -5125,36 +5127,36 @@
         <v>34</v>
       </c>
       <c r="R12" s="19"/>
-      <c r="S12" s="150" t="s">
+      <c r="S12" s="148" t="s">
         <v>35</v>
       </c>
-      <c r="T12" s="150"/>
-      <c r="U12" s="150"/>
-      <c r="V12" s="150"/>
-      <c r="W12" s="150"/>
-      <c r="X12" s="150"/>
-      <c r="Y12" s="150"/>
-      <c r="Z12" s="150"/>
-      <c r="AA12" s="150"/>
-      <c r="AB12" s="150"/>
-      <c r="AC12" s="149" t="s">
+      <c r="T12" s="148"/>
+      <c r="U12" s="148"/>
+      <c r="V12" s="148"/>
+      <c r="W12" s="148"/>
+      <c r="X12" s="148"/>
+      <c r="Y12" s="148"/>
+      <c r="Z12" s="148"/>
+      <c r="AA12" s="148"/>
+      <c r="AB12" s="148"/>
+      <c r="AC12" s="147" t="s">
         <v>36</v>
       </c>
-      <c r="AD12" s="149"/>
-      <c r="AE12" s="149"/>
-      <c r="AF12" s="149"/>
-      <c r="AG12" s="149"/>
-      <c r="AH12" s="149"/>
-      <c r="AI12" s="149"/>
-      <c r="AJ12" s="149"/>
-      <c r="AK12" s="149"/>
-      <c r="AL12" s="149"/>
-      <c r="AM12" s="140" t="s">
+      <c r="AD12" s="147"/>
+      <c r="AE12" s="147"/>
+      <c r="AF12" s="147"/>
+      <c r="AG12" s="147"/>
+      <c r="AH12" s="147"/>
+      <c r="AI12" s="147"/>
+      <c r="AJ12" s="147"/>
+      <c r="AK12" s="147"/>
+      <c r="AL12" s="147"/>
+      <c r="AM12" s="138" t="s">
         <v>130</v>
       </c>
-      <c r="AN12" s="140"/>
-    </row>
-    <row r="13" spans="1:40" ht="15" x14ac:dyDescent="0.2">
+      <c r="AN12" s="138"/>
+    </row>
+    <row r="13" spans="1:40" ht="15">
       <c r="A13" s="18"/>
       <c r="B13" s="18"/>
       <c r="C13" s="18"/>
@@ -5183,46 +5185,46 @@
       </c>
       <c r="Q13" s="19"/>
       <c r="R13" s="19"/>
-      <c r="S13" s="143" t="s">
+      <c r="S13" s="141" t="s">
         <v>38</v>
       </c>
-      <c r="T13" s="143"/>
-      <c r="U13" s="143"/>
-      <c r="V13" s="147" t="s">
+      <c r="T13" s="141"/>
+      <c r="U13" s="141"/>
+      <c r="V13" s="145" t="s">
         <v>39</v>
       </c>
-      <c r="W13" s="147"/>
-      <c r="X13" s="147"/>
-      <c r="Y13" s="148" t="s">
+      <c r="W13" s="145"/>
+      <c r="X13" s="145"/>
+      <c r="Y13" s="146" t="s">
         <v>40</v>
       </c>
-      <c r="Z13" s="148"/>
-      <c r="AA13" s="148"/>
-      <c r="AB13" s="141" t="s">
+      <c r="Z13" s="146"/>
+      <c r="AA13" s="146"/>
+      <c r="AB13" s="139" t="s">
         <v>41</v>
       </c>
-      <c r="AC13" s="144" t="s">
+      <c r="AC13" s="142" t="s">
         <v>38</v>
       </c>
-      <c r="AD13" s="144"/>
-      <c r="AE13" s="144"/>
-      <c r="AF13" s="145" t="s">
+      <c r="AD13" s="142"/>
+      <c r="AE13" s="142"/>
+      <c r="AF13" s="143" t="s">
         <v>39</v>
       </c>
-      <c r="AG13" s="145"/>
-      <c r="AH13" s="145"/>
-      <c r="AI13" s="146" t="s">
+      <c r="AG13" s="143"/>
+      <c r="AH13" s="143"/>
+      <c r="AI13" s="144" t="s">
         <v>40</v>
       </c>
-      <c r="AJ13" s="146"/>
-      <c r="AK13" s="146"/>
-      <c r="AL13" s="142" t="s">
+      <c r="AJ13" s="144"/>
+      <c r="AK13" s="144"/>
+      <c r="AL13" s="140" t="s">
         <v>41</v>
       </c>
-      <c r="AM13" s="140"/>
-      <c r="AN13" s="140"/>
-    </row>
-    <row r="14" spans="1:40" ht="15" x14ac:dyDescent="0.2">
+      <c r="AM13" s="138"/>
+      <c r="AN13" s="138"/>
+    </row>
+    <row r="14" spans="1:40" ht="15">
       <c r="A14" s="26" t="s">
         <v>42</v>
       </c>
@@ -5300,7 +5302,7 @@
       <c r="AA14" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="AB14" s="141"/>
+      <c r="AB14" s="139"/>
       <c r="AC14" s="27" t="s">
         <v>58</v>
       </c>
@@ -5328,7 +5330,7 @@
       <c r="AK14" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="AL14" s="142"/>
+      <c r="AL14" s="140"/>
       <c r="AM14" s="83" t="s">
         <v>131</v>
       </c>
@@ -5336,7 +5338,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="15" spans="1:40" ht="15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:40" ht="15">
       <c r="A15" s="59">
         <v>12</v>
       </c>
@@ -5415,7 +5417,7 @@
       <c r="AM15" s="84"/>
       <c r="AN15" s="86"/>
     </row>
-    <row r="16" spans="1:40" ht="15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:40" ht="15">
       <c r="A16" s="59">
         <f>A15+1</f>
         <v>13</v>
@@ -5483,7 +5485,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:40" ht="15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:40" ht="15">
       <c r="A17" s="59">
         <f t="shared" ref="A17:A26" si="1">A16+1</f>
         <v>14</v>
@@ -5549,7 +5551,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:40" ht="15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:40" ht="15">
       <c r="A18" s="59">
         <f t="shared" si="1"/>
         <v>15</v>
@@ -5631,7 +5633,7 @@
       <c r="AM18" s="84"/>
       <c r="AN18" s="86"/>
     </row>
-    <row r="19" spans="1:40" ht="15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:40" ht="15">
       <c r="A19" s="59">
         <f t="shared" si="1"/>
         <v>16</v>
@@ -5713,7 +5715,7 @@
       <c r="AM19" s="84"/>
       <c r="AN19" s="86"/>
     </row>
-    <row r="20" spans="1:40" ht="15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:40" ht="15">
       <c r="A20" s="59">
         <f t="shared" si="1"/>
         <v>17</v>
@@ -5793,7 +5795,7 @@
       <c r="AM20" s="84"/>
       <c r="AN20" s="86"/>
     </row>
-    <row r="21" spans="1:40" ht="15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:40" ht="15">
       <c r="A21" s="59">
         <f t="shared" si="1"/>
         <v>18</v>
@@ -5863,7 +5865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:40" ht="15" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:40" ht="15">
       <c r="A22" s="59">
         <f>A21+1</f>
         <v>19</v>
@@ -5943,7 +5945,7 @@
       <c r="AM22" s="84"/>
       <c r="AN22" s="86"/>
     </row>
-    <row r="23" spans="1:40" s="100" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:40" s="100" customFormat="1" ht="15">
       <c r="A23" s="90">
         <f>A22+1</f>
         <v>20</v>
@@ -6023,7 +6025,7 @@
       <c r="AM23" s="99"/>
       <c r="AN23" s="99"/>
     </row>
-    <row r="24" spans="1:40" ht="15" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:40" ht="15">
       <c r="A24" s="59">
         <f t="shared" si="1"/>
         <v>21</v>
@@ -6103,7 +6105,7 @@
       <c r="AM24" s="84"/>
       <c r="AN24" s="86"/>
     </row>
-    <row r="25" spans="1:40" ht="15" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:40" ht="15">
       <c r="A25" s="59">
         <f t="shared" si="1"/>
         <v>22</v>
@@ -6183,7 +6185,7 @@
       <c r="AM25" s="84"/>
       <c r="AN25" s="86"/>
     </row>
-    <row r="26" spans="1:40" ht="15" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:40" ht="15">
       <c r="A26" s="59">
         <f t="shared" si="1"/>
         <v>23</v>
@@ -6263,7 +6265,7 @@
       <c r="AM26" s="84"/>
       <c r="AN26" s="86"/>
     </row>
-    <row r="27" spans="1:40" ht="15" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:40" ht="15">
       <c r="A27" s="38" t="s">
         <v>118</v>
       </c>
@@ -6351,7 +6353,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:40" ht="15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:40" ht="15">
       <c r="Q28" s="39" t="s">
         <v>64</v>
       </c>
@@ -6369,12 +6371,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:40">
       <c r="A29" s="38" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="30" spans="1:40" ht="15" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:40" ht="15">
       <c r="A30" s="38" t="s">
         <v>66</v>
       </c>
@@ -6382,7 +6384,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="31" spans="1:40" ht="15" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:40" ht="15">
       <c r="A31" s="38" t="s">
         <v>68</v>
       </c>
@@ -6390,13 +6392,13 @@
         <v>69</v>
       </c>
     </row>
-    <row r="32" spans="1:40" ht="15" x14ac:dyDescent="0.2">
-      <c r="A32" s="136" t="s">
+    <row r="32" spans="1:40" ht="15">
+      <c r="A32" s="117" t="s">
         <v>70</v>
       </c>
-      <c r="B32" s="136"/>
-      <c r="C32" s="136"/>
-      <c r="D32" s="136"/>
+      <c r="B32" s="117"/>
+      <c r="C32" s="117"/>
+      <c r="D32" s="117"/>
       <c r="M32" s="43" t="s">
         <v>71</v>
       </c>
@@ -6404,74 +6406,74 @@
         <v>72</v>
       </c>
     </row>
-    <row r="33" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:17" ht="15">
       <c r="Q33" s="42" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="34" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:17" ht="15">
       <c r="Q34" s="42" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="35" spans="1:17" ht="15" x14ac:dyDescent="0.2">
-      <c r="A35" s="137" t="s">
+    <row r="35" spans="1:17" ht="15">
+      <c r="A35" s="118" t="s">
         <v>75</v>
       </c>
-      <c r="B35" s="137"/>
-      <c r="C35" s="137"/>
-      <c r="D35" s="137"/>
-      <c r="G35" s="138">
+      <c r="B35" s="118"/>
+      <c r="C35" s="118"/>
+      <c r="D35" s="118"/>
+      <c r="G35" s="119">
         <v>43465</v>
       </c>
-      <c r="H35" s="139"/>
-      <c r="M35" s="130" t="s">
+      <c r="H35" s="120"/>
+      <c r="M35" s="121" t="s">
         <v>133</v>
       </c>
-      <c r="N35" s="130"/>
-      <c r="O35" s="130"/>
+      <c r="N35" s="121"/>
+      <c r="O35" s="121"/>
       <c r="Q35" s="42" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="36" spans="1:17" ht="15" x14ac:dyDescent="0.2">
-      <c r="A36" s="120" t="s">
+    <row r="36" spans="1:17" ht="15">
+      <c r="A36" s="125" t="s">
         <v>77</v>
       </c>
-      <c r="B36" s="120"/>
-      <c r="C36" s="120"/>
-      <c r="D36" s="120"/>
+      <c r="B36" s="125"/>
+      <c r="C36" s="125"/>
+      <c r="D36" s="125"/>
       <c r="E36" s="43"/>
       <c r="F36" s="43"/>
-      <c r="G36" s="132" t="s">
+      <c r="G36" s="123" t="s">
         <v>78</v>
       </c>
-      <c r="H36" s="132"/>
+      <c r="H36" s="123"/>
       <c r="I36" s="44"/>
       <c r="J36" s="44"/>
-      <c r="M36" s="133" t="s">
+      <c r="M36" s="124" t="s">
         <v>86</v>
       </c>
-      <c r="N36" s="133"/>
-      <c r="O36" s="133"/>
+      <c r="N36" s="124"/>
+      <c r="O36" s="124"/>
       <c r="Q36" s="42" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="37" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:17" ht="15">
       <c r="E37" s="44"/>
       <c r="F37" s="44"/>
     </row>
-    <row r="38" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:17" ht="15">
       <c r="K38" s="44"/>
     </row>
-    <row r="39" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:17" ht="15">
       <c r="B39" s="44"/>
       <c r="C39" s="44"/>
       <c r="K39" s="44"/>
       <c r="Q39" s="45"/>
     </row>
-    <row r="43" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:17" ht="14.25">
       <c r="B43" s="46"/>
       <c r="C43" s="46"/>
       <c r="D43" s="47"/>
@@ -6486,7 +6488,7 @@
       <c r="M43" s="49"/>
       <c r="N43" s="50"/>
     </row>
-    <row r="44" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:17" ht="14.25">
       <c r="B44" s="46"/>
       <c r="C44" s="46"/>
       <c r="D44" s="47"/>
@@ -6501,7 +6503,7 @@
       <c r="M44" s="49"/>
       <c r="N44" s="50"/>
     </row>
-    <row r="45" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:17" ht="15">
       <c r="B45" s="42"/>
       <c r="C45" s="42"/>
       <c r="D45" s="45"/>
@@ -6516,7 +6518,7 @@
       <c r="M45" s="45"/>
       <c r="N45" s="50"/>
     </row>
-    <row r="46" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:17" ht="15">
       <c r="B46" s="42"/>
       <c r="C46" s="42"/>
       <c r="D46" s="45"/>
@@ -6531,7 +6533,7 @@
       <c r="M46" s="45"/>
       <c r="N46" s="50"/>
     </row>
-    <row r="47" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:17" ht="15">
       <c r="B47" s="42"/>
       <c r="C47" s="42"/>
       <c r="D47" s="45"/>
@@ -6546,7 +6548,7 @@
       <c r="M47" s="45"/>
       <c r="N47" s="50"/>
     </row>
-    <row r="48" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:17" ht="14.25">
       <c r="B48" s="46"/>
       <c r="C48" s="46"/>
       <c r="D48" s="47"/>
@@ -6561,7 +6563,7 @@
       <c r="M48" s="49"/>
       <c r="N48" s="50"/>
     </row>
-    <row r="49" spans="2:14" ht="15" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:14" ht="15">
       <c r="B49" s="42"/>
       <c r="C49" s="42"/>
       <c r="D49" s="45"/>
@@ -6576,7 +6578,7 @@
       <c r="M49" s="45"/>
       <c r="N49" s="50"/>
     </row>
-    <row r="50" spans="2:14" ht="15" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:14" ht="15">
       <c r="B50" s="42"/>
       <c r="C50" s="42"/>
       <c r="D50" s="45"/>
@@ -6591,10 +6593,10 @@
       <c r="M50" s="49"/>
       <c r="N50" s="50"/>
     </row>
-    <row r="51" spans="2:14" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="B51" s="134"/>
-      <c r="C51" s="134"/>
-      <c r="D51" s="135"/>
+    <row r="51" spans="2:14" ht="14.25">
+      <c r="B51" s="115"/>
+      <c r="C51" s="115"/>
+      <c r="D51" s="116"/>
       <c r="E51" s="47"/>
       <c r="F51" s="47"/>
       <c r="G51" s="47"/>
@@ -6606,7 +6608,7 @@
       <c r="M51" s="49"/>
       <c r="N51" s="50"/>
     </row>
-    <row r="52" spans="2:14" ht="15" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:14" ht="15">
       <c r="B52" s="51"/>
       <c r="C52" s="51"/>
       <c r="D52" s="52"/>
@@ -6621,7 +6623,7 @@
       <c r="M52" s="49"/>
       <c r="N52" s="50"/>
     </row>
-    <row r="53" spans="2:14" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:14" ht="14.25">
       <c r="B53" s="46"/>
       <c r="C53" s="46"/>
       <c r="D53" s="47"/>
@@ -6636,7 +6638,7 @@
       <c r="M53" s="49"/>
       <c r="N53" s="50"/>
     </row>
-    <row r="54" spans="2:14" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:14" ht="14.25">
       <c r="B54" s="46"/>
       <c r="C54" s="46"/>
       <c r="D54" s="47"/>
@@ -6651,7 +6653,7 @@
       <c r="M54" s="49"/>
       <c r="N54" s="50"/>
     </row>
-    <row r="55" spans="2:14" ht="15" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:14" ht="15">
       <c r="B55" s="42"/>
       <c r="C55" s="42"/>
       <c r="D55" s="45"/>
@@ -6666,7 +6668,7 @@
       <c r="M55" s="45"/>
       <c r="N55" s="50"/>
     </row>
-    <row r="56" spans="2:14" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:14" ht="14.25">
       <c r="B56" s="46"/>
       <c r="C56" s="46"/>
       <c r="D56" s="47"/>
@@ -6681,7 +6683,7 @@
       <c r="M56" s="49"/>
       <c r="N56" s="50"/>
     </row>
-    <row r="57" spans="2:14" ht="15" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:14" ht="15">
       <c r="B57" s="42"/>
       <c r="C57" s="42"/>
       <c r="D57" s="45"/>
@@ -6696,7 +6698,7 @@
       <c r="M57" s="45"/>
       <c r="N57" s="50"/>
     </row>
-    <row r="58" spans="2:14" ht="15" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:14" ht="15">
       <c r="B58" s="42"/>
       <c r="C58" s="42"/>
       <c r="D58" s="45"/>
@@ -6711,7 +6713,7 @@
       <c r="M58" s="45"/>
       <c r="N58" s="50"/>
     </row>
-    <row r="59" spans="2:14" ht="15" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:14" ht="15">
       <c r="B59" s="42"/>
       <c r="C59" s="42"/>
       <c r="D59" s="45"/>
@@ -6726,10 +6728,10 @@
       <c r="M59" s="45"/>
       <c r="N59" s="50"/>
     </row>
-    <row r="60" spans="2:14" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="B60" s="134"/>
-      <c r="C60" s="134"/>
-      <c r="D60" s="135"/>
+    <row r="60" spans="2:14" ht="14.25">
+      <c r="B60" s="115"/>
+      <c r="C60" s="115"/>
+      <c r="D60" s="116"/>
       <c r="E60" s="47"/>
       <c r="F60" s="47"/>
       <c r="G60" s="47"/>
@@ -6741,7 +6743,7 @@
       <c r="M60" s="49"/>
       <c r="N60" s="50"/>
     </row>
-    <row r="61" spans="2:14" ht="15" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:14" ht="15">
       <c r="B61" s="42"/>
       <c r="C61" s="42"/>
       <c r="D61" s="45"/>
@@ -6756,7 +6758,7 @@
       <c r="M61" s="45"/>
       <c r="N61" s="50"/>
     </row>
-    <row r="62" spans="2:14" ht="15" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:14" ht="15">
       <c r="B62" s="42"/>
       <c r="C62" s="42"/>
       <c r="D62" s="45"/>
@@ -6771,10 +6773,10 @@
       <c r="M62" s="45"/>
       <c r="N62" s="50"/>
     </row>
-    <row r="63" spans="2:14" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="B63" s="134"/>
-      <c r="C63" s="134"/>
-      <c r="D63" s="135"/>
+    <row r="63" spans="2:14" ht="14.25">
+      <c r="B63" s="115"/>
+      <c r="C63" s="115"/>
+      <c r="D63" s="116"/>
       <c r="E63" s="47"/>
       <c r="F63" s="47"/>
       <c r="G63" s="47"/>
@@ -6786,7 +6788,7 @@
       <c r="M63" s="49"/>
       <c r="N63" s="50"/>
     </row>
-    <row r="64" spans="2:14" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:14" ht="14.25">
       <c r="B64" s="46"/>
       <c r="C64" s="46"/>
       <c r="D64" s="47"/>
@@ -6801,7 +6803,7 @@
       <c r="M64" s="49"/>
       <c r="N64" s="50"/>
     </row>
-    <row r="65" spans="2:14" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:14" ht="14.25">
       <c r="B65" s="46"/>
       <c r="C65" s="46"/>
       <c r="D65" s="47"/>
@@ -6816,7 +6818,7 @@
       <c r="M65" s="49"/>
       <c r="N65" s="50"/>
     </row>
-    <row r="66" spans="2:14" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:14" ht="14.25">
       <c r="B66" s="46"/>
       <c r="C66" s="46"/>
       <c r="D66" s="47"/>
@@ -6831,7 +6833,7 @@
       <c r="M66" s="49"/>
       <c r="N66" s="50"/>
     </row>
-    <row r="67" spans="2:14" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:14" ht="14.25">
       <c r="B67" s="46"/>
       <c r="C67" s="46"/>
       <c r="D67" s="47"/>
@@ -6846,7 +6848,7 @@
       <c r="M67" s="49"/>
       <c r="N67" s="50"/>
     </row>
-    <row r="68" spans="2:14" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:14" ht="14.25">
       <c r="B68" s="46"/>
       <c r="C68" s="46"/>
       <c r="D68" s="47"/>
@@ -6861,10 +6863,10 @@
       <c r="M68" s="49"/>
       <c r="N68" s="50"/>
     </row>
-    <row r="69" spans="2:14" ht="15" x14ac:dyDescent="0.2">
-      <c r="B69" s="151"/>
-      <c r="C69" s="151"/>
-      <c r="D69" s="151"/>
+    <row r="69" spans="2:14" ht="15">
+      <c r="B69" s="137"/>
+      <c r="C69" s="137"/>
+      <c r="D69" s="137"/>
       <c r="E69" s="47"/>
       <c r="F69" s="47"/>
       <c r="G69" s="47"/>
@@ -6876,7 +6878,7 @@
       <c r="M69" s="49"/>
       <c r="N69" s="50"/>
     </row>
-    <row r="70" spans="2:14" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:14" ht="14.25">
       <c r="B70" s="46"/>
       <c r="C70" s="46"/>
       <c r="D70" s="47"/>
@@ -6891,7 +6893,7 @@
       <c r="M70" s="49"/>
       <c r="N70" s="50"/>
     </row>
-    <row r="71" spans="2:14" ht="15" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:14" ht="15">
       <c r="B71" s="53"/>
       <c r="C71" s="53"/>
       <c r="D71" s="52"/>
@@ -6908,20 +6910,6 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="L9:N9"/>
-    <mergeCell ref="A1:R1"/>
-    <mergeCell ref="A2:R2"/>
-    <mergeCell ref="A3:R3"/>
-    <mergeCell ref="A5:R5"/>
-    <mergeCell ref="A7:G7"/>
-    <mergeCell ref="B69:D69"/>
-    <mergeCell ref="A32:D32"/>
-    <mergeCell ref="A35:D35"/>
-    <mergeCell ref="G35:H35"/>
-    <mergeCell ref="M35:O35"/>
-    <mergeCell ref="A36:D36"/>
     <mergeCell ref="AM12:AN13"/>
     <mergeCell ref="AB13:AB14"/>
     <mergeCell ref="B51:D51"/>
@@ -6938,6 +6926,20 @@
     <mergeCell ref="M36:O36"/>
     <mergeCell ref="AC12:AL12"/>
     <mergeCell ref="S12:AB12"/>
+    <mergeCell ref="B69:D69"/>
+    <mergeCell ref="A32:D32"/>
+    <mergeCell ref="A35:D35"/>
+    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="M35:O35"/>
+    <mergeCell ref="A36:D36"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="L9:N9"/>
+    <mergeCell ref="A1:R1"/>
+    <mergeCell ref="A2:R2"/>
+    <mergeCell ref="A3:R3"/>
+    <mergeCell ref="A5:R5"/>
+    <mergeCell ref="A7:G7"/>
   </mergeCells>
   <pageMargins left="0.5" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="258" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Refactor Employee module add Pipeline | Add DBM and CSC Report | Fix Promotion Report | Refactor BirthdayRepository
</commit_message>
<xml_diff>
--- a/public/CSC_PLANTILLA.xlsx
+++ b/public/CSC_PLANTILLA.xlsx
@@ -598,7 +598,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="000\-000\-000"/>
   </numFmts>
-  <fonts count="25">
+  <fonts count="24">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -635,11 +635,6 @@
     <font>
       <sz val="10"/>
       <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="13"/>
-      <name val="Candara"/>
       <family val="2"/>
     </font>
     <font>
@@ -1022,13 +1017,13 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="154">
+  <cellXfs count="156">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
@@ -1036,13 +1031,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1133,30 +1128,24 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1165,124 +1154,121 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="23" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="14" fontId="22" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="23" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="14" fontId="22" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="23" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="14" fontId="22" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="23" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="14" fontId="22" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="23" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="14" fontId="22" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="4" fontId="23" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="4" fontId="22" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="4" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="43" fontId="23" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="22" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="23" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="4" fontId="22" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="43" fontId="23" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="43" fontId="22" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="43" fontId="23" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="23" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="43" fontId="22" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="4" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1291,34 +1277,34 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="4" fontId="23" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="4" fontId="22" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="43" fontId="23" fillId="8" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="22" fillId="8" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="23" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="14" fontId="22" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="23" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="14" fontId="22" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1330,13 +1316,13 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="23" fillId="3" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="43" fontId="22" fillId="3" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="43" fontId="23" fillId="3" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="43" fontId="22" fillId="3" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1360,46 +1346,73 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="23" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="22" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="22" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="4" fontId="22" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="22" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1433,13 +1446,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" indent="7"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1475,20 +1488,8 @@
     <xf numFmtId="0" fontId="5" fillId="11" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="23" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -3125,8 +3126,8 @@
   </sheetPr>
   <dimension ref="A1:AB70"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A2" zoomScale="145" zoomScaleNormal="130" zoomScaleSheetLayoutView="145" workbookViewId="0">
-      <selection activeCell="P15" sqref="P15:AB25"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A10" zoomScale="145" zoomScaleNormal="130" zoomScaleSheetLayoutView="145" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -3149,7 +3150,7 @@
     <col min="17" max="17" width="11.7109375" style="2" customWidth="1"/>
     <col min="18" max="18" width="13" style="2" customWidth="1"/>
     <col min="19" max="19" width="12.5703125" style="2" customWidth="1"/>
-    <col min="20" max="20" width="12.5703125" style="104" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="12.5703125" style="101" hidden="1" customWidth="1"/>
     <col min="21" max="22" width="12.5703125" style="2" hidden="1" customWidth="1"/>
     <col min="23" max="23" width="14.42578125" style="2" hidden="1" customWidth="1"/>
     <col min="24" max="24" width="16.85546875" style="2" hidden="1" customWidth="1"/>
@@ -3180,161 +3181,161 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="15">
-      <c r="A1" s="125" t="s">
+      <c r="A1" s="131" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="125"/>
-      <c r="C1" s="125"/>
-      <c r="D1" s="125"/>
-      <c r="E1" s="125"/>
-      <c r="F1" s="125"/>
-      <c r="G1" s="125"/>
-      <c r="H1" s="125"/>
-      <c r="I1" s="125"/>
-      <c r="J1" s="125"/>
-      <c r="K1" s="125"/>
-      <c r="L1" s="125"/>
-      <c r="M1" s="125"/>
-      <c r="N1" s="125"/>
-      <c r="O1" s="125"/>
-      <c r="P1" s="125"/>
-      <c r="Q1" s="125"/>
-      <c r="R1" s="125"/>
-      <c r="S1" s="125"/>
-      <c r="T1" s="125"/>
-      <c r="U1" s="125"/>
-      <c r="V1" s="125"/>
-      <c r="W1" s="125"/>
-      <c r="X1" s="125"/>
-      <c r="Y1" s="125"/>
-      <c r="Z1" s="125"/>
-      <c r="AA1" s="125"/>
-      <c r="AB1" s="125"/>
+      <c r="B1" s="131"/>
+      <c r="C1" s="131"/>
+      <c r="D1" s="131"/>
+      <c r="E1" s="131"/>
+      <c r="F1" s="131"/>
+      <c r="G1" s="131"/>
+      <c r="H1" s="131"/>
+      <c r="I1" s="131"/>
+      <c r="J1" s="131"/>
+      <c r="K1" s="131"/>
+      <c r="L1" s="131"/>
+      <c r="M1" s="131"/>
+      <c r="N1" s="131"/>
+      <c r="O1" s="131"/>
+      <c r="P1" s="131"/>
+      <c r="Q1" s="131"/>
+      <c r="R1" s="131"/>
+      <c r="S1" s="131"/>
+      <c r="T1" s="131"/>
+      <c r="U1" s="131"/>
+      <c r="V1" s="131"/>
+      <c r="W1" s="131"/>
+      <c r="X1" s="131"/>
+      <c r="Y1" s="131"/>
+      <c r="Z1" s="131"/>
+      <c r="AA1" s="131"/>
+      <c r="AB1" s="131"/>
     </row>
     <row r="2" spans="1:28" ht="15">
-      <c r="A2" s="125" t="s">
+      <c r="A2" s="131" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="125"/>
-      <c r="C2" s="125"/>
-      <c r="D2" s="125"/>
-      <c r="E2" s="125"/>
-      <c r="F2" s="125"/>
-      <c r="G2" s="125"/>
-      <c r="H2" s="125"/>
-      <c r="I2" s="125"/>
-      <c r="J2" s="125"/>
-      <c r="K2" s="125"/>
-      <c r="L2" s="125"/>
-      <c r="M2" s="125"/>
-      <c r="N2" s="125"/>
-      <c r="O2" s="125"/>
-      <c r="P2" s="125"/>
-      <c r="Q2" s="125"/>
-      <c r="R2" s="125"/>
-      <c r="S2" s="125"/>
-      <c r="T2" s="125"/>
-      <c r="U2" s="125"/>
-      <c r="V2" s="125"/>
-      <c r="W2" s="125"/>
-      <c r="X2" s="125"/>
-      <c r="Y2" s="125"/>
-      <c r="Z2" s="125"/>
-      <c r="AA2" s="125"/>
-      <c r="AB2" s="125"/>
+      <c r="B2" s="131"/>
+      <c r="C2" s="131"/>
+      <c r="D2" s="131"/>
+      <c r="E2" s="131"/>
+      <c r="F2" s="131"/>
+      <c r="G2" s="131"/>
+      <c r="H2" s="131"/>
+      <c r="I2" s="131"/>
+      <c r="J2" s="131"/>
+      <c r="K2" s="131"/>
+      <c r="L2" s="131"/>
+      <c r="M2" s="131"/>
+      <c r="N2" s="131"/>
+      <c r="O2" s="131"/>
+      <c r="P2" s="131"/>
+      <c r="Q2" s="131"/>
+      <c r="R2" s="131"/>
+      <c r="S2" s="131"/>
+      <c r="T2" s="131"/>
+      <c r="U2" s="131"/>
+      <c r="V2" s="131"/>
+      <c r="W2" s="131"/>
+      <c r="X2" s="131"/>
+      <c r="Y2" s="131"/>
+      <c r="Z2" s="131"/>
+      <c r="AA2" s="131"/>
+      <c r="AB2" s="131"/>
     </row>
     <row r="3" spans="1:28" ht="14.25">
-      <c r="A3" s="126" t="s">
+      <c r="A3" s="132" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="126"/>
-      <c r="C3" s="126"/>
-      <c r="D3" s="126"/>
-      <c r="E3" s="126"/>
-      <c r="F3" s="126"/>
-      <c r="G3" s="126"/>
-      <c r="H3" s="126"/>
-      <c r="I3" s="126"/>
-      <c r="J3" s="126"/>
-      <c r="K3" s="126"/>
-      <c r="L3" s="126"/>
-      <c r="M3" s="126"/>
-      <c r="N3" s="126"/>
-      <c r="O3" s="126"/>
-      <c r="P3" s="126"/>
-      <c r="Q3" s="126"/>
-      <c r="R3" s="126"/>
-      <c r="S3" s="126"/>
-      <c r="T3" s="126"/>
-      <c r="U3" s="126"/>
-      <c r="V3" s="126"/>
-      <c r="W3" s="126"/>
-      <c r="X3" s="126"/>
-      <c r="Y3" s="126"/>
-      <c r="Z3" s="126"/>
-      <c r="AA3" s="126"/>
-      <c r="AB3" s="126"/>
+      <c r="B3" s="132"/>
+      <c r="C3" s="132"/>
+      <c r="D3" s="132"/>
+      <c r="E3" s="132"/>
+      <c r="F3" s="132"/>
+      <c r="G3" s="132"/>
+      <c r="H3" s="132"/>
+      <c r="I3" s="132"/>
+      <c r="J3" s="132"/>
+      <c r="K3" s="132"/>
+      <c r="L3" s="132"/>
+      <c r="M3" s="132"/>
+      <c r="N3" s="132"/>
+      <c r="O3" s="132"/>
+      <c r="P3" s="132"/>
+      <c r="Q3" s="132"/>
+      <c r="R3" s="132"/>
+      <c r="S3" s="132"/>
+      <c r="T3" s="132"/>
+      <c r="U3" s="132"/>
+      <c r="V3" s="132"/>
+      <c r="W3" s="132"/>
+      <c r="X3" s="132"/>
+      <c r="Y3" s="132"/>
+      <c r="Z3" s="132"/>
+      <c r="AA3" s="132"/>
+      <c r="AB3" s="132"/>
     </row>
     <row r="4" spans="1:28" ht="12.75" customHeight="1">
-      <c r="A4" s="125" t="s">
+      <c r="A4" s="131" t="s">
         <v>159</v>
       </c>
-      <c r="B4" s="125"/>
-      <c r="C4" s="125"/>
-      <c r="D4" s="125"/>
-      <c r="E4" s="125"/>
-      <c r="F4" s="125"/>
-      <c r="G4" s="125"/>
-      <c r="H4" s="125"/>
-      <c r="I4" s="125"/>
-      <c r="J4" s="125"/>
-      <c r="K4" s="125"/>
-      <c r="L4" s="125"/>
-      <c r="M4" s="125"/>
-      <c r="N4" s="125"/>
-      <c r="O4" s="125"/>
-      <c r="P4" s="125"/>
-      <c r="Q4" s="125"/>
-      <c r="R4" s="125"/>
-      <c r="S4" s="125"/>
-      <c r="T4" s="125"/>
-      <c r="U4" s="125"/>
-      <c r="V4" s="125"/>
-      <c r="W4" s="125"/>
-      <c r="X4" s="125"/>
-      <c r="Y4" s="125"/>
-      <c r="Z4" s="125"/>
-      <c r="AA4" s="125"/>
-      <c r="AB4" s="125"/>
+      <c r="B4" s="131"/>
+      <c r="C4" s="131"/>
+      <c r="D4" s="131"/>
+      <c r="E4" s="131"/>
+      <c r="F4" s="131"/>
+      <c r="G4" s="131"/>
+      <c r="H4" s="131"/>
+      <c r="I4" s="131"/>
+      <c r="J4" s="131"/>
+      <c r="K4" s="131"/>
+      <c r="L4" s="131"/>
+      <c r="M4" s="131"/>
+      <c r="N4" s="131"/>
+      <c r="O4" s="131"/>
+      <c r="P4" s="131"/>
+      <c r="Q4" s="131"/>
+      <c r="R4" s="131"/>
+      <c r="S4" s="131"/>
+      <c r="T4" s="131"/>
+      <c r="U4" s="131"/>
+      <c r="V4" s="131"/>
+      <c r="W4" s="131"/>
+      <c r="X4" s="131"/>
+      <c r="Y4" s="131"/>
+      <c r="Z4" s="131"/>
+      <c r="AA4" s="131"/>
+      <c r="AB4" s="131"/>
     </row>
     <row r="5" spans="1:28" ht="15" customHeight="1">
-      <c r="B5" s="44"/>
-      <c r="C5" s="44"/>
-      <c r="D5" s="44"/>
-      <c r="E5" s="44"/>
-      <c r="F5" s="44"/>
-      <c r="G5" s="44"/>
-      <c r="H5" s="44"/>
-      <c r="I5" s="44"/>
-      <c r="J5" s="44"/>
-      <c r="K5" s="44"/>
-      <c r="L5" s="44"/>
-      <c r="M5" s="44"/>
-      <c r="N5" s="44"/>
-      <c r="O5" s="44"/>
-      <c r="P5" s="44"/>
-      <c r="Q5" s="44"/>
-      <c r="R5" s="44"/>
-      <c r="S5" s="44"/>
-      <c r="T5" s="44"/>
-      <c r="U5" s="44"/>
-      <c r="V5" s="44"/>
-      <c r="W5" s="44"/>
-      <c r="X5" s="44"/>
-      <c r="Y5" s="44"/>
-      <c r="Z5" s="44"/>
-      <c r="AA5" s="44"/>
-      <c r="AB5" s="44"/>
+      <c r="B5" s="42"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="42"/>
+      <c r="H5" s="42"/>
+      <c r="I5" s="42"/>
+      <c r="J5" s="42"/>
+      <c r="K5" s="42"/>
+      <c r="L5" s="42"/>
+      <c r="M5" s="42"/>
+      <c r="N5" s="42"/>
+      <c r="O5" s="42"/>
+      <c r="P5" s="42"/>
+      <c r="Q5" s="42"/>
+      <c r="R5" s="42"/>
+      <c r="S5" s="42"/>
+      <c r="T5" s="42"/>
+      <c r="U5" s="42"/>
+      <c r="V5" s="42"/>
+      <c r="W5" s="42"/>
+      <c r="X5" s="42"/>
+      <c r="Y5" s="42"/>
+      <c r="Z5" s="42"/>
+      <c r="AA5" s="42"/>
+      <c r="AB5" s="42"/>
     </row>
     <row r="7" spans="1:28" ht="15">
       <c r="A7" s="3" t="s">
@@ -3360,7 +3361,7 @@
       <c r="Q7" s="6"/>
       <c r="R7" s="6"/>
       <c r="S7" s="6"/>
-      <c r="T7" s="105"/>
+      <c r="T7" s="102"/>
       <c r="U7" s="6"/>
       <c r="V7" s="6"/>
       <c r="W7" s="6"/>
@@ -3390,7 +3391,7 @@
       <c r="Q8" s="12"/>
       <c r="R8" s="12"/>
       <c r="S8" s="12"/>
-      <c r="T8" s="106"/>
+      <c r="T8" s="103"/>
       <c r="U8" s="12"/>
       <c r="V8" s="12"/>
       <c r="W8" s="12"/>
@@ -3408,25 +3409,25 @@
       <c r="E9" s="14"/>
       <c r="F9" s="14"/>
       <c r="G9" s="15"/>
-      <c r="H9" s="127" t="s">
+      <c r="H9" s="133" t="s">
         <v>5</v>
       </c>
-      <c r="I9" s="128"/>
-      <c r="J9" s="128"/>
-      <c r="K9" s="129"/>
+      <c r="I9" s="134"/>
+      <c r="J9" s="134"/>
+      <c r="K9" s="135"/>
       <c r="L9" s="14"/>
-      <c r="M9" s="130" t="s">
+      <c r="M9" s="136" t="s">
         <v>6</v>
       </c>
-      <c r="N9" s="131"/>
+      <c r="N9" s="137"/>
       <c r="O9" s="14"/>
-      <c r="P9" s="132" t="s">
+      <c r="P9" s="138" t="s">
         <v>7</v>
       </c>
-      <c r="Q9" s="133"/>
-      <c r="R9" s="134"/>
+      <c r="Q9" s="139"/>
+      <c r="R9" s="140"/>
       <c r="S9" s="15"/>
-      <c r="T9" s="107"/>
+      <c r="T9" s="104"/>
       <c r="U9" s="15"/>
       <c r="V9" s="15"/>
       <c r="W9" s="15"/>
@@ -3450,23 +3451,23 @@
       <c r="I10" s="15"/>
       <c r="J10" s="15"/>
       <c r="K10" s="15"/>
-      <c r="L10" s="20" t="s">
+      <c r="L10" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="M10" s="21" t="s">
+      <c r="M10" s="119" t="s">
         <v>10</v>
       </c>
-      <c r="N10" s="21" t="s">
+      <c r="N10" s="119" t="s">
         <v>11</v>
       </c>
-      <c r="O10" s="20" t="s">
+      <c r="O10" s="17" t="s">
         <v>12</v>
       </c>
       <c r="P10" s="14"/>
       <c r="Q10" s="15"/>
       <c r="R10" s="15"/>
       <c r="S10" s="17"/>
-      <c r="T10" s="108"/>
+      <c r="T10" s="105"/>
       <c r="U10" s="17"/>
       <c r="V10" s="17"/>
       <c r="W10" s="17"/>
@@ -3504,16 +3505,16 @@
       <c r="K11" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="L11" s="20" t="s">
+      <c r="L11" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="M11" s="20" t="s">
+      <c r="M11" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="N11" s="20" t="s">
+      <c r="N11" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="O11" s="20" t="s">
+      <c r="O11" s="17" t="s">
         <v>21</v>
       </c>
       <c r="P11" s="18"/>
@@ -3522,7 +3523,7 @@
       <c r="S11" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="T11" s="108"/>
+      <c r="T11" s="105"/>
       <c r="U11" s="17"/>
       <c r="V11" s="17"/>
       <c r="W11" s="17"/>
@@ -3550,16 +3551,16 @@
       <c r="I12" s="19"/>
       <c r="J12" s="19"/>
       <c r="K12" s="19"/>
-      <c r="L12" s="20" t="s">
+      <c r="L12" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="M12" s="20" t="s">
+      <c r="M12" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="N12" s="20" t="s">
+      <c r="N12" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="O12" s="20" t="s">
+      <c r="O12" s="17" t="s">
         <v>28</v>
       </c>
       <c r="P12" s="23" t="s">
@@ -3574,7 +3575,7 @@
       <c r="S12" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="T12" s="109"/>
+      <c r="T12" s="106"/>
       <c r="U12" s="24"/>
       <c r="V12" s="24"/>
       <c r="W12" s="24"/>
@@ -3600,23 +3601,23 @@
       <c r="I13" s="19"/>
       <c r="J13" s="19"/>
       <c r="K13" s="19"/>
-      <c r="L13" s="20" t="s">
+      <c r="L13" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="M13" s="20" t="s">
+      <c r="M13" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="N13" s="20" t="s">
+      <c r="N13" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="O13" s="20" t="s">
+      <c r="O13" s="17" t="s">
         <v>37</v>
       </c>
       <c r="P13" s="18"/>
       <c r="Q13" s="19"/>
       <c r="R13" s="19"/>
       <c r="S13" s="24"/>
-      <c r="T13" s="109"/>
+      <c r="T13" s="106"/>
       <c r="U13" s="24">
         <v>2019</v>
       </c>
@@ -3680,7 +3681,7 @@
       <c r="S14" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="T14" s="110"/>
+      <c r="T14" s="107"/>
       <c r="U14" s="25" t="s">
         <v>154</v>
       </c>
@@ -3708,77 +3709,77 @@
     </row>
     <row r="15" spans="1:28" ht="15">
       <c r="A15" s="28"/>
-      <c r="B15" s="55"/>
-      <c r="C15" s="55"/>
-      <c r="D15" s="56"/>
-      <c r="E15" s="56"/>
-      <c r="F15" s="63"/>
-      <c r="G15" s="66"/>
-      <c r="H15" s="69"/>
-      <c r="I15" s="103"/>
-      <c r="J15" s="102"/>
-      <c r="K15" s="72"/>
-      <c r="L15" s="66"/>
-      <c r="M15" s="66"/>
-      <c r="N15" s="66"/>
-      <c r="O15" s="66"/>
-      <c r="P15" s="149"/>
-      <c r="Q15" s="66"/>
-      <c r="R15" s="66"/>
-      <c r="S15" s="60"/>
-      <c r="U15" s="150"/>
-      <c r="V15" s="151"/>
-      <c r="W15" s="114"/>
-      <c r="X15" s="152"/>
-      <c r="Y15" s="152"/>
-      <c r="Z15" s="60"/>
-      <c r="AA15" s="60"/>
-      <c r="AB15" s="66"/>
+      <c r="B15" s="53"/>
+      <c r="C15" s="53"/>
+      <c r="D15" s="54"/>
+      <c r="E15" s="54"/>
+      <c r="F15" s="61"/>
+      <c r="G15" s="64"/>
+      <c r="H15" s="117"/>
+      <c r="I15" s="100"/>
+      <c r="J15" s="99"/>
+      <c r="K15" s="118"/>
+      <c r="L15" s="64"/>
+      <c r="M15" s="64"/>
+      <c r="N15" s="64"/>
+      <c r="O15" s="64"/>
+      <c r="P15" s="112"/>
+      <c r="Q15" s="64"/>
+      <c r="R15" s="64"/>
+      <c r="S15" s="58"/>
+      <c r="U15" s="113"/>
+      <c r="V15" s="114"/>
+      <c r="W15" s="111"/>
+      <c r="X15" s="115"/>
+      <c r="Y15" s="115"/>
+      <c r="Z15" s="58"/>
+      <c r="AA15" s="58"/>
+      <c r="AB15" s="64"/>
     </row>
     <row r="16" spans="1:28" ht="15">
       <c r="A16" s="28"/>
-      <c r="B16" s="55"/>
-      <c r="C16" s="55"/>
-      <c r="D16" s="56"/>
-      <c r="E16" s="56"/>
-      <c r="F16" s="63"/>
-      <c r="G16" s="66"/>
-      <c r="H16" s="75"/>
-      <c r="I16" s="75"/>
-      <c r="J16" s="75"/>
-      <c r="K16" s="76"/>
-      <c r="L16" s="66"/>
-      <c r="M16" s="66"/>
-      <c r="N16" s="66"/>
-      <c r="O16" s="66"/>
-      <c r="P16" s="66"/>
-      <c r="Q16" s="66"/>
-      <c r="R16" s="66"/>
-      <c r="S16" s="60"/>
-      <c r="T16" s="153" t="s">
+      <c r="B16" s="53"/>
+      <c r="C16" s="53"/>
+      <c r="D16" s="54"/>
+      <c r="E16" s="54"/>
+      <c r="F16" s="61"/>
+      <c r="G16" s="64"/>
+      <c r="H16" s="117"/>
+      <c r="I16" s="73"/>
+      <c r="J16" s="73"/>
+      <c r="K16" s="117"/>
+      <c r="L16" s="64"/>
+      <c r="M16" s="64"/>
+      <c r="N16" s="64"/>
+      <c r="O16" s="64"/>
+      <c r="P16" s="64"/>
+      <c r="Q16" s="64"/>
+      <c r="R16" s="64"/>
+      <c r="S16" s="58"/>
+      <c r="T16" s="116" t="s">
         <v>146</v>
       </c>
-      <c r="U16" s="153"/>
-      <c r="V16" s="150"/>
-      <c r="W16" s="150"/>
-      <c r="X16" s="150"/>
-      <c r="Y16" s="150"/>
-      <c r="Z16" s="60"/>
-      <c r="AA16" s="68"/>
-      <c r="AB16" s="66"/>
+      <c r="U16" s="116"/>
+      <c r="V16" s="113"/>
+      <c r="W16" s="113"/>
+      <c r="X16" s="113"/>
+      <c r="Y16" s="113"/>
+      <c r="Z16" s="58"/>
+      <c r="AA16" s="66"/>
+      <c r="AB16" s="64"/>
     </row>
     <row r="17" spans="1:28" ht="15">
       <c r="A17" s="28"/>
       <c r="B17" s="29"/>
       <c r="C17" s="29"/>
-      <c r="D17" s="56"/>
-      <c r="E17" s="56"/>
-      <c r="F17" s="63"/>
+      <c r="D17" s="54"/>
+      <c r="E17" s="54"/>
+      <c r="F17" s="61"/>
       <c r="G17" s="30"/>
-      <c r="H17" s="33"/>
+      <c r="H17" s="117"/>
       <c r="I17" s="33"/>
       <c r="J17" s="33"/>
-      <c r="K17" s="34"/>
+      <c r="K17" s="120"/>
       <c r="L17" s="30"/>
       <c r="M17" s="30"/>
       <c r="N17" s="30"/>
@@ -3787,30 +3788,30 @@
       <c r="Q17" s="30"/>
       <c r="R17" s="30"/>
       <c r="S17" s="30"/>
-      <c r="T17" s="153" t="s">
+      <c r="T17" s="116" t="s">
         <v>144</v>
       </c>
-      <c r="U17" s="153"/>
-      <c r="V17" s="150"/>
-      <c r="W17" s="150"/>
-      <c r="X17" s="150"/>
-      <c r="Y17" s="150"/>
+      <c r="U17" s="116"/>
+      <c r="V17" s="113"/>
+      <c r="W17" s="113"/>
+      <c r="X17" s="113"/>
+      <c r="Y17" s="113"/>
       <c r="Z17" s="30"/>
-      <c r="AA17" s="35"/>
+      <c r="AA17" s="155"/>
       <c r="AB17" s="30"/>
     </row>
     <row r="18" spans="1:28" ht="15">
       <c r="A18" s="28"/>
       <c r="B18" s="29"/>
       <c r="C18" s="29"/>
-      <c r="D18" s="56"/>
-      <c r="E18" s="56"/>
-      <c r="F18" s="63"/>
+      <c r="D18" s="54"/>
+      <c r="E18" s="54"/>
+      <c r="F18" s="61"/>
       <c r="G18" s="30"/>
-      <c r="H18" s="33"/>
+      <c r="H18" s="117"/>
       <c r="I18" s="33"/>
       <c r="J18" s="33"/>
-      <c r="K18" s="34"/>
+      <c r="K18" s="120"/>
       <c r="L18" s="30"/>
       <c r="M18" s="30"/>
       <c r="N18" s="30"/>
@@ -3819,30 +3820,30 @@
       <c r="Q18" s="30"/>
       <c r="R18" s="30"/>
       <c r="S18" s="30"/>
-      <c r="T18" s="153" t="s">
+      <c r="T18" s="116" t="s">
         <v>147</v>
       </c>
-      <c r="U18" s="153"/>
-      <c r="V18" s="150"/>
-      <c r="W18" s="150"/>
-      <c r="X18" s="150"/>
-      <c r="Y18" s="150"/>
+      <c r="U18" s="116"/>
+      <c r="V18" s="113"/>
+      <c r="W18" s="113"/>
+      <c r="X18" s="113"/>
+      <c r="Y18" s="113"/>
       <c r="Z18" s="30"/>
-      <c r="AA18" s="35"/>
+      <c r="AA18" s="155"/>
       <c r="AB18" s="30"/>
     </row>
     <row r="19" spans="1:28" ht="15">
       <c r="A19" s="28"/>
       <c r="B19" s="29"/>
       <c r="C19" s="29"/>
-      <c r="D19" s="56"/>
-      <c r="E19" s="56"/>
-      <c r="F19" s="63"/>
+      <c r="D19" s="54"/>
+      <c r="E19" s="54"/>
+      <c r="F19" s="61"/>
       <c r="G19" s="30"/>
-      <c r="H19" s="33"/>
+      <c r="H19" s="117"/>
       <c r="I19" s="33"/>
       <c r="J19" s="33"/>
-      <c r="K19" s="34"/>
+      <c r="K19" s="120"/>
       <c r="L19" s="30"/>
       <c r="M19" s="30"/>
       <c r="N19" s="30"/>
@@ -3851,62 +3852,62 @@
       <c r="Q19" s="30"/>
       <c r="R19" s="30"/>
       <c r="S19" s="30"/>
-      <c r="T19" s="153" t="s">
+      <c r="T19" s="116" t="s">
         <v>148</v>
       </c>
-      <c r="U19" s="153"/>
-      <c r="V19" s="150"/>
-      <c r="W19" s="150"/>
-      <c r="X19" s="150"/>
-      <c r="Y19" s="150"/>
+      <c r="U19" s="116"/>
+      <c r="V19" s="113"/>
+      <c r="W19" s="113"/>
+      <c r="X19" s="113"/>
+      <c r="Y19" s="113"/>
       <c r="Z19" s="30"/>
-      <c r="AA19" s="35"/>
+      <c r="AA19" s="155"/>
       <c r="AB19" s="30"/>
     </row>
     <row r="20" spans="1:28" ht="15">
       <c r="A20" s="28"/>
       <c r="B20" s="29"/>
       <c r="C20" s="29"/>
-      <c r="D20" s="56"/>
-      <c r="E20" s="56"/>
-      <c r="F20" s="63"/>
+      <c r="D20" s="54"/>
+      <c r="E20" s="54"/>
+      <c r="F20" s="61"/>
       <c r="G20" s="30"/>
-      <c r="H20" s="33"/>
+      <c r="H20" s="117"/>
       <c r="I20" s="33"/>
       <c r="J20" s="33"/>
-      <c r="K20" s="34"/>
+      <c r="K20" s="120"/>
       <c r="L20" s="30"/>
       <c r="M20" s="30"/>
       <c r="N20" s="30"/>
       <c r="O20" s="30"/>
       <c r="P20" s="30"/>
-      <c r="Q20" s="36"/>
+      <c r="Q20" s="35"/>
       <c r="R20" s="30"/>
       <c r="S20" s="31"/>
-      <c r="T20" s="153" t="s">
+      <c r="T20" s="116" t="s">
         <v>149</v>
       </c>
-      <c r="U20" s="153"/>
-      <c r="V20" s="150"/>
-      <c r="W20" s="150"/>
-      <c r="X20" s="150"/>
-      <c r="Y20" s="150"/>
+      <c r="U20" s="116"/>
+      <c r="V20" s="113"/>
+      <c r="W20" s="113"/>
+      <c r="X20" s="113"/>
+      <c r="Y20" s="113"/>
       <c r="Z20" s="31"/>
-      <c r="AA20" s="30"/>
+      <c r="AA20" s="31"/>
       <c r="AB20" s="30"/>
     </row>
     <row r="21" spans="1:28" ht="15">
       <c r="A21" s="28"/>
       <c r="B21" s="29"/>
       <c r="C21" s="29"/>
-      <c r="D21" s="56"/>
-      <c r="E21" s="56"/>
-      <c r="F21" s="63"/>
+      <c r="D21" s="54"/>
+      <c r="E21" s="54"/>
+      <c r="F21" s="61"/>
       <c r="G21" s="30"/>
-      <c r="H21" s="33"/>
+      <c r="H21" s="117"/>
       <c r="I21" s="33"/>
       <c r="J21" s="33"/>
-      <c r="K21" s="34"/>
+      <c r="K21" s="120"/>
       <c r="L21" s="30"/>
       <c r="M21" s="30"/>
       <c r="N21" s="30"/>
@@ -3915,30 +3916,30 @@
       <c r="Q21" s="30"/>
       <c r="R21" s="30"/>
       <c r="S21" s="30"/>
-      <c r="T21" s="153" t="s">
+      <c r="T21" s="116" t="s">
         <v>150</v>
       </c>
-      <c r="U21" s="153"/>
-      <c r="V21" s="150"/>
-      <c r="W21" s="150"/>
-      <c r="X21" s="150"/>
-      <c r="Y21" s="150"/>
+      <c r="U21" s="116"/>
+      <c r="V21" s="113"/>
+      <c r="W21" s="113"/>
+      <c r="X21" s="113"/>
+      <c r="Y21" s="113"/>
       <c r="Z21" s="30"/>
-      <c r="AA21" s="30"/>
+      <c r="AA21" s="31"/>
       <c r="AB21" s="30"/>
     </row>
     <row r="22" spans="1:28" ht="15">
       <c r="A22" s="28"/>
       <c r="B22" s="29"/>
       <c r="C22" s="29"/>
-      <c r="D22" s="56"/>
-      <c r="E22" s="56"/>
-      <c r="F22" s="63"/>
+      <c r="D22" s="54"/>
+      <c r="E22" s="54"/>
+      <c r="F22" s="61"/>
       <c r="G22" s="30"/>
-      <c r="H22" s="33"/>
+      <c r="H22" s="117"/>
       <c r="I22" s="33"/>
       <c r="J22" s="33"/>
-      <c r="K22" s="34"/>
+      <c r="K22" s="120"/>
       <c r="L22" s="30"/>
       <c r="M22" s="30"/>
       <c r="N22" s="30"/>
@@ -3947,30 +3948,30 @@
       <c r="Q22" s="30"/>
       <c r="R22" s="30"/>
       <c r="S22" s="30"/>
-      <c r="T22" s="153" t="s">
+      <c r="T22" s="116" t="s">
         <v>151</v>
       </c>
-      <c r="U22" s="153"/>
-      <c r="V22" s="150"/>
-      <c r="W22" s="150"/>
-      <c r="X22" s="150"/>
-      <c r="Y22" s="150"/>
+      <c r="U22" s="116"/>
+      <c r="V22" s="113"/>
+      <c r="W22" s="113"/>
+      <c r="X22" s="113"/>
+      <c r="Y22" s="113"/>
       <c r="Z22" s="30"/>
-      <c r="AA22" s="30"/>
+      <c r="AA22" s="31"/>
       <c r="AB22" s="30"/>
     </row>
     <row r="23" spans="1:28" ht="15">
       <c r="A23" s="28"/>
       <c r="B23" s="29"/>
       <c r="C23" s="29"/>
-      <c r="D23" s="56"/>
-      <c r="E23" s="56"/>
-      <c r="F23" s="63"/>
+      <c r="D23" s="54"/>
+      <c r="E23" s="54"/>
+      <c r="F23" s="61"/>
       <c r="G23" s="30"/>
-      <c r="H23" s="33"/>
+      <c r="H23" s="117"/>
       <c r="I23" s="33"/>
       <c r="J23" s="33"/>
-      <c r="K23" s="34"/>
+      <c r="K23" s="120"/>
       <c r="L23" s="30"/>
       <c r="M23" s="30"/>
       <c r="N23" s="30"/>
@@ -3979,30 +3980,30 @@
       <c r="Q23" s="30"/>
       <c r="R23" s="30"/>
       <c r="S23" s="30"/>
-      <c r="T23" s="153" t="s">
+      <c r="T23" s="116" t="s">
         <v>152</v>
       </c>
-      <c r="U23" s="153"/>
-      <c r="V23" s="150"/>
-      <c r="W23" s="150"/>
-      <c r="X23" s="150"/>
-      <c r="Y23" s="150"/>
+      <c r="U23" s="116"/>
+      <c r="V23" s="113"/>
+      <c r="W23" s="113"/>
+      <c r="X23" s="113"/>
+      <c r="Y23" s="113"/>
       <c r="Z23" s="30"/>
-      <c r="AA23" s="30"/>
+      <c r="AA23" s="31"/>
       <c r="AB23" s="30"/>
     </row>
-    <row r="24" spans="1:28" ht="17.25">
+    <row r="24" spans="1:28" ht="15">
       <c r="A24" s="28"/>
       <c r="B24" s="29"/>
       <c r="C24" s="29"/>
-      <c r="D24" s="56"/>
-      <c r="E24" s="56"/>
-      <c r="F24" s="63"/>
+      <c r="D24" s="54"/>
+      <c r="E24" s="54"/>
+      <c r="F24" s="61"/>
       <c r="G24" s="30"/>
-      <c r="H24" s="33"/>
+      <c r="H24" s="117"/>
       <c r="I24" s="33"/>
       <c r="J24" s="33"/>
-      <c r="K24" s="34"/>
+      <c r="K24" s="120"/>
       <c r="L24" s="30"/>
       <c r="M24" s="30"/>
       <c r="N24" s="30"/>
@@ -4011,30 +4012,30 @@
       <c r="Q24" s="30"/>
       <c r="R24" s="30"/>
       <c r="S24" s="30"/>
-      <c r="T24" s="153" t="s">
+      <c r="T24" s="116" t="s">
         <v>153</v>
       </c>
-      <c r="U24" s="153"/>
-      <c r="V24" s="150"/>
-      <c r="W24" s="150"/>
-      <c r="X24" s="150"/>
-      <c r="Y24" s="150"/>
+      <c r="U24" s="116"/>
+      <c r="V24" s="113"/>
+      <c r="W24" s="113"/>
+      <c r="X24" s="113"/>
+      <c r="Y24" s="113"/>
       <c r="Z24" s="30"/>
-      <c r="AA24" s="37"/>
+      <c r="AA24" s="58"/>
       <c r="AB24" s="30"/>
     </row>
     <row r="25" spans="1:28" ht="15">
       <c r="A25" s="28"/>
       <c r="B25" s="29"/>
       <c r="C25" s="29"/>
-      <c r="D25" s="56"/>
-      <c r="E25" s="56"/>
-      <c r="F25" s="63"/>
+      <c r="D25" s="54"/>
+      <c r="E25" s="54"/>
+      <c r="F25" s="61"/>
       <c r="G25" s="30"/>
-      <c r="H25" s="34"/>
+      <c r="H25" s="117"/>
       <c r="I25" s="34"/>
       <c r="J25" s="34"/>
-      <c r="K25" s="34"/>
+      <c r="K25" s="120"/>
       <c r="L25" s="30"/>
       <c r="M25" s="30"/>
       <c r="N25" s="30"/>
@@ -4043,532 +4044,532 @@
       <c r="Q25" s="30"/>
       <c r="R25" s="30"/>
       <c r="S25" s="30"/>
-      <c r="T25" s="153" t="s">
+      <c r="T25" s="116" t="s">
         <v>145</v>
       </c>
-      <c r="U25" s="153"/>
-      <c r="V25" s="150"/>
-      <c r="W25" s="150"/>
-      <c r="X25" s="150"/>
-      <c r="Y25" s="150"/>
+      <c r="U25" s="116"/>
+      <c r="V25" s="113"/>
+      <c r="W25" s="113"/>
+      <c r="X25" s="113"/>
+      <c r="Y25" s="113"/>
       <c r="Z25" s="30"/>
       <c r="AA25" s="31"/>
       <c r="AB25" s="30"/>
     </row>
     <row r="26" spans="1:28" ht="15">
-      <c r="A26" s="38" t="s">
+      <c r="A26" s="36" t="s">
         <v>117</v>
       </c>
-      <c r="V26" s="111"/>
-      <c r="W26" s="111"/>
-      <c r="X26" s="111"/>
-      <c r="Y26" s="111"/>
+      <c r="V26" s="108"/>
+      <c r="W26" s="108"/>
+      <c r="X26" s="108"/>
+      <c r="Y26" s="108"/>
     </row>
     <row r="27" spans="1:28" ht="15">
-      <c r="V27" s="111"/>
-      <c r="W27" s="111"/>
-      <c r="X27" s="111"/>
-      <c r="Y27" s="111"/>
-      <c r="AB27" s="39" t="s">
+      <c r="V27" s="108"/>
+      <c r="W27" s="108"/>
+      <c r="X27" s="108"/>
+      <c r="Y27" s="108"/>
+      <c r="AB27" s="37" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="28" spans="1:28">
-      <c r="A28" s="38" t="s">
+      <c r="A28" s="36" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="29" spans="1:28" ht="15">
-      <c r="A29" s="38" t="s">
+      <c r="A29" s="36" t="s">
         <v>66</v>
       </c>
-      <c r="AB29" s="42" t="s">
+      <c r="AB29" s="40" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="30" spans="1:28" ht="15">
-      <c r="A30" s="38" t="s">
+      <c r="A30" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="AB30" s="42" t="s">
+      <c r="AB30" s="40" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="31" spans="1:28" ht="15">
-      <c r="AB31" s="42" t="s">
+      <c r="AB31" s="40" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="32" spans="1:28" ht="15">
-      <c r="F32" s="117" t="s">
+      <c r="F32" s="123" t="s">
         <v>70</v>
       </c>
-      <c r="G32" s="117"/>
-      <c r="H32" s="117"/>
-      <c r="I32" s="117"/>
-      <c r="J32" s="117"/>
-      <c r="K32" s="117"/>
-      <c r="L32" s="117"/>
-      <c r="Q32" s="43" t="s">
+      <c r="G32" s="123"/>
+      <c r="H32" s="123"/>
+      <c r="I32" s="123"/>
+      <c r="J32" s="123"/>
+      <c r="K32" s="123"/>
+      <c r="L32" s="123"/>
+      <c r="Q32" s="41" t="s">
         <v>71</v>
       </c>
-      <c r="AB32" s="42" t="s">
+      <c r="AB32" s="40" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="33" spans="1:28" ht="15">
-      <c r="AB33" s="42" t="s">
+      <c r="AB33" s="40" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="34" spans="1:28" ht="15">
-      <c r="A34" s="118" t="s">
+      <c r="A34" s="124" t="s">
         <v>142</v>
       </c>
-      <c r="B34" s="118"/>
-      <c r="C34" s="118"/>
-      <c r="D34" s="118"/>
-      <c r="E34" s="118"/>
-      <c r="F34" s="118"/>
-      <c r="G34" s="118"/>
-      <c r="K34" s="119"/>
-      <c r="L34" s="120"/>
-      <c r="Q34" s="121" t="s">
+      <c r="B34" s="124"/>
+      <c r="C34" s="124"/>
+      <c r="D34" s="124"/>
+      <c r="E34" s="124"/>
+      <c r="F34" s="124"/>
+      <c r="G34" s="124"/>
+      <c r="K34" s="125"/>
+      <c r="L34" s="126"/>
+      <c r="Q34" s="127" t="s">
         <v>143</v>
       </c>
-      <c r="R34" s="121"/>
-      <c r="S34" s="121"/>
-      <c r="T34" s="112"/>
-      <c r="U34" s="39"/>
-      <c r="V34" s="39"/>
-      <c r="W34" s="39"/>
-      <c r="X34" s="39"/>
-      <c r="Y34" s="39"/>
-      <c r="AB34" s="42" t="s">
+      <c r="R34" s="127"/>
+      <c r="S34" s="127"/>
+      <c r="T34" s="109"/>
+      <c r="U34" s="37"/>
+      <c r="V34" s="37"/>
+      <c r="W34" s="37"/>
+      <c r="X34" s="37"/>
+      <c r="Y34" s="37"/>
+      <c r="AB34" s="40" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="35" spans="1:28" ht="15">
-      <c r="A35" s="122" t="s">
+      <c r="A35" s="128" t="s">
         <v>141</v>
       </c>
-      <c r="B35" s="122"/>
-      <c r="C35" s="122"/>
-      <c r="D35" s="122"/>
-      <c r="E35" s="122"/>
-      <c r="F35" s="122"/>
-      <c r="G35" s="122"/>
-      <c r="H35" s="43"/>
-      <c r="I35" s="43"/>
-      <c r="J35" s="43"/>
-      <c r="K35" s="123" t="s">
+      <c r="B35" s="128"/>
+      <c r="C35" s="128"/>
+      <c r="D35" s="128"/>
+      <c r="E35" s="128"/>
+      <c r="F35" s="128"/>
+      <c r="G35" s="128"/>
+      <c r="H35" s="41"/>
+      <c r="I35" s="41"/>
+      <c r="J35" s="41"/>
+      <c r="K35" s="129" t="s">
         <v>78</v>
       </c>
-      <c r="L35" s="123"/>
-      <c r="M35" s="44"/>
-      <c r="N35" s="44"/>
-      <c r="Q35" s="124" t="s">
+      <c r="L35" s="129"/>
+      <c r="M35" s="42"/>
+      <c r="N35" s="42"/>
+      <c r="Q35" s="130" t="s">
         <v>86</v>
       </c>
-      <c r="R35" s="124"/>
-      <c r="S35" s="124"/>
-      <c r="T35" s="113"/>
-      <c r="U35" s="42"/>
-      <c r="V35" s="42"/>
-      <c r="W35" s="42"/>
-      <c r="X35" s="42"/>
-      <c r="Y35" s="42"/>
-      <c r="AB35" s="42" t="s">
+      <c r="R35" s="130"/>
+      <c r="S35" s="130"/>
+      <c r="T35" s="110"/>
+      <c r="U35" s="40"/>
+      <c r="V35" s="40"/>
+      <c r="W35" s="40"/>
+      <c r="X35" s="40"/>
+      <c r="Y35" s="40"/>
+      <c r="AB35" s="40" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="36" spans="1:28" ht="15">
-      <c r="H36" s="44"/>
-      <c r="I36" s="44"/>
-      <c r="J36" s="44"/>
+      <c r="H36" s="42"/>
+      <c r="I36" s="42"/>
+      <c r="J36" s="42"/>
     </row>
     <row r="37" spans="1:28" ht="15">
-      <c r="O37" s="44"/>
+      <c r="O37" s="42"/>
     </row>
     <row r="38" spans="1:28" ht="15">
-      <c r="B38" s="44"/>
-      <c r="C38" s="44"/>
-      <c r="D38" s="46"/>
-      <c r="E38" s="46"/>
-      <c r="F38" s="46"/>
-      <c r="O38" s="44"/>
-      <c r="AA38" s="45"/>
+      <c r="B38" s="42"/>
+      <c r="C38" s="42"/>
+      <c r="D38" s="44"/>
+      <c r="E38" s="44"/>
+      <c r="F38" s="44"/>
+      <c r="O38" s="42"/>
+      <c r="AA38" s="43"/>
     </row>
     <row r="40" spans="1:28" ht="14.25">
-      <c r="D40" s="46"/>
-      <c r="E40" s="46"/>
-      <c r="F40" s="46"/>
+      <c r="D40" s="44"/>
+      <c r="E40" s="44"/>
+      <c r="F40" s="44"/>
     </row>
     <row r="41" spans="1:28" ht="14.25">
-      <c r="D41" s="46"/>
-      <c r="E41" s="46"/>
-      <c r="F41" s="46"/>
+      <c r="D41" s="44"/>
+      <c r="E41" s="44"/>
+      <c r="F41" s="44"/>
     </row>
     <row r="42" spans="1:28" ht="14.25">
-      <c r="B42" s="46"/>
-      <c r="C42" s="46"/>
-      <c r="D42" s="46"/>
-      <c r="E42" s="46"/>
-      <c r="F42" s="46"/>
-      <c r="G42" s="47"/>
-      <c r="H42" s="47"/>
-      <c r="I42" s="47"/>
-      <c r="J42" s="47"/>
-      <c r="K42" s="79"/>
-      <c r="L42" s="101"/>
-      <c r="M42" s="79"/>
-      <c r="N42" s="79"/>
-      <c r="O42" s="101"/>
-      <c r="P42" s="101"/>
-      <c r="Q42" s="49"/>
-      <c r="R42" s="50"/>
+      <c r="B42" s="44"/>
+      <c r="C42" s="44"/>
+      <c r="D42" s="44"/>
+      <c r="E42" s="44"/>
+      <c r="F42" s="44"/>
+      <c r="G42" s="45"/>
+      <c r="H42" s="45"/>
+      <c r="I42" s="45"/>
+      <c r="J42" s="45"/>
+      <c r="K42" s="76"/>
+      <c r="L42" s="98"/>
+      <c r="M42" s="76"/>
+      <c r="N42" s="76"/>
+      <c r="O42" s="98"/>
+      <c r="P42" s="98"/>
+      <c r="Q42" s="47"/>
+      <c r="R42" s="48"/>
     </row>
     <row r="43" spans="1:28" ht="14.25">
-      <c r="B43" s="46"/>
-      <c r="C43" s="46"/>
-      <c r="D43" s="46"/>
-      <c r="E43" s="46"/>
-      <c r="F43" s="46"/>
-      <c r="G43" s="47"/>
-      <c r="H43" s="47"/>
-      <c r="I43" s="47"/>
-      <c r="J43" s="47"/>
-      <c r="K43" s="79"/>
-      <c r="L43" s="101"/>
-      <c r="M43" s="79"/>
-      <c r="N43" s="79"/>
-      <c r="O43" s="101"/>
-      <c r="P43" s="101"/>
-      <c r="Q43" s="49"/>
-      <c r="R43" s="50"/>
+      <c r="B43" s="44"/>
+      <c r="C43" s="44"/>
+      <c r="D43" s="44"/>
+      <c r="E43" s="44"/>
+      <c r="F43" s="44"/>
+      <c r="G43" s="45"/>
+      <c r="H43" s="45"/>
+      <c r="I43" s="45"/>
+      <c r="J43" s="45"/>
+      <c r="K43" s="76"/>
+      <c r="L43" s="98"/>
+      <c r="M43" s="76"/>
+      <c r="N43" s="76"/>
+      <c r="O43" s="98"/>
+      <c r="P43" s="98"/>
+      <c r="Q43" s="47"/>
+      <c r="R43" s="48"/>
     </row>
     <row r="44" spans="1:28" ht="15">
-      <c r="B44" s="42"/>
-      <c r="C44" s="42"/>
-      <c r="D44" s="46"/>
-      <c r="E44" s="46"/>
-      <c r="F44" s="46"/>
-      <c r="G44" s="45"/>
-      <c r="H44" s="47"/>
-      <c r="I44" s="47"/>
-      <c r="J44" s="47"/>
-      <c r="K44" s="79"/>
-      <c r="L44" s="42"/>
-      <c r="M44" s="42"/>
-      <c r="N44" s="79"/>
-      <c r="O44" s="101"/>
-      <c r="P44" s="42"/>
-      <c r="Q44" s="45"/>
-      <c r="R44" s="50"/>
+      <c r="B44" s="40"/>
+      <c r="C44" s="40"/>
+      <c r="D44" s="44"/>
+      <c r="E44" s="44"/>
+      <c r="F44" s="44"/>
+      <c r="G44" s="43"/>
+      <c r="H44" s="45"/>
+      <c r="I44" s="45"/>
+      <c r="J44" s="45"/>
+      <c r="K44" s="76"/>
+      <c r="L44" s="40"/>
+      <c r="M44" s="40"/>
+      <c r="N44" s="76"/>
+      <c r="O44" s="98"/>
+      <c r="P44" s="40"/>
+      <c r="Q44" s="43"/>
+      <c r="R44" s="48"/>
     </row>
     <row r="45" spans="1:28" ht="15">
-      <c r="B45" s="42"/>
-      <c r="C45" s="42"/>
-      <c r="D45" s="42"/>
-      <c r="E45" s="42"/>
-      <c r="F45" s="42"/>
-      <c r="G45" s="45"/>
-      <c r="H45" s="47"/>
-      <c r="I45" s="47"/>
-      <c r="J45" s="47"/>
-      <c r="K45" s="79"/>
-      <c r="L45" s="42"/>
-      <c r="M45" s="42"/>
-      <c r="N45" s="79"/>
-      <c r="O45" s="101"/>
-      <c r="P45" s="42"/>
-      <c r="Q45" s="45"/>
-      <c r="R45" s="50"/>
+      <c r="B45" s="40"/>
+      <c r="C45" s="40"/>
+      <c r="D45" s="40"/>
+      <c r="E45" s="40"/>
+      <c r="F45" s="40"/>
+      <c r="G45" s="43"/>
+      <c r="H45" s="45"/>
+      <c r="I45" s="45"/>
+      <c r="J45" s="45"/>
+      <c r="K45" s="76"/>
+      <c r="L45" s="40"/>
+      <c r="M45" s="40"/>
+      <c r="N45" s="76"/>
+      <c r="O45" s="98"/>
+      <c r="P45" s="40"/>
+      <c r="Q45" s="43"/>
+      <c r="R45" s="48"/>
     </row>
     <row r="46" spans="1:28" ht="15">
-      <c r="B46" s="42"/>
-      <c r="C46" s="42"/>
-      <c r="D46" s="46"/>
-      <c r="E46" s="46"/>
-      <c r="F46" s="46"/>
-      <c r="G46" s="45"/>
-      <c r="H46" s="47"/>
-      <c r="I46" s="47"/>
-      <c r="J46" s="47"/>
-      <c r="K46" s="79"/>
-      <c r="L46" s="42"/>
-      <c r="M46" s="42"/>
-      <c r="N46" s="79"/>
-      <c r="O46" s="101"/>
-      <c r="P46" s="42"/>
-      <c r="Q46" s="45"/>
-      <c r="R46" s="50"/>
+      <c r="B46" s="40"/>
+      <c r="C46" s="40"/>
+      <c r="D46" s="44"/>
+      <c r="E46" s="44"/>
+      <c r="F46" s="44"/>
+      <c r="G46" s="43"/>
+      <c r="H46" s="45"/>
+      <c r="I46" s="45"/>
+      <c r="J46" s="45"/>
+      <c r="K46" s="76"/>
+      <c r="L46" s="40"/>
+      <c r="M46" s="40"/>
+      <c r="N46" s="76"/>
+      <c r="O46" s="98"/>
+      <c r="P46" s="40"/>
+      <c r="Q46" s="43"/>
+      <c r="R46" s="48"/>
     </row>
     <row r="47" spans="1:28" ht="14.25">
-      <c r="B47" s="46"/>
-      <c r="C47" s="46"/>
-      <c r="D47" s="46"/>
-      <c r="E47" s="46"/>
-      <c r="F47" s="46"/>
-      <c r="G47" s="47"/>
-      <c r="H47" s="47"/>
-      <c r="I47" s="47"/>
-      <c r="J47" s="47"/>
-      <c r="K47" s="79"/>
-      <c r="L47" s="101"/>
-      <c r="M47" s="79"/>
-      <c r="N47" s="79"/>
-      <c r="O47" s="101"/>
-      <c r="P47" s="101"/>
-      <c r="Q47" s="49"/>
-      <c r="R47" s="50"/>
+      <c r="B47" s="44"/>
+      <c r="C47" s="44"/>
+      <c r="D47" s="44"/>
+      <c r="E47" s="44"/>
+      <c r="F47" s="44"/>
+      <c r="G47" s="45"/>
+      <c r="H47" s="45"/>
+      <c r="I47" s="45"/>
+      <c r="J47" s="45"/>
+      <c r="K47" s="76"/>
+      <c r="L47" s="98"/>
+      <c r="M47" s="76"/>
+      <c r="N47" s="76"/>
+      <c r="O47" s="98"/>
+      <c r="P47" s="98"/>
+      <c r="Q47" s="47"/>
+      <c r="R47" s="48"/>
     </row>
     <row r="48" spans="1:28" ht="15">
-      <c r="B48" s="42"/>
-      <c r="C48" s="42"/>
-      <c r="D48" s="46"/>
-      <c r="E48" s="46"/>
-      <c r="F48" s="46"/>
-      <c r="G48" s="45"/>
-      <c r="H48" s="47"/>
-      <c r="I48" s="47"/>
-      <c r="J48" s="47"/>
-      <c r="K48" s="79"/>
-      <c r="L48" s="101"/>
-      <c r="M48" s="79"/>
-      <c r="N48" s="79"/>
-      <c r="O48" s="101"/>
-      <c r="P48" s="42"/>
-      <c r="Q48" s="45"/>
-      <c r="R48" s="50"/>
+      <c r="B48" s="40"/>
+      <c r="C48" s="40"/>
+      <c r="D48" s="44"/>
+      <c r="E48" s="44"/>
+      <c r="F48" s="44"/>
+      <c r="G48" s="43"/>
+      <c r="H48" s="45"/>
+      <c r="I48" s="45"/>
+      <c r="J48" s="45"/>
+      <c r="K48" s="76"/>
+      <c r="L48" s="98"/>
+      <c r="M48" s="76"/>
+      <c r="N48" s="76"/>
+      <c r="O48" s="98"/>
+      <c r="P48" s="40"/>
+      <c r="Q48" s="43"/>
+      <c r="R48" s="48"/>
     </row>
     <row r="49" spans="2:28" ht="15">
-      <c r="B49" s="42"/>
-      <c r="C49" s="42"/>
-      <c r="D49" s="46"/>
-      <c r="E49" s="46"/>
-      <c r="F49" s="46"/>
-      <c r="G49" s="45"/>
-      <c r="H49" s="47"/>
-      <c r="I49" s="47"/>
-      <c r="J49" s="47"/>
-      <c r="K49" s="79"/>
-      <c r="L49" s="101"/>
-      <c r="M49" s="79"/>
-      <c r="N49" s="79"/>
-      <c r="O49" s="101"/>
-      <c r="P49" s="42"/>
-      <c r="Q49" s="49"/>
-      <c r="R49" s="50"/>
+      <c r="B49" s="40"/>
+      <c r="C49" s="40"/>
+      <c r="D49" s="44"/>
+      <c r="E49" s="44"/>
+      <c r="F49" s="44"/>
+      <c r="G49" s="43"/>
+      <c r="H49" s="45"/>
+      <c r="I49" s="45"/>
+      <c r="J49" s="45"/>
+      <c r="K49" s="76"/>
+      <c r="L49" s="98"/>
+      <c r="M49" s="76"/>
+      <c r="N49" s="76"/>
+      <c r="O49" s="98"/>
+      <c r="P49" s="40"/>
+      <c r="Q49" s="47"/>
+      <c r="R49" s="48"/>
     </row>
     <row r="50" spans="2:28" ht="14.25">
-      <c r="B50" s="115"/>
-      <c r="C50" s="115"/>
-      <c r="D50" s="115"/>
-      <c r="E50" s="115"/>
-      <c r="F50" s="115"/>
-      <c r="G50" s="116"/>
-      <c r="H50" s="47"/>
-      <c r="I50" s="47"/>
-      <c r="J50" s="47"/>
-      <c r="K50" s="79"/>
-      <c r="L50" s="101"/>
-      <c r="M50" s="79"/>
-      <c r="N50" s="79"/>
-      <c r="O50" s="101"/>
-      <c r="P50" s="101"/>
-      <c r="Q50" s="49"/>
-      <c r="R50" s="50"/>
+      <c r="B50" s="121"/>
+      <c r="C50" s="121"/>
+      <c r="D50" s="121"/>
+      <c r="E50" s="121"/>
+      <c r="F50" s="121"/>
+      <c r="G50" s="122"/>
+      <c r="H50" s="45"/>
+      <c r="I50" s="45"/>
+      <c r="J50" s="45"/>
+      <c r="K50" s="76"/>
+      <c r="L50" s="98"/>
+      <c r="M50" s="76"/>
+      <c r="N50" s="76"/>
+      <c r="O50" s="98"/>
+      <c r="P50" s="98"/>
+      <c r="Q50" s="47"/>
+      <c r="R50" s="48"/>
     </row>
     <row r="51" spans="2:28" ht="15">
-      <c r="B51" s="51"/>
-      <c r="C51" s="51"/>
-      <c r="D51" s="46"/>
-      <c r="E51" s="46"/>
-      <c r="F51" s="46"/>
-      <c r="G51" s="52"/>
-      <c r="H51" s="47"/>
-      <c r="I51" s="47"/>
-      <c r="J51" s="47"/>
-      <c r="K51" s="79"/>
-      <c r="L51" s="101"/>
-      <c r="M51" s="79"/>
-      <c r="N51" s="79"/>
-      <c r="O51" s="101"/>
-      <c r="P51" s="101"/>
-      <c r="Q51" s="49"/>
-      <c r="R51" s="50"/>
+      <c r="B51" s="49"/>
+      <c r="C51" s="49"/>
+      <c r="D51" s="44"/>
+      <c r="E51" s="44"/>
+      <c r="F51" s="44"/>
+      <c r="G51" s="50"/>
+      <c r="H51" s="45"/>
+      <c r="I51" s="45"/>
+      <c r="J51" s="45"/>
+      <c r="K51" s="76"/>
+      <c r="L51" s="98"/>
+      <c r="M51" s="76"/>
+      <c r="N51" s="76"/>
+      <c r="O51" s="98"/>
+      <c r="P51" s="98"/>
+      <c r="Q51" s="47"/>
+      <c r="R51" s="48"/>
     </row>
     <row r="52" spans="2:28" ht="14.25">
-      <c r="B52" s="46"/>
-      <c r="C52" s="46"/>
-      <c r="D52" s="46"/>
-      <c r="E52" s="46"/>
-      <c r="F52" s="46"/>
-      <c r="G52" s="47"/>
-      <c r="H52" s="47"/>
-      <c r="I52" s="47"/>
-      <c r="J52" s="47"/>
-      <c r="K52" s="79"/>
-      <c r="L52" s="101"/>
-      <c r="M52" s="79"/>
-      <c r="N52" s="79"/>
-      <c r="O52" s="101"/>
-      <c r="P52" s="101"/>
-      <c r="Q52" s="49"/>
-      <c r="R52" s="50"/>
+      <c r="B52" s="44"/>
+      <c r="C52" s="44"/>
+      <c r="D52" s="44"/>
+      <c r="E52" s="44"/>
+      <c r="F52" s="44"/>
+      <c r="G52" s="45"/>
+      <c r="H52" s="45"/>
+      <c r="I52" s="45"/>
+      <c r="J52" s="45"/>
+      <c r="K52" s="76"/>
+      <c r="L52" s="98"/>
+      <c r="M52" s="76"/>
+      <c r="N52" s="76"/>
+      <c r="O52" s="98"/>
+      <c r="P52" s="98"/>
+      <c r="Q52" s="47"/>
+      <c r="R52" s="48"/>
     </row>
     <row r="53" spans="2:28" ht="14.25">
-      <c r="B53" s="46"/>
-      <c r="C53" s="46"/>
-      <c r="D53" s="46"/>
-      <c r="E53" s="46"/>
-      <c r="F53" s="46"/>
-      <c r="G53" s="47"/>
-      <c r="H53" s="47"/>
-      <c r="I53" s="47"/>
-      <c r="J53" s="47"/>
-      <c r="K53" s="79"/>
-      <c r="L53" s="101"/>
-      <c r="M53" s="79"/>
-      <c r="N53" s="79"/>
-      <c r="O53" s="101"/>
-      <c r="P53" s="101"/>
-      <c r="Q53" s="49"/>
-      <c r="R53" s="50"/>
+      <c r="B53" s="44"/>
+      <c r="C53" s="44"/>
+      <c r="D53" s="44"/>
+      <c r="E53" s="44"/>
+      <c r="F53" s="44"/>
+      <c r="G53" s="45"/>
+      <c r="H53" s="45"/>
+      <c r="I53" s="45"/>
+      <c r="J53" s="45"/>
+      <c r="K53" s="76"/>
+      <c r="L53" s="98"/>
+      <c r="M53" s="76"/>
+      <c r="N53" s="76"/>
+      <c r="O53" s="98"/>
+      <c r="P53" s="98"/>
+      <c r="Q53" s="47"/>
+      <c r="R53" s="48"/>
     </row>
     <row r="54" spans="2:28" ht="15">
-      <c r="B54" s="42"/>
-      <c r="C54" s="42"/>
-      <c r="D54" s="46"/>
-      <c r="E54" s="46"/>
-      <c r="F54" s="46"/>
-      <c r="G54" s="45"/>
-      <c r="H54" s="47"/>
-      <c r="I54" s="47"/>
-      <c r="J54" s="47"/>
-      <c r="K54" s="79"/>
-      <c r="L54" s="101"/>
-      <c r="M54" s="79"/>
-      <c r="N54" s="79"/>
-      <c r="O54" s="101"/>
-      <c r="P54" s="42"/>
-      <c r="Q54" s="45"/>
-      <c r="R54" s="50"/>
+      <c r="B54" s="40"/>
+      <c r="C54" s="40"/>
+      <c r="D54" s="44"/>
+      <c r="E54" s="44"/>
+      <c r="F54" s="44"/>
+      <c r="G54" s="43"/>
+      <c r="H54" s="45"/>
+      <c r="I54" s="45"/>
+      <c r="J54" s="45"/>
+      <c r="K54" s="76"/>
+      <c r="L54" s="98"/>
+      <c r="M54" s="76"/>
+      <c r="N54" s="76"/>
+      <c r="O54" s="98"/>
+      <c r="P54" s="40"/>
+      <c r="Q54" s="43"/>
+      <c r="R54" s="48"/>
     </row>
     <row r="55" spans="2:28" ht="14.25">
-      <c r="B55" s="46"/>
-      <c r="C55" s="46"/>
-      <c r="D55" s="46"/>
-      <c r="E55" s="46"/>
-      <c r="F55" s="46"/>
-      <c r="G55" s="47"/>
-      <c r="H55" s="47"/>
-      <c r="I55" s="47"/>
-      <c r="J55" s="47"/>
-      <c r="K55" s="79"/>
-      <c r="L55" s="101"/>
-      <c r="M55" s="79"/>
-      <c r="N55" s="79"/>
-      <c r="O55" s="101"/>
-      <c r="P55" s="101"/>
-      <c r="Q55" s="49"/>
-      <c r="R55" s="50"/>
+      <c r="B55" s="44"/>
+      <c r="C55" s="44"/>
+      <c r="D55" s="44"/>
+      <c r="E55" s="44"/>
+      <c r="F55" s="44"/>
+      <c r="G55" s="45"/>
+      <c r="H55" s="45"/>
+      <c r="I55" s="45"/>
+      <c r="J55" s="45"/>
+      <c r="K55" s="76"/>
+      <c r="L55" s="98"/>
+      <c r="M55" s="76"/>
+      <c r="N55" s="76"/>
+      <c r="O55" s="98"/>
+      <c r="P55" s="98"/>
+      <c r="Q55" s="47"/>
+      <c r="R55" s="48"/>
     </row>
     <row r="56" spans="2:28" ht="15">
-      <c r="B56" s="42"/>
-      <c r="C56" s="42"/>
-      <c r="D56" s="46"/>
-      <c r="E56" s="46"/>
-      <c r="F56" s="46"/>
-      <c r="G56" s="45"/>
-      <c r="H56" s="47"/>
-      <c r="I56" s="47"/>
-      <c r="J56" s="47"/>
-      <c r="K56" s="79"/>
-      <c r="L56" s="101"/>
-      <c r="M56" s="79"/>
-      <c r="N56" s="79"/>
-      <c r="O56" s="101"/>
-      <c r="P56" s="42"/>
-      <c r="Q56" s="45"/>
-      <c r="R56" s="50"/>
+      <c r="B56" s="40"/>
+      <c r="C56" s="40"/>
+      <c r="D56" s="44"/>
+      <c r="E56" s="44"/>
+      <c r="F56" s="44"/>
+      <c r="G56" s="43"/>
+      <c r="H56" s="45"/>
+      <c r="I56" s="45"/>
+      <c r="J56" s="45"/>
+      <c r="K56" s="76"/>
+      <c r="L56" s="98"/>
+      <c r="M56" s="76"/>
+      <c r="N56" s="76"/>
+      <c r="O56" s="98"/>
+      <c r="P56" s="40"/>
+      <c r="Q56" s="43"/>
+      <c r="R56" s="48"/>
     </row>
     <row r="57" spans="2:28" ht="15">
-      <c r="B57" s="42"/>
-      <c r="C57" s="42"/>
-      <c r="D57" s="46"/>
-      <c r="E57" s="46"/>
-      <c r="F57" s="46"/>
-      <c r="G57" s="45"/>
-      <c r="H57" s="47"/>
-      <c r="I57" s="47"/>
-      <c r="J57" s="47"/>
-      <c r="K57" s="79"/>
-      <c r="L57" s="101"/>
-      <c r="M57" s="79"/>
-      <c r="N57" s="79"/>
-      <c r="O57" s="101"/>
-      <c r="P57" s="42"/>
-      <c r="Q57" s="45"/>
-      <c r="R57" s="50"/>
+      <c r="B57" s="40"/>
+      <c r="C57" s="40"/>
+      <c r="D57" s="44"/>
+      <c r="E57" s="44"/>
+      <c r="F57" s="44"/>
+      <c r="G57" s="43"/>
+      <c r="H57" s="45"/>
+      <c r="I57" s="45"/>
+      <c r="J57" s="45"/>
+      <c r="K57" s="76"/>
+      <c r="L57" s="98"/>
+      <c r="M57" s="76"/>
+      <c r="N57" s="76"/>
+      <c r="O57" s="98"/>
+      <c r="P57" s="40"/>
+      <c r="Q57" s="43"/>
+      <c r="R57" s="48"/>
     </row>
     <row r="58" spans="2:28" ht="15">
-      <c r="B58" s="42"/>
-      <c r="C58" s="42"/>
-      <c r="D58" s="42"/>
-      <c r="E58" s="42"/>
-      <c r="F58" s="42"/>
-      <c r="G58" s="45"/>
-      <c r="H58" s="47"/>
-      <c r="I58" s="47"/>
-      <c r="J58" s="47"/>
-      <c r="K58" s="79"/>
-      <c r="L58" s="101"/>
-      <c r="M58" s="79"/>
-      <c r="N58" s="79"/>
-      <c r="O58" s="101"/>
-      <c r="P58" s="42"/>
-      <c r="Q58" s="45"/>
-      <c r="R58" s="50"/>
+      <c r="B58" s="40"/>
+      <c r="C58" s="40"/>
+      <c r="D58" s="40"/>
+      <c r="E58" s="40"/>
+      <c r="F58" s="40"/>
+      <c r="G58" s="43"/>
+      <c r="H58" s="45"/>
+      <c r="I58" s="45"/>
+      <c r="J58" s="45"/>
+      <c r="K58" s="76"/>
+      <c r="L58" s="98"/>
+      <c r="M58" s="76"/>
+      <c r="N58" s="76"/>
+      <c r="O58" s="98"/>
+      <c r="P58" s="40"/>
+      <c r="Q58" s="43"/>
+      <c r="R58" s="48"/>
     </row>
     <row r="59" spans="2:28" ht="14.25">
-      <c r="B59" s="115"/>
-      <c r="C59" s="115"/>
-      <c r="D59" s="115"/>
-      <c r="E59" s="115"/>
-      <c r="F59" s="115"/>
-      <c r="G59" s="116"/>
-      <c r="H59" s="47"/>
-      <c r="I59" s="47"/>
-      <c r="J59" s="47"/>
-      <c r="K59" s="79"/>
-      <c r="L59" s="101"/>
-      <c r="M59" s="79"/>
-      <c r="N59" s="79"/>
-      <c r="O59" s="101"/>
-      <c r="P59" s="101"/>
-      <c r="Q59" s="49"/>
-      <c r="R59" s="50"/>
+      <c r="B59" s="121"/>
+      <c r="C59" s="121"/>
+      <c r="D59" s="121"/>
+      <c r="E59" s="121"/>
+      <c r="F59" s="121"/>
+      <c r="G59" s="122"/>
+      <c r="H59" s="45"/>
+      <c r="I59" s="45"/>
+      <c r="J59" s="45"/>
+      <c r="K59" s="76"/>
+      <c r="L59" s="98"/>
+      <c r="M59" s="76"/>
+      <c r="N59" s="76"/>
+      <c r="O59" s="98"/>
+      <c r="P59" s="98"/>
+      <c r="Q59" s="47"/>
+      <c r="R59" s="48"/>
     </row>
     <row r="60" spans="2:28" ht="15">
-      <c r="B60" s="42"/>
-      <c r="C60" s="42"/>
-      <c r="D60" s="46"/>
-      <c r="E60" s="46"/>
-      <c r="F60" s="46"/>
-      <c r="G60" s="45"/>
-      <c r="H60" s="47"/>
-      <c r="I60" s="47"/>
-      <c r="J60" s="47"/>
-      <c r="K60" s="79"/>
-      <c r="L60" s="101"/>
-      <c r="M60" s="79"/>
-      <c r="N60" s="79"/>
-      <c r="O60" s="101"/>
-      <c r="P60" s="42"/>
-      <c r="Q60" s="45"/>
-      <c r="R60" s="50"/>
+      <c r="B60" s="40"/>
+      <c r="C60" s="40"/>
+      <c r="D60" s="44"/>
+      <c r="E60" s="44"/>
+      <c r="F60" s="44"/>
+      <c r="G60" s="43"/>
+      <c r="H60" s="45"/>
+      <c r="I60" s="45"/>
+      <c r="J60" s="45"/>
+      <c r="K60" s="76"/>
+      <c r="L60" s="98"/>
+      <c r="M60" s="76"/>
+      <c r="N60" s="76"/>
+      <c r="O60" s="98"/>
+      <c r="P60" s="40"/>
+      <c r="Q60" s="43"/>
+      <c r="R60" s="48"/>
     </row>
     <row r="61" spans="2:28">
       <c r="G61" s="1"/>
@@ -4723,42 +4724,42 @@
       <c r="AB68" s="1"/>
     </row>
     <row r="69" spans="2:28" ht="14.25">
-      <c r="B69" s="46"/>
-      <c r="C69" s="46"/>
-      <c r="D69" s="46"/>
-      <c r="E69" s="46"/>
-      <c r="F69" s="46"/>
-      <c r="G69" s="47"/>
-      <c r="H69" s="47"/>
-      <c r="I69" s="47"/>
-      <c r="J69" s="47"/>
-      <c r="K69" s="79"/>
-      <c r="L69" s="101"/>
-      <c r="M69" s="79"/>
-      <c r="N69" s="79"/>
-      <c r="O69" s="101"/>
-      <c r="P69" s="101"/>
-      <c r="Q69" s="49"/>
-      <c r="R69" s="50"/>
+      <c r="B69" s="44"/>
+      <c r="C69" s="44"/>
+      <c r="D69" s="44"/>
+      <c r="E69" s="44"/>
+      <c r="F69" s="44"/>
+      <c r="G69" s="45"/>
+      <c r="H69" s="45"/>
+      <c r="I69" s="45"/>
+      <c r="J69" s="45"/>
+      <c r="K69" s="76"/>
+      <c r="L69" s="98"/>
+      <c r="M69" s="76"/>
+      <c r="N69" s="76"/>
+      <c r="O69" s="98"/>
+      <c r="P69" s="98"/>
+      <c r="Q69" s="47"/>
+      <c r="R69" s="48"/>
     </row>
     <row r="70" spans="2:28" ht="15">
-      <c r="B70" s="53"/>
-      <c r="C70" s="53"/>
-      <c r="D70" s="53"/>
-      <c r="E70" s="53"/>
-      <c r="F70" s="53"/>
-      <c r="G70" s="52"/>
-      <c r="H70" s="47"/>
-      <c r="I70" s="47"/>
-      <c r="J70" s="47"/>
-      <c r="K70" s="80"/>
-      <c r="L70" s="101"/>
-      <c r="M70" s="79"/>
-      <c r="N70" s="80"/>
-      <c r="O70" s="101"/>
-      <c r="P70" s="101"/>
-      <c r="Q70" s="49"/>
-      <c r="R70" s="49"/>
+      <c r="B70" s="51"/>
+      <c r="C70" s="51"/>
+      <c r="D70" s="51"/>
+      <c r="E70" s="51"/>
+      <c r="F70" s="51"/>
+      <c r="G70" s="50"/>
+      <c r="H70" s="45"/>
+      <c r="I70" s="45"/>
+      <c r="J70" s="45"/>
+      <c r="K70" s="77"/>
+      <c r="L70" s="98"/>
+      <c r="M70" s="76"/>
+      <c r="N70" s="77"/>
+      <c r="O70" s="98"/>
+      <c r="P70" s="98"/>
+      <c r="Q70" s="47"/>
+      <c r="R70" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="16">
@@ -4841,70 +4842,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:40" ht="15">
-      <c r="A1" s="125" t="s">
+      <c r="A1" s="131" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="125"/>
-      <c r="C1" s="125"/>
-      <c r="D1" s="125"/>
-      <c r="E1" s="125"/>
-      <c r="F1" s="125"/>
-      <c r="G1" s="125"/>
-      <c r="H1" s="125"/>
-      <c r="I1" s="125"/>
-      <c r="J1" s="125"/>
-      <c r="K1" s="125"/>
-      <c r="L1" s="125"/>
-      <c r="M1" s="125"/>
-      <c r="N1" s="125"/>
-      <c r="O1" s="125"/>
-      <c r="P1" s="125"/>
-      <c r="Q1" s="125"/>
-      <c r="R1" s="125"/>
+      <c r="B1" s="131"/>
+      <c r="C1" s="131"/>
+      <c r="D1" s="131"/>
+      <c r="E1" s="131"/>
+      <c r="F1" s="131"/>
+      <c r="G1" s="131"/>
+      <c r="H1" s="131"/>
+      <c r="I1" s="131"/>
+      <c r="J1" s="131"/>
+      <c r="K1" s="131"/>
+      <c r="L1" s="131"/>
+      <c r="M1" s="131"/>
+      <c r="N1" s="131"/>
+      <c r="O1" s="131"/>
+      <c r="P1" s="131"/>
+      <c r="Q1" s="131"/>
+      <c r="R1" s="131"/>
     </row>
     <row r="2" spans="1:40" ht="15">
-      <c r="A2" s="125" t="s">
+      <c r="A2" s="131" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="125"/>
-      <c r="C2" s="125"/>
-      <c r="D2" s="125"/>
-      <c r="E2" s="125"/>
-      <c r="F2" s="125"/>
-      <c r="G2" s="125"/>
-      <c r="H2" s="125"/>
-      <c r="I2" s="125"/>
-      <c r="J2" s="125"/>
-      <c r="K2" s="125"/>
-      <c r="L2" s="125"/>
-      <c r="M2" s="125"/>
-      <c r="N2" s="125"/>
-      <c r="O2" s="125"/>
-      <c r="P2" s="125"/>
-      <c r="Q2" s="125"/>
-      <c r="R2" s="125"/>
+      <c r="B2" s="131"/>
+      <c r="C2" s="131"/>
+      <c r="D2" s="131"/>
+      <c r="E2" s="131"/>
+      <c r="F2" s="131"/>
+      <c r="G2" s="131"/>
+      <c r="H2" s="131"/>
+      <c r="I2" s="131"/>
+      <c r="J2" s="131"/>
+      <c r="K2" s="131"/>
+      <c r="L2" s="131"/>
+      <c r="M2" s="131"/>
+      <c r="N2" s="131"/>
+      <c r="O2" s="131"/>
+      <c r="P2" s="131"/>
+      <c r="Q2" s="131"/>
+      <c r="R2" s="131"/>
     </row>
     <row r="3" spans="1:40" ht="14.25">
-      <c r="A3" s="126" t="s">
+      <c r="A3" s="132" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="126"/>
-      <c r="C3" s="126"/>
-      <c r="D3" s="126"/>
-      <c r="E3" s="126"/>
-      <c r="F3" s="126"/>
-      <c r="G3" s="126"/>
-      <c r="H3" s="126"/>
-      <c r="I3" s="126"/>
-      <c r="J3" s="126"/>
-      <c r="K3" s="126"/>
-      <c r="L3" s="126"/>
-      <c r="M3" s="126"/>
-      <c r="N3" s="126"/>
-      <c r="O3" s="126"/>
-      <c r="P3" s="126"/>
-      <c r="Q3" s="126"/>
-      <c r="R3" s="126"/>
+      <c r="B3" s="132"/>
+      <c r="C3" s="132"/>
+      <c r="D3" s="132"/>
+      <c r="E3" s="132"/>
+      <c r="F3" s="132"/>
+      <c r="G3" s="132"/>
+      <c r="H3" s="132"/>
+      <c r="I3" s="132"/>
+      <c r="J3" s="132"/>
+      <c r="K3" s="132"/>
+      <c r="L3" s="132"/>
+      <c r="M3" s="132"/>
+      <c r="N3" s="132"/>
+      <c r="O3" s="132"/>
+      <c r="P3" s="132"/>
+      <c r="Q3" s="132"/>
+      <c r="R3" s="132"/>
     </row>
     <row r="4" spans="1:40">
       <c r="A4" s="2"/>
@@ -4917,37 +4918,37 @@
       <c r="L4" s="2"/>
     </row>
     <row r="5" spans="1:40" ht="15">
-      <c r="A5" s="125" t="s">
+      <c r="A5" s="131" t="s">
         <v>129</v>
       </c>
-      <c r="B5" s="125"/>
-      <c r="C5" s="125"/>
-      <c r="D5" s="125"/>
-      <c r="E5" s="125"/>
-      <c r="F5" s="125"/>
-      <c r="G5" s="125"/>
-      <c r="H5" s="125"/>
-      <c r="I5" s="125"/>
-      <c r="J5" s="125"/>
-      <c r="K5" s="125"/>
-      <c r="L5" s="125"/>
-      <c r="M5" s="125"/>
-      <c r="N5" s="125"/>
-      <c r="O5" s="125"/>
-      <c r="P5" s="125"/>
-      <c r="Q5" s="125"/>
-      <c r="R5" s="125"/>
+      <c r="B5" s="131"/>
+      <c r="C5" s="131"/>
+      <c r="D5" s="131"/>
+      <c r="E5" s="131"/>
+      <c r="F5" s="131"/>
+      <c r="G5" s="131"/>
+      <c r="H5" s="131"/>
+      <c r="I5" s="131"/>
+      <c r="J5" s="131"/>
+      <c r="K5" s="131"/>
+      <c r="L5" s="131"/>
+      <c r="M5" s="131"/>
+      <c r="N5" s="131"/>
+      <c r="O5" s="131"/>
+      <c r="P5" s="131"/>
+      <c r="Q5" s="131"/>
+      <c r="R5" s="131"/>
     </row>
     <row r="7" spans="1:40" ht="15">
-      <c r="A7" s="135" t="s">
+      <c r="A7" s="141" t="s">
         <v>89</v>
       </c>
-      <c r="B7" s="136"/>
-      <c r="C7" s="136"/>
-      <c r="D7" s="136"/>
-      <c r="E7" s="136"/>
-      <c r="F7" s="136"/>
-      <c r="G7" s="136"/>
+      <c r="B7" s="142"/>
+      <c r="C7" s="142"/>
+      <c r="D7" s="142"/>
+      <c r="E7" s="142"/>
+      <c r="F7" s="142"/>
+      <c r="G7" s="142"/>
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
       <c r="J7" s="7"/>
@@ -4987,22 +4988,22 @@
       <c r="B9" s="14"/>
       <c r="C9" s="14"/>
       <c r="D9" s="15"/>
-      <c r="E9" s="127" t="s">
+      <c r="E9" s="133" t="s">
         <v>5</v>
       </c>
-      <c r="F9" s="128"/>
-      <c r="G9" s="129"/>
+      <c r="F9" s="134"/>
+      <c r="G9" s="135"/>
       <c r="H9" s="14"/>
-      <c r="I9" s="130" t="s">
+      <c r="I9" s="136" t="s">
         <v>6</v>
       </c>
-      <c r="J9" s="131"/>
+      <c r="J9" s="137"/>
       <c r="K9" s="14"/>
-      <c r="L9" s="132" t="s">
+      <c r="L9" s="138" t="s">
         <v>7</v>
       </c>
-      <c r="M9" s="133"/>
-      <c r="N9" s="134"/>
+      <c r="M9" s="139"/>
+      <c r="N9" s="140"/>
       <c r="O9" s="15"/>
       <c r="P9" s="15"/>
       <c r="Q9" s="16"/>
@@ -5127,34 +5128,34 @@
         <v>34</v>
       </c>
       <c r="R12" s="19"/>
-      <c r="S12" s="148" t="s">
+      <c r="S12" s="154" t="s">
         <v>35</v>
       </c>
-      <c r="T12" s="148"/>
-      <c r="U12" s="148"/>
-      <c r="V12" s="148"/>
-      <c r="W12" s="148"/>
-      <c r="X12" s="148"/>
-      <c r="Y12" s="148"/>
-      <c r="Z12" s="148"/>
-      <c r="AA12" s="148"/>
-      <c r="AB12" s="148"/>
-      <c r="AC12" s="147" t="s">
+      <c r="T12" s="154"/>
+      <c r="U12" s="154"/>
+      <c r="V12" s="154"/>
+      <c r="W12" s="154"/>
+      <c r="X12" s="154"/>
+      <c r="Y12" s="154"/>
+      <c r="Z12" s="154"/>
+      <c r="AA12" s="154"/>
+      <c r="AB12" s="154"/>
+      <c r="AC12" s="153" t="s">
         <v>36</v>
       </c>
-      <c r="AD12" s="147"/>
-      <c r="AE12" s="147"/>
-      <c r="AF12" s="147"/>
-      <c r="AG12" s="147"/>
-      <c r="AH12" s="147"/>
-      <c r="AI12" s="147"/>
-      <c r="AJ12" s="147"/>
-      <c r="AK12" s="147"/>
-      <c r="AL12" s="147"/>
-      <c r="AM12" s="138" t="s">
+      <c r="AD12" s="153"/>
+      <c r="AE12" s="153"/>
+      <c r="AF12" s="153"/>
+      <c r="AG12" s="153"/>
+      <c r="AH12" s="153"/>
+      <c r="AI12" s="153"/>
+      <c r="AJ12" s="153"/>
+      <c r="AK12" s="153"/>
+      <c r="AL12" s="153"/>
+      <c r="AM12" s="144" t="s">
         <v>130</v>
       </c>
-      <c r="AN12" s="138"/>
+      <c r="AN12" s="144"/>
     </row>
     <row r="13" spans="1:40" ht="15">
       <c r="A13" s="18"/>
@@ -5185,44 +5186,44 @@
       </c>
       <c r="Q13" s="19"/>
       <c r="R13" s="19"/>
-      <c r="S13" s="141" t="s">
+      <c r="S13" s="147" t="s">
         <v>38</v>
       </c>
-      <c r="T13" s="141"/>
-      <c r="U13" s="141"/>
-      <c r="V13" s="145" t="s">
+      <c r="T13" s="147"/>
+      <c r="U13" s="147"/>
+      <c r="V13" s="151" t="s">
         <v>39</v>
       </c>
-      <c r="W13" s="145"/>
-      <c r="X13" s="145"/>
-      <c r="Y13" s="146" t="s">
+      <c r="W13" s="151"/>
+      <c r="X13" s="151"/>
+      <c r="Y13" s="152" t="s">
         <v>40</v>
       </c>
-      <c r="Z13" s="146"/>
-      <c r="AA13" s="146"/>
-      <c r="AB13" s="139" t="s">
+      <c r="Z13" s="152"/>
+      <c r="AA13" s="152"/>
+      <c r="AB13" s="145" t="s">
         <v>41</v>
       </c>
-      <c r="AC13" s="142" t="s">
+      <c r="AC13" s="148" t="s">
         <v>38</v>
       </c>
-      <c r="AD13" s="142"/>
-      <c r="AE13" s="142"/>
-      <c r="AF13" s="143" t="s">
+      <c r="AD13" s="148"/>
+      <c r="AE13" s="148"/>
+      <c r="AF13" s="149" t="s">
         <v>39</v>
       </c>
-      <c r="AG13" s="143"/>
-      <c r="AH13" s="143"/>
-      <c r="AI13" s="144" t="s">
+      <c r="AG13" s="149"/>
+      <c r="AH13" s="149"/>
+      <c r="AI13" s="150" t="s">
         <v>40</v>
       </c>
-      <c r="AJ13" s="144"/>
-      <c r="AK13" s="144"/>
-      <c r="AL13" s="140" t="s">
+      <c r="AJ13" s="150"/>
+      <c r="AK13" s="150"/>
+      <c r="AL13" s="146" t="s">
         <v>41</v>
       </c>
-      <c r="AM13" s="138"/>
-      <c r="AN13" s="138"/>
+      <c r="AM13" s="144"/>
+      <c r="AN13" s="144"/>
     </row>
     <row r="14" spans="1:40" ht="15">
       <c r="A14" s="26" t="s">
@@ -5302,7 +5303,7 @@
       <c r="AA14" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="AB14" s="139"/>
+      <c r="AB14" s="145"/>
       <c r="AC14" s="27" t="s">
         <v>58</v>
       </c>
@@ -5330,66 +5331,66 @@
       <c r="AK14" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="AL14" s="140"/>
-      <c r="AM14" s="83" t="s">
+      <c r="AL14" s="146"/>
+      <c r="AM14" s="80" t="s">
         <v>131</v>
       </c>
-      <c r="AN14" s="85" t="s">
+      <c r="AN14" s="82" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="15" spans="1:40" ht="15">
-      <c r="A15" s="59">
+      <c r="A15" s="57">
         <v>12</v>
       </c>
-      <c r="B15" s="61" t="s">
+      <c r="B15" s="59" t="s">
         <v>121</v>
       </c>
-      <c r="C15" s="82"/>
-      <c r="D15" s="62">
+      <c r="C15" s="79"/>
+      <c r="D15" s="60">
         <v>27</v>
       </c>
-      <c r="E15" s="69">
+      <c r="E15" s="67">
         <v>887244</v>
       </c>
-      <c r="F15" s="69">
+      <c r="F15" s="67">
         <v>87229</v>
       </c>
-      <c r="G15" s="72">
+      <c r="G15" s="70">
         <f>F15*12</f>
         <v>1046748</v>
       </c>
-      <c r="H15" s="62">
+      <c r="H15" s="60">
         <v>1</v>
       </c>
-      <c r="I15" s="66" t="s">
+      <c r="I15" s="64" t="s">
         <v>61</v>
       </c>
-      <c r="J15" s="66" t="s">
+      <c r="J15" s="64" t="s">
         <v>27</v>
       </c>
-      <c r="K15" s="66" t="s">
+      <c r="K15" s="64" t="s">
         <v>62</v>
       </c>
-      <c r="L15" s="55" t="s">
+      <c r="L15" s="53" t="s">
         <v>104</v>
       </c>
-      <c r="M15" s="55" t="s">
+      <c r="M15" s="53" t="s">
         <v>128</v>
       </c>
-      <c r="N15" s="55" t="s">
+      <c r="N15" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="O15" s="58">
+      <c r="O15" s="56">
         <v>20497</v>
       </c>
-      <c r="P15" s="60">
+      <c r="P15" s="58">
         <v>33786</v>
       </c>
-      <c r="Q15" s="60">
+      <c r="Q15" s="58">
         <v>42587</v>
       </c>
-      <c r="R15" s="66" t="s">
+      <c r="R15" s="64" t="s">
         <v>127</v>
       </c>
       <c r="S15" s="32"/>
@@ -5414,52 +5415,52 @@
       <c r="AJ15" s="32"/>
       <c r="AK15" s="32"/>
       <c r="AL15" s="32"/>
-      <c r="AM15" s="84"/>
-      <c r="AN15" s="86"/>
+      <c r="AM15" s="81"/>
+      <c r="AN15" s="83"/>
     </row>
     <row r="16" spans="1:40" ht="15">
-      <c r="A16" s="59">
+      <c r="A16" s="57">
         <f>A15+1</f>
         <v>13</v>
       </c>
-      <c r="B16" s="61" t="s">
+      <c r="B16" s="59" t="s">
         <v>121</v>
       </c>
-      <c r="C16" s="82"/>
-      <c r="D16" s="62">
+      <c r="C16" s="79"/>
+      <c r="D16" s="60">
         <v>27</v>
       </c>
-      <c r="E16" s="69">
+      <c r="E16" s="67">
         <v>887244</v>
       </c>
-      <c r="F16" s="69">
+      <c r="F16" s="67">
         <v>87229</v>
       </c>
-      <c r="G16" s="72">
+      <c r="G16" s="70">
         <f t="shared" ref="G16:G26" si="0">F16*12</f>
         <v>1046748</v>
       </c>
-      <c r="H16" s="62">
+      <c r="H16" s="60">
         <v>1</v>
       </c>
-      <c r="I16" s="66" t="s">
+      <c r="I16" s="64" t="s">
         <v>61</v>
       </c>
-      <c r="J16" s="66" t="s">
+      <c r="J16" s="64" t="s">
         <v>27</v>
       </c>
-      <c r="K16" s="66" t="s">
+      <c r="K16" s="64" t="s">
         <v>62</v>
       </c>
-      <c r="L16" s="56" t="s">
+      <c r="L16" s="54" t="s">
         <v>105</v>
       </c>
-      <c r="M16" s="55"/>
-      <c r="N16" s="55"/>
-      <c r="O16" s="58"/>
-      <c r="P16" s="60"/>
-      <c r="Q16" s="68"/>
-      <c r="R16" s="66"/>
+      <c r="M16" s="53"/>
+      <c r="N16" s="53"/>
+      <c r="O16" s="56"/>
+      <c r="P16" s="58"/>
+      <c r="Q16" s="66"/>
+      <c r="R16" s="64"/>
       <c r="S16" s="32"/>
       <c r="T16" s="32"/>
       <c r="U16" s="32"/>
@@ -5480,52 +5481,52 @@
       <c r="AJ16" s="32"/>
       <c r="AK16" s="32"/>
       <c r="AL16" s="32"/>
-      <c r="AM16" s="84"/>
-      <c r="AN16" s="86">
+      <c r="AM16" s="81"/>
+      <c r="AN16" s="83">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:40" ht="15">
-      <c r="A17" s="59">
+      <c r="A17" s="57">
         <f t="shared" ref="A17:A26" si="1">A16+1</f>
         <v>14</v>
       </c>
-      <c r="B17" s="61" t="s">
+      <c r="B17" s="59" t="s">
         <v>121</v>
       </c>
-      <c r="C17" s="82"/>
-      <c r="D17" s="62">
+      <c r="C17" s="79"/>
+      <c r="D17" s="60">
         <v>27</v>
       </c>
-      <c r="E17" s="77"/>
-      <c r="F17" s="77">
+      <c r="E17" s="74"/>
+      <c r="F17" s="74">
         <v>87229</v>
       </c>
-      <c r="G17" s="72">
+      <c r="G17" s="70">
         <f t="shared" si="0"/>
         <v>1046748</v>
       </c>
-      <c r="H17" s="62">
+      <c r="H17" s="60">
         <v>1</v>
       </c>
-      <c r="I17" s="66" t="s">
+      <c r="I17" s="64" t="s">
         <v>61</v>
       </c>
-      <c r="J17" s="66" t="s">
+      <c r="J17" s="64" t="s">
         <v>27</v>
       </c>
-      <c r="K17" s="66" t="s">
+      <c r="K17" s="64" t="s">
         <v>62</v>
       </c>
-      <c r="L17" s="56" t="s">
+      <c r="L17" s="54" t="s">
         <v>106</v>
       </c>
-      <c r="M17" s="55"/>
-      <c r="N17" s="55"/>
-      <c r="O17" s="55"/>
-      <c r="P17" s="66"/>
-      <c r="Q17" s="71"/>
-      <c r="R17" s="66"/>
+      <c r="M17" s="53"/>
+      <c r="N17" s="53"/>
+      <c r="O17" s="53"/>
+      <c r="P17" s="64"/>
+      <c r="Q17" s="69"/>
+      <c r="R17" s="64"/>
       <c r="S17" s="32"/>
       <c r="T17" s="32"/>
       <c r="U17" s="32"/>
@@ -5546,66 +5547,66 @@
       <c r="AJ17" s="32"/>
       <c r="AK17" s="32"/>
       <c r="AL17" s="32"/>
-      <c r="AM17" s="84"/>
-      <c r="AN17" s="86">
+      <c r="AM17" s="81"/>
+      <c r="AN17" s="83">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:40" ht="15">
-      <c r="A18" s="59">
+      <c r="A18" s="57">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="B18" s="61" t="s">
+      <c r="B18" s="59" t="s">
         <v>134</v>
       </c>
-      <c r="C18" s="61" t="s">
+      <c r="C18" s="59" t="s">
         <v>137</v>
       </c>
-      <c r="D18" s="62">
+      <c r="D18" s="60">
         <v>26</v>
       </c>
-      <c r="E18" s="69">
+      <c r="E18" s="67">
         <v>812280</v>
       </c>
-      <c r="F18" s="69">
+      <c r="F18" s="67">
         <v>80039</v>
       </c>
-      <c r="G18" s="72">
+      <c r="G18" s="70">
         <f t="shared" si="0"/>
         <v>960468</v>
       </c>
-      <c r="H18" s="62">
+      <c r="H18" s="60">
         <v>2</v>
       </c>
-      <c r="I18" s="66" t="s">
+      <c r="I18" s="64" t="s">
         <v>61</v>
       </c>
-      <c r="J18" s="66" t="s">
+      <c r="J18" s="64" t="s">
         <v>27</v>
       </c>
-      <c r="K18" s="66" t="s">
+      <c r="K18" s="64" t="s">
         <v>62</v>
       </c>
-      <c r="L18" s="55" t="s">
+      <c r="L18" s="53" t="s">
         <v>90</v>
       </c>
-      <c r="M18" s="55" t="s">
+      <c r="M18" s="53" t="s">
         <v>91</v>
       </c>
-      <c r="N18" s="55" t="s">
+      <c r="N18" s="53" t="s">
         <v>92</v>
       </c>
-      <c r="O18" s="55" t="s">
+      <c r="O18" s="53" t="s">
         <v>93</v>
       </c>
-      <c r="P18" s="55" t="s">
+      <c r="P18" s="53" t="s">
         <v>119</v>
       </c>
-      <c r="Q18" s="65">
+      <c r="Q18" s="63">
         <v>41856</v>
       </c>
-      <c r="R18" s="66" t="s">
+      <c r="R18" s="64" t="s">
         <v>38</v>
       </c>
       <c r="S18" s="32"/>
@@ -5630,64 +5631,64 @@
       <c r="AJ18" s="32"/>
       <c r="AK18" s="32"/>
       <c r="AL18" s="32"/>
-      <c r="AM18" s="84"/>
-      <c r="AN18" s="86"/>
+      <c r="AM18" s="81"/>
+      <c r="AN18" s="83"/>
     </row>
     <row r="19" spans="1:40" ht="15">
-      <c r="A19" s="59">
+      <c r="A19" s="57">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="B19" s="61" t="s">
+      <c r="B19" s="59" t="s">
         <v>135</v>
       </c>
-      <c r="C19" s="61" t="s">
+      <c r="C19" s="59" t="s">
         <v>136</v>
       </c>
-      <c r="D19" s="62">
+      <c r="D19" s="60">
         <v>24</v>
       </c>
-      <c r="E19" s="69">
+      <c r="E19" s="67">
         <v>679320</v>
       </c>
-      <c r="F19" s="69">
+      <c r="F19" s="67">
         <v>65296</v>
       </c>
-      <c r="G19" s="72">
+      <c r="G19" s="70">
         <f t="shared" si="0"/>
         <v>783552</v>
       </c>
-      <c r="H19" s="62">
+      <c r="H19" s="60">
         <v>2</v>
       </c>
-      <c r="I19" s="66" t="s">
+      <c r="I19" s="64" t="s">
         <v>61</v>
       </c>
-      <c r="J19" s="66" t="s">
+      <c r="J19" s="64" t="s">
         <v>27</v>
       </c>
-      <c r="K19" s="66" t="s">
+      <c r="K19" s="64" t="s">
         <v>62</v>
       </c>
-      <c r="L19" s="55" t="s">
+      <c r="L19" s="53" t="s">
         <v>94</v>
       </c>
-      <c r="M19" s="55" t="s">
+      <c r="M19" s="53" t="s">
         <v>95</v>
       </c>
-      <c r="N19" s="55" t="s">
+      <c r="N19" s="53" t="s">
         <v>83</v>
       </c>
-      <c r="O19" s="55" t="s">
+      <c r="O19" s="53" t="s">
         <v>96</v>
       </c>
-      <c r="P19" s="58">
+      <c r="P19" s="56">
         <v>37371</v>
       </c>
-      <c r="Q19" s="65">
+      <c r="Q19" s="63">
         <v>41913</v>
       </c>
-      <c r="R19" s="66" t="s">
+      <c r="R19" s="64" t="s">
         <v>38</v>
       </c>
       <c r="S19" s="32"/>
@@ -5712,62 +5713,62 @@
       <c r="AJ19" s="32"/>
       <c r="AK19" s="32"/>
       <c r="AL19" s="32"/>
-      <c r="AM19" s="84"/>
-      <c r="AN19" s="86"/>
+      <c r="AM19" s="81"/>
+      <c r="AN19" s="83"/>
     </row>
     <row r="20" spans="1:40" ht="15">
-      <c r="A20" s="59">
+      <c r="A20" s="57">
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="B20" s="61" t="s">
+      <c r="B20" s="59" t="s">
         <v>122</v>
       </c>
-      <c r="C20" s="82"/>
-      <c r="D20" s="62">
+      <c r="C20" s="79"/>
+      <c r="D20" s="60">
         <v>22</v>
       </c>
-      <c r="E20" s="69">
+      <c r="E20" s="67">
         <v>597972</v>
       </c>
-      <c r="F20" s="69">
+      <c r="F20" s="67">
         <v>56487</v>
       </c>
-      <c r="G20" s="72">
+      <c r="G20" s="70">
         <f t="shared" si="0"/>
         <v>677844</v>
       </c>
-      <c r="H20" s="62">
+      <c r="H20" s="60">
         <v>6</v>
       </c>
-      <c r="I20" s="66" t="s">
+      <c r="I20" s="64" t="s">
         <v>61</v>
       </c>
-      <c r="J20" s="66" t="s">
+      <c r="J20" s="64" t="s">
         <v>27</v>
       </c>
-      <c r="K20" s="66" t="s">
+      <c r="K20" s="64" t="s">
         <v>11</v>
       </c>
-      <c r="L20" s="55" t="s">
+      <c r="L20" s="53" t="s">
         <v>82</v>
       </c>
-      <c r="M20" s="55" t="s">
+      <c r="M20" s="53" t="s">
         <v>87</v>
       </c>
-      <c r="N20" s="55" t="s">
+      <c r="N20" s="53" t="s">
         <v>84</v>
       </c>
-      <c r="O20" s="55" t="s">
+      <c r="O20" s="53" t="s">
         <v>97</v>
       </c>
-      <c r="P20" s="55" t="s">
+      <c r="P20" s="53" t="s">
         <v>120</v>
       </c>
-      <c r="Q20" s="58">
+      <c r="Q20" s="56">
         <v>37330</v>
       </c>
-      <c r="R20" s="66" t="s">
+      <c r="R20" s="64" t="s">
         <v>38</v>
       </c>
       <c r="S20" s="32"/>
@@ -5792,54 +5793,54 @@
       <c r="AJ20" s="32"/>
       <c r="AK20" s="32"/>
       <c r="AL20" s="32"/>
-      <c r="AM20" s="84"/>
-      <c r="AN20" s="86"/>
+      <c r="AM20" s="81"/>
+      <c r="AN20" s="83"/>
     </row>
     <row r="21" spans="1:40" ht="15">
-      <c r="A21" s="59">
+      <c r="A21" s="57">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="B21" s="61" t="s">
+      <c r="B21" s="59" t="s">
         <v>80</v>
       </c>
-      <c r="C21" s="61" t="s">
+      <c r="C21" s="59" t="s">
         <v>138</v>
       </c>
-      <c r="D21" s="62">
+      <c r="D21" s="60">
         <v>18</v>
       </c>
-      <c r="E21" s="69">
+      <c r="E21" s="67">
         <v>419952</v>
       </c>
-      <c r="F21" s="69">
+      <c r="F21" s="67">
         <v>38085</v>
       </c>
-      <c r="G21" s="72">
+      <c r="G21" s="70">
         <f t="shared" si="0"/>
         <v>457020</v>
       </c>
-      <c r="H21" s="62">
+      <c r="H21" s="60">
         <v>1</v>
       </c>
-      <c r="I21" s="66" t="s">
+      <c r="I21" s="64" t="s">
         <v>61</v>
       </c>
-      <c r="J21" s="66" t="s">
+      <c r="J21" s="64" t="s">
         <v>27</v>
       </c>
-      <c r="K21" s="66" t="s">
+      <c r="K21" s="64" t="s">
         <v>63</v>
       </c>
-      <c r="L21" s="56" t="s">
+      <c r="L21" s="54" t="s">
         <v>88</v>
       </c>
-      <c r="M21" s="55"/>
-      <c r="N21" s="55"/>
-      <c r="O21" s="55"/>
-      <c r="P21" s="55"/>
-      <c r="Q21" s="58"/>
-      <c r="R21" s="66"/>
+      <c r="M21" s="53"/>
+      <c r="N21" s="53"/>
+      <c r="O21" s="53"/>
+      <c r="P21" s="53"/>
+      <c r="Q21" s="56"/>
+      <c r="R21" s="64"/>
       <c r="S21" s="32"/>
       <c r="T21" s="32"/>
       <c r="U21" s="32"/>
@@ -5860,61 +5861,61 @@
       <c r="AJ21" s="32"/>
       <c r="AK21" s="32"/>
       <c r="AL21" s="32"/>
-      <c r="AM21" s="84"/>
-      <c r="AN21" s="86">
+      <c r="AM21" s="81"/>
+      <c r="AN21" s="83">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:40" ht="15">
-      <c r="A22" s="59">
+      <c r="A22" s="57">
         <f>A21+1</f>
         <v>19</v>
       </c>
-      <c r="B22" s="61" t="s">
+      <c r="B22" s="59" t="s">
         <v>126</v>
       </c>
-      <c r="C22" s="88"/>
-      <c r="D22" s="62">
+      <c r="C22" s="85"/>
+      <c r="D22" s="60">
         <v>11</v>
       </c>
-      <c r="E22" s="73">
+      <c r="E22" s="71">
         <v>228924</v>
       </c>
-      <c r="F22" s="73">
+      <c r="F22" s="71">
         <v>19620</v>
       </c>
-      <c r="G22" s="72">
+      <c r="G22" s="70">
         <f t="shared" si="0"/>
         <v>235440</v>
       </c>
-      <c r="H22" s="74">
+      <c r="H22" s="72">
         <v>1</v>
       </c>
-      <c r="I22" s="66" t="s">
+      <c r="I22" s="64" t="s">
         <v>61</v>
       </c>
-      <c r="J22" s="66" t="s">
+      <c r="J22" s="64" t="s">
         <v>27</v>
       </c>
-      <c r="K22" s="66" t="s">
+      <c r="K22" s="64" t="s">
         <v>63</v>
       </c>
-      <c r="L22" s="64" t="s">
+      <c r="L22" s="62" t="s">
         <v>107</v>
       </c>
-      <c r="M22" s="64" t="s">
+      <c r="M22" s="62" t="s">
         <v>108</v>
       </c>
-      <c r="N22" s="64" t="s">
+      <c r="N22" s="62" t="s">
         <v>109</v>
       </c>
-      <c r="O22" s="67">
+      <c r="O22" s="65">
         <v>31943</v>
       </c>
-      <c r="P22" s="67">
+      <c r="P22" s="65">
         <v>42068</v>
       </c>
-      <c r="Q22" s="65">
+      <c r="Q22" s="63">
         <v>43000</v>
       </c>
       <c r="R22" s="30" t="s">
@@ -5942,142 +5943,142 @@
       <c r="AJ22" s="32"/>
       <c r="AK22" s="32"/>
       <c r="AL22" s="32"/>
-      <c r="AM22" s="84"/>
-      <c r="AN22" s="86"/>
-    </row>
-    <row r="23" spans="1:40" s="100" customFormat="1" ht="15">
-      <c r="A23" s="90">
+      <c r="AM22" s="81"/>
+      <c r="AN22" s="83"/>
+    </row>
+    <row r="23" spans="1:40" s="97" customFormat="1" ht="15">
+      <c r="A23" s="87">
         <f>A22+1</f>
         <v>20</v>
       </c>
-      <c r="B23" s="89" t="s">
+      <c r="B23" s="86" t="s">
         <v>123</v>
       </c>
-      <c r="C23" s="89"/>
-      <c r="D23" s="91">
+      <c r="C23" s="86"/>
+      <c r="D23" s="88">
         <v>10</v>
       </c>
-      <c r="E23" s="92">
+      <c r="E23" s="89">
         <v>212760</v>
       </c>
-      <c r="F23" s="92">
+      <c r="F23" s="89">
         <v>18217</v>
       </c>
-      <c r="G23" s="93">
+      <c r="G23" s="90">
         <f t="shared" si="0"/>
         <v>218604</v>
       </c>
-      <c r="H23" s="91">
+      <c r="H23" s="88">
         <v>1</v>
       </c>
-      <c r="I23" s="94" t="s">
+      <c r="I23" s="91" t="s">
         <v>61</v>
       </c>
-      <c r="J23" s="94" t="s">
+      <c r="J23" s="91" t="s">
         <v>27</v>
       </c>
-      <c r="K23" s="94" t="s">
+      <c r="K23" s="91" t="s">
         <v>9</v>
       </c>
-      <c r="L23" s="95" t="s">
+      <c r="L23" s="92" t="s">
         <v>113</v>
       </c>
-      <c r="M23" s="95" t="s">
+      <c r="M23" s="92" t="s">
         <v>114</v>
       </c>
-      <c r="N23" s="95" t="s">
+      <c r="N23" s="92" t="s">
         <v>115</v>
       </c>
-      <c r="O23" s="96">
+      <c r="O23" s="93">
         <v>24506</v>
       </c>
-      <c r="P23" s="95" t="s">
+      <c r="P23" s="92" t="s">
         <v>116</v>
       </c>
-      <c r="Q23" s="97">
+      <c r="Q23" s="94">
         <v>43045</v>
       </c>
-      <c r="R23" s="98" t="s">
+      <c r="R23" s="95" t="s">
         <v>38</v>
       </c>
-      <c r="S23" s="99">
+      <c r="S23" s="96">
         <v>1</v>
       </c>
-      <c r="T23" s="99"/>
-      <c r="U23" s="99"/>
-      <c r="V23" s="99"/>
-      <c r="W23" s="99"/>
-      <c r="X23" s="99"/>
-      <c r="Y23" s="99"/>
-      <c r="Z23" s="99"/>
-      <c r="AA23" s="99"/>
-      <c r="AB23" s="99"/>
-      <c r="AC23" s="99"/>
-      <c r="AD23" s="99"/>
-      <c r="AE23" s="99"/>
-      <c r="AF23" s="99"/>
-      <c r="AG23" s="99"/>
-      <c r="AH23" s="99"/>
-      <c r="AI23" s="99"/>
-      <c r="AJ23" s="99"/>
-      <c r="AK23" s="99"/>
-      <c r="AL23" s="99"/>
-      <c r="AM23" s="99"/>
-      <c r="AN23" s="99"/>
+      <c r="T23" s="96"/>
+      <c r="U23" s="96"/>
+      <c r="V23" s="96"/>
+      <c r="W23" s="96"/>
+      <c r="X23" s="96"/>
+      <c r="Y23" s="96"/>
+      <c r="Z23" s="96"/>
+      <c r="AA23" s="96"/>
+      <c r="AB23" s="96"/>
+      <c r="AC23" s="96"/>
+      <c r="AD23" s="96"/>
+      <c r="AE23" s="96"/>
+      <c r="AF23" s="96"/>
+      <c r="AG23" s="96"/>
+      <c r="AH23" s="96"/>
+      <c r="AI23" s="96"/>
+      <c r="AJ23" s="96"/>
+      <c r="AK23" s="96"/>
+      <c r="AL23" s="96"/>
+      <c r="AM23" s="96"/>
+      <c r="AN23" s="96"/>
     </row>
     <row r="24" spans="1:40" ht="15">
-      <c r="A24" s="59">
+      <c r="A24" s="57">
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="B24" s="61" t="s">
+      <c r="B24" s="59" t="s">
         <v>123</v>
       </c>
-      <c r="C24" s="82"/>
-      <c r="D24" s="62">
+      <c r="C24" s="79"/>
+      <c r="D24" s="60">
         <v>10</v>
       </c>
-      <c r="E24" s="69">
+      <c r="E24" s="67">
         <v>223608</v>
       </c>
-      <c r="F24" s="69">
+      <c r="F24" s="67">
         <v>19095</v>
       </c>
-      <c r="G24" s="72">
+      <c r="G24" s="70">
         <f t="shared" si="0"/>
         <v>229140</v>
       </c>
-      <c r="H24" s="62">
+      <c r="H24" s="60">
         <v>6</v>
       </c>
-      <c r="I24" s="66" t="s">
+      <c r="I24" s="64" t="s">
         <v>61</v>
       </c>
-      <c r="J24" s="66" t="s">
+      <c r="J24" s="64" t="s">
         <v>27</v>
       </c>
-      <c r="K24" s="66" t="s">
+      <c r="K24" s="64" t="s">
         <v>9</v>
       </c>
-      <c r="L24" s="55" t="s">
+      <c r="L24" s="53" t="s">
         <v>98</v>
       </c>
-      <c r="M24" s="55" t="s">
+      <c r="M24" s="53" t="s">
         <v>99</v>
       </c>
-      <c r="N24" s="55" t="s">
+      <c r="N24" s="53" t="s">
         <v>100</v>
       </c>
-      <c r="O24" s="55" t="s">
+      <c r="O24" s="53" t="s">
         <v>101</v>
       </c>
-      <c r="P24" s="58">
+      <c r="P24" s="56">
         <v>28977</v>
       </c>
-      <c r="Q24" s="58">
+      <c r="Q24" s="56">
         <v>37043</v>
       </c>
-      <c r="R24" s="66" t="s">
+      <c r="R24" s="64" t="s">
         <v>38</v>
       </c>
       <c r="S24" s="32">
@@ -6102,62 +6103,62 @@
       <c r="AJ24" s="32"/>
       <c r="AK24" s="32"/>
       <c r="AL24" s="32"/>
-      <c r="AM24" s="84"/>
-      <c r="AN24" s="86"/>
+      <c r="AM24" s="81"/>
+      <c r="AN24" s="83"/>
     </row>
     <row r="25" spans="1:40" ht="15">
-      <c r="A25" s="59">
+      <c r="A25" s="57">
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="B25" s="61" t="s">
+      <c r="B25" s="59" t="s">
         <v>124</v>
       </c>
-      <c r="C25" s="82"/>
-      <c r="D25" s="62">
+      <c r="C25" s="79"/>
+      <c r="D25" s="60">
         <v>8</v>
       </c>
-      <c r="E25" s="69">
+      <c r="E25" s="67">
         <v>184416</v>
       </c>
-      <c r="F25" s="69">
+      <c r="F25" s="67">
         <v>15818</v>
       </c>
-      <c r="G25" s="72">
+      <c r="G25" s="70">
         <f t="shared" si="0"/>
         <v>189816</v>
       </c>
-      <c r="H25" s="62">
+      <c r="H25" s="60">
         <v>1</v>
       </c>
-      <c r="I25" s="66" t="s">
+      <c r="I25" s="64" t="s">
         <v>61</v>
       </c>
-      <c r="J25" s="66" t="s">
+      <c r="J25" s="64" t="s">
         <v>27</v>
       </c>
-      <c r="K25" s="66" t="s">
+      <c r="K25" s="64" t="s">
         <v>9</v>
       </c>
-      <c r="L25" s="57" t="s">
+      <c r="L25" s="55" t="s">
         <v>110</v>
       </c>
-      <c r="M25" s="78" t="s">
+      <c r="M25" s="75" t="s">
         <v>111</v>
       </c>
-      <c r="N25" s="57" t="s">
+      <c r="N25" s="55" t="s">
         <v>112</v>
       </c>
-      <c r="O25" s="58">
+      <c r="O25" s="56">
         <v>30200</v>
       </c>
-      <c r="P25" s="58">
+      <c r="P25" s="56">
         <v>42087</v>
       </c>
-      <c r="Q25" s="60">
+      <c r="Q25" s="58">
         <v>43045</v>
       </c>
-      <c r="R25" s="66" t="s">
+      <c r="R25" s="64" t="s">
         <v>38</v>
       </c>
       <c r="S25" s="32"/>
@@ -6182,62 +6183,62 @@
       <c r="AJ25" s="32"/>
       <c r="AK25" s="32"/>
       <c r="AL25" s="32"/>
-      <c r="AM25" s="84"/>
-      <c r="AN25" s="86"/>
+      <c r="AM25" s="81"/>
+      <c r="AN25" s="83"/>
     </row>
     <row r="26" spans="1:40" ht="15">
-      <c r="A26" s="59">
+      <c r="A26" s="57">
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
-      <c r="B26" s="61" t="s">
+      <c r="B26" s="59" t="s">
         <v>125</v>
       </c>
-      <c r="C26" s="82"/>
-      <c r="D26" s="62">
+      <c r="C26" s="79"/>
+      <c r="D26" s="60">
         <v>6</v>
       </c>
-      <c r="E26" s="69">
+      <c r="E26" s="67">
         <v>162048</v>
       </c>
-      <c r="F26" s="69">
+      <c r="F26" s="67">
         <v>13973</v>
       </c>
-      <c r="G26" s="72">
+      <c r="G26" s="70">
         <f t="shared" si="0"/>
         <v>167676</v>
       </c>
-      <c r="H26" s="62">
+      <c r="H26" s="60">
         <v>2</v>
       </c>
-      <c r="I26" s="66" t="s">
+      <c r="I26" s="64" t="s">
         <v>61</v>
       </c>
-      <c r="J26" s="66" t="s">
+      <c r="J26" s="64" t="s">
         <v>27</v>
       </c>
-      <c r="K26" s="66" t="s">
+      <c r="K26" s="64" t="s">
         <v>9</v>
       </c>
-      <c r="L26" s="55" t="s">
+      <c r="L26" s="53" t="s">
         <v>102</v>
       </c>
-      <c r="M26" s="55" t="s">
+      <c r="M26" s="53" t="s">
         <v>85</v>
       </c>
-      <c r="N26" s="55" t="s">
+      <c r="N26" s="53" t="s">
         <v>103</v>
       </c>
-      <c r="O26" s="58">
+      <c r="O26" s="56">
         <v>22967</v>
       </c>
-      <c r="P26" s="58">
+      <c r="P26" s="56">
         <v>37043</v>
       </c>
-      <c r="Q26" s="58">
+      <c r="Q26" s="56">
         <v>41260</v>
       </c>
-      <c r="R26" s="66" t="s">
+      <c r="R26" s="64" t="s">
         <v>38</v>
       </c>
       <c r="S26" s="32"/>
@@ -6262,15 +6263,15 @@
       <c r="AJ26" s="32"/>
       <c r="AK26" s="32"/>
       <c r="AL26" s="32"/>
-      <c r="AM26" s="84"/>
-      <c r="AN26" s="86"/>
+      <c r="AM26" s="81"/>
+      <c r="AN26" s="83"/>
     </row>
     <row r="27" spans="1:40" ht="15">
-      <c r="A27" s="38" t="s">
+      <c r="A27" s="36" t="s">
         <v>118</v>
       </c>
-      <c r="E27" s="70"/>
-      <c r="F27" s="81"/>
+      <c r="E27" s="68"/>
+      <c r="F27" s="78"/>
       <c r="G27" s="6"/>
       <c r="S27" s="1">
         <f>SUM(S15:S26)</f>
@@ -6354,559 +6355,559 @@
       </c>
     </row>
     <row r="28" spans="1:40" ht="15">
-      <c r="Q28" s="39" t="s">
+      <c r="Q28" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="R28" s="40"/>
-      <c r="S28" s="41">
+      <c r="R28" s="38"/>
+      <c r="S28" s="39">
         <f>SUM(S27:AL27)</f>
         <v>9</v>
       </c>
-      <c r="AM28" s="87">
+      <c r="AM28" s="84">
         <f>SUM(AM15:AM26)</f>
         <v>0</v>
       </c>
-      <c r="AN28" s="87">
+      <c r="AN28" s="84">
         <f>SUM(AN15:AN26)</f>
         <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:40">
-      <c r="A29" s="38" t="s">
+      <c r="A29" s="36" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="30" spans="1:40" ht="15">
-      <c r="A30" s="38" t="s">
+      <c r="A30" s="36" t="s">
         <v>66</v>
       </c>
-      <c r="Q30" s="42" t="s">
+      <c r="Q30" s="40" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="31" spans="1:40" ht="15">
-      <c r="A31" s="38" t="s">
+      <c r="A31" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="Q31" s="42" t="s">
+      <c r="Q31" s="40" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="32" spans="1:40" ht="15">
-      <c r="A32" s="117" t="s">
+      <c r="A32" s="123" t="s">
         <v>70</v>
       </c>
-      <c r="B32" s="117"/>
-      <c r="C32" s="117"/>
-      <c r="D32" s="117"/>
-      <c r="M32" s="43" t="s">
+      <c r="B32" s="123"/>
+      <c r="C32" s="123"/>
+      <c r="D32" s="123"/>
+      <c r="M32" s="41" t="s">
         <v>71</v>
       </c>
-      <c r="Q32" s="42" t="s">
+      <c r="Q32" s="40" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="33" spans="1:17" ht="15">
-      <c r="Q33" s="42" t="s">
+      <c r="Q33" s="40" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="34" spans="1:17" ht="15">
-      <c r="Q34" s="42" t="s">
+      <c r="Q34" s="40" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="35" spans="1:17" ht="15">
-      <c r="A35" s="118" t="s">
+      <c r="A35" s="124" t="s">
         <v>75</v>
       </c>
-      <c r="B35" s="118"/>
-      <c r="C35" s="118"/>
-      <c r="D35" s="118"/>
-      <c r="G35" s="119">
+      <c r="B35" s="124"/>
+      <c r="C35" s="124"/>
+      <c r="D35" s="124"/>
+      <c r="G35" s="125">
         <v>43465</v>
       </c>
-      <c r="H35" s="120"/>
-      <c r="M35" s="121" t="s">
+      <c r="H35" s="126"/>
+      <c r="M35" s="127" t="s">
         <v>133</v>
       </c>
-      <c r="N35" s="121"/>
-      <c r="O35" s="121"/>
-      <c r="Q35" s="42" t="s">
+      <c r="N35" s="127"/>
+      <c r="O35" s="127"/>
+      <c r="Q35" s="40" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="36" spans="1:17" ht="15">
-      <c r="A36" s="125" t="s">
+      <c r="A36" s="131" t="s">
         <v>77</v>
       </c>
-      <c r="B36" s="125"/>
-      <c r="C36" s="125"/>
-      <c r="D36" s="125"/>
-      <c r="E36" s="43"/>
-      <c r="F36" s="43"/>
-      <c r="G36" s="123" t="s">
+      <c r="B36" s="131"/>
+      <c r="C36" s="131"/>
+      <c r="D36" s="131"/>
+      <c r="E36" s="41"/>
+      <c r="F36" s="41"/>
+      <c r="G36" s="129" t="s">
         <v>78</v>
       </c>
-      <c r="H36" s="123"/>
-      <c r="I36" s="44"/>
-      <c r="J36" s="44"/>
-      <c r="M36" s="124" t="s">
+      <c r="H36" s="129"/>
+      <c r="I36" s="42"/>
+      <c r="J36" s="42"/>
+      <c r="M36" s="130" t="s">
         <v>86</v>
       </c>
-      <c r="N36" s="124"/>
-      <c r="O36" s="124"/>
-      <c r="Q36" s="42" t="s">
+      <c r="N36" s="130"/>
+      <c r="O36" s="130"/>
+      <c r="Q36" s="40" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="37" spans="1:17" ht="15">
-      <c r="E37" s="44"/>
-      <c r="F37" s="44"/>
+      <c r="E37" s="42"/>
+      <c r="F37" s="42"/>
     </row>
     <row r="38" spans="1:17" ht="15">
-      <c r="K38" s="44"/>
+      <c r="K38" s="42"/>
     </row>
     <row r="39" spans="1:17" ht="15">
-      <c r="B39" s="44"/>
-      <c r="C39" s="44"/>
-      <c r="K39" s="44"/>
-      <c r="Q39" s="45"/>
+      <c r="B39" s="42"/>
+      <c r="C39" s="42"/>
+      <c r="K39" s="42"/>
+      <c r="Q39" s="43"/>
     </row>
     <row r="43" spans="1:17" ht="14.25">
-      <c r="B43" s="46"/>
-      <c r="C43" s="46"/>
-      <c r="D43" s="47"/>
-      <c r="E43" s="47"/>
-      <c r="F43" s="47"/>
-      <c r="G43" s="47"/>
-      <c r="H43" s="48"/>
-      <c r="I43" s="47"/>
-      <c r="J43" s="47"/>
-      <c r="K43" s="48"/>
-      <c r="L43" s="48"/>
-      <c r="M43" s="49"/>
-      <c r="N43" s="50"/>
+      <c r="B43" s="44"/>
+      <c r="C43" s="44"/>
+      <c r="D43" s="45"/>
+      <c r="E43" s="45"/>
+      <c r="F43" s="45"/>
+      <c r="G43" s="45"/>
+      <c r="H43" s="46"/>
+      <c r="I43" s="45"/>
+      <c r="J43" s="45"/>
+      <c r="K43" s="46"/>
+      <c r="L43" s="46"/>
+      <c r="M43" s="47"/>
+      <c r="N43" s="48"/>
     </row>
     <row r="44" spans="1:17" ht="14.25">
-      <c r="B44" s="46"/>
-      <c r="C44" s="46"/>
-      <c r="D44" s="47"/>
-      <c r="E44" s="47"/>
-      <c r="F44" s="47"/>
-      <c r="G44" s="47"/>
-      <c r="H44" s="48"/>
-      <c r="I44" s="47"/>
-      <c r="J44" s="47"/>
-      <c r="K44" s="48"/>
-      <c r="L44" s="48"/>
-      <c r="M44" s="49"/>
-      <c r="N44" s="50"/>
+      <c r="B44" s="44"/>
+      <c r="C44" s="44"/>
+      <c r="D44" s="45"/>
+      <c r="E44" s="45"/>
+      <c r="F44" s="45"/>
+      <c r="G44" s="45"/>
+      <c r="H44" s="46"/>
+      <c r="I44" s="45"/>
+      <c r="J44" s="45"/>
+      <c r="K44" s="46"/>
+      <c r="L44" s="46"/>
+      <c r="M44" s="47"/>
+      <c r="N44" s="48"/>
     </row>
     <row r="45" spans="1:17" ht="15">
-      <c r="B45" s="42"/>
-      <c r="C45" s="42"/>
-      <c r="D45" s="45"/>
-      <c r="E45" s="47"/>
-      <c r="F45" s="47"/>
-      <c r="G45" s="47"/>
-      <c r="H45" s="42"/>
-      <c r="I45" s="42"/>
-      <c r="J45" s="47"/>
-      <c r="K45" s="48"/>
-      <c r="L45" s="42"/>
-      <c r="M45" s="45"/>
-      <c r="N45" s="50"/>
+      <c r="B45" s="40"/>
+      <c r="C45" s="40"/>
+      <c r="D45" s="43"/>
+      <c r="E45" s="45"/>
+      <c r="F45" s="45"/>
+      <c r="G45" s="45"/>
+      <c r="H45" s="40"/>
+      <c r="I45" s="40"/>
+      <c r="J45" s="45"/>
+      <c r="K45" s="46"/>
+      <c r="L45" s="40"/>
+      <c r="M45" s="43"/>
+      <c r="N45" s="48"/>
     </row>
     <row r="46" spans="1:17" ht="15">
-      <c r="B46" s="42"/>
-      <c r="C46" s="42"/>
-      <c r="D46" s="45"/>
-      <c r="E46" s="47"/>
-      <c r="F46" s="47"/>
-      <c r="G46" s="47"/>
-      <c r="H46" s="42"/>
-      <c r="I46" s="42"/>
-      <c r="J46" s="47"/>
-      <c r="K46" s="48"/>
-      <c r="L46" s="42"/>
-      <c r="M46" s="45"/>
-      <c r="N46" s="50"/>
+      <c r="B46" s="40"/>
+      <c r="C46" s="40"/>
+      <c r="D46" s="43"/>
+      <c r="E46" s="45"/>
+      <c r="F46" s="45"/>
+      <c r="G46" s="45"/>
+      <c r="H46" s="40"/>
+      <c r="I46" s="40"/>
+      <c r="J46" s="45"/>
+      <c r="K46" s="46"/>
+      <c r="L46" s="40"/>
+      <c r="M46" s="43"/>
+      <c r="N46" s="48"/>
     </row>
     <row r="47" spans="1:17" ht="15">
-      <c r="B47" s="42"/>
-      <c r="C47" s="42"/>
-      <c r="D47" s="45"/>
-      <c r="E47" s="47"/>
-      <c r="F47" s="47"/>
-      <c r="G47" s="47"/>
-      <c r="H47" s="42"/>
-      <c r="I47" s="42"/>
-      <c r="J47" s="47"/>
-      <c r="K47" s="48"/>
-      <c r="L47" s="42"/>
-      <c r="M47" s="45"/>
-      <c r="N47" s="50"/>
+      <c r="B47" s="40"/>
+      <c r="C47" s="40"/>
+      <c r="D47" s="43"/>
+      <c r="E47" s="45"/>
+      <c r="F47" s="45"/>
+      <c r="G47" s="45"/>
+      <c r="H47" s="40"/>
+      <c r="I47" s="40"/>
+      <c r="J47" s="45"/>
+      <c r="K47" s="46"/>
+      <c r="L47" s="40"/>
+      <c r="M47" s="43"/>
+      <c r="N47" s="48"/>
     </row>
     <row r="48" spans="1:17" ht="14.25">
-      <c r="B48" s="46"/>
-      <c r="C48" s="46"/>
-      <c r="D48" s="47"/>
-      <c r="E48" s="47"/>
-      <c r="F48" s="47"/>
-      <c r="G48" s="47"/>
-      <c r="H48" s="48"/>
-      <c r="I48" s="47"/>
-      <c r="J48" s="47"/>
-      <c r="K48" s="48"/>
-      <c r="L48" s="48"/>
-      <c r="M48" s="49"/>
-      <c r="N48" s="50"/>
+      <c r="B48" s="44"/>
+      <c r="C48" s="44"/>
+      <c r="D48" s="45"/>
+      <c r="E48" s="45"/>
+      <c r="F48" s="45"/>
+      <c r="G48" s="45"/>
+      <c r="H48" s="46"/>
+      <c r="I48" s="45"/>
+      <c r="J48" s="45"/>
+      <c r="K48" s="46"/>
+      <c r="L48" s="46"/>
+      <c r="M48" s="47"/>
+      <c r="N48" s="48"/>
     </row>
     <row r="49" spans="2:14" ht="15">
-      <c r="B49" s="42"/>
-      <c r="C49" s="42"/>
-      <c r="D49" s="45"/>
-      <c r="E49" s="47"/>
-      <c r="F49" s="47"/>
-      <c r="G49" s="47"/>
-      <c r="H49" s="48"/>
-      <c r="I49" s="47"/>
-      <c r="J49" s="47"/>
-      <c r="K49" s="48"/>
-      <c r="L49" s="42"/>
-      <c r="M49" s="45"/>
-      <c r="N49" s="50"/>
+      <c r="B49" s="40"/>
+      <c r="C49" s="40"/>
+      <c r="D49" s="43"/>
+      <c r="E49" s="45"/>
+      <c r="F49" s="45"/>
+      <c r="G49" s="45"/>
+      <c r="H49" s="46"/>
+      <c r="I49" s="45"/>
+      <c r="J49" s="45"/>
+      <c r="K49" s="46"/>
+      <c r="L49" s="40"/>
+      <c r="M49" s="43"/>
+      <c r="N49" s="48"/>
     </row>
     <row r="50" spans="2:14" ht="15">
-      <c r="B50" s="42"/>
-      <c r="C50" s="42"/>
-      <c r="D50" s="45"/>
-      <c r="E50" s="47"/>
-      <c r="F50" s="47"/>
-      <c r="G50" s="47"/>
-      <c r="H50" s="48"/>
-      <c r="I50" s="47"/>
-      <c r="J50" s="47"/>
-      <c r="K50" s="48"/>
-      <c r="L50" s="42"/>
-      <c r="M50" s="49"/>
-      <c r="N50" s="50"/>
+      <c r="B50" s="40"/>
+      <c r="C50" s="40"/>
+      <c r="D50" s="43"/>
+      <c r="E50" s="45"/>
+      <c r="F50" s="45"/>
+      <c r="G50" s="45"/>
+      <c r="H50" s="46"/>
+      <c r="I50" s="45"/>
+      <c r="J50" s="45"/>
+      <c r="K50" s="46"/>
+      <c r="L50" s="40"/>
+      <c r="M50" s="47"/>
+      <c r="N50" s="48"/>
     </row>
     <row r="51" spans="2:14" ht="14.25">
-      <c r="B51" s="115"/>
-      <c r="C51" s="115"/>
-      <c r="D51" s="116"/>
-      <c r="E51" s="47"/>
-      <c r="F51" s="47"/>
-      <c r="G51" s="47"/>
-      <c r="H51" s="48"/>
-      <c r="I51" s="47"/>
-      <c r="J51" s="47"/>
-      <c r="K51" s="48"/>
-      <c r="L51" s="48"/>
-      <c r="M51" s="49"/>
-      <c r="N51" s="50"/>
+      <c r="B51" s="121"/>
+      <c r="C51" s="121"/>
+      <c r="D51" s="122"/>
+      <c r="E51" s="45"/>
+      <c r="F51" s="45"/>
+      <c r="G51" s="45"/>
+      <c r="H51" s="46"/>
+      <c r="I51" s="45"/>
+      <c r="J51" s="45"/>
+      <c r="K51" s="46"/>
+      <c r="L51" s="46"/>
+      <c r="M51" s="47"/>
+      <c r="N51" s="48"/>
     </row>
     <row r="52" spans="2:14" ht="15">
-      <c r="B52" s="51"/>
-      <c r="C52" s="51"/>
-      <c r="D52" s="52"/>
-      <c r="E52" s="47"/>
-      <c r="F52" s="47"/>
-      <c r="G52" s="47"/>
-      <c r="H52" s="48"/>
-      <c r="I52" s="47"/>
-      <c r="J52" s="47"/>
-      <c r="K52" s="48"/>
-      <c r="L52" s="48"/>
-      <c r="M52" s="49"/>
-      <c r="N52" s="50"/>
+      <c r="B52" s="49"/>
+      <c r="C52" s="49"/>
+      <c r="D52" s="50"/>
+      <c r="E52" s="45"/>
+      <c r="F52" s="45"/>
+      <c r="G52" s="45"/>
+      <c r="H52" s="46"/>
+      <c r="I52" s="45"/>
+      <c r="J52" s="45"/>
+      <c r="K52" s="46"/>
+      <c r="L52" s="46"/>
+      <c r="M52" s="47"/>
+      <c r="N52" s="48"/>
     </row>
     <row r="53" spans="2:14" ht="14.25">
-      <c r="B53" s="46"/>
-      <c r="C53" s="46"/>
-      <c r="D53" s="47"/>
-      <c r="E53" s="47"/>
-      <c r="F53" s="47"/>
-      <c r="G53" s="47"/>
-      <c r="H53" s="48"/>
-      <c r="I53" s="47"/>
-      <c r="J53" s="47"/>
-      <c r="K53" s="48"/>
-      <c r="L53" s="48"/>
-      <c r="M53" s="49"/>
-      <c r="N53" s="50"/>
+      <c r="B53" s="44"/>
+      <c r="C53" s="44"/>
+      <c r="D53" s="45"/>
+      <c r="E53" s="45"/>
+      <c r="F53" s="45"/>
+      <c r="G53" s="45"/>
+      <c r="H53" s="46"/>
+      <c r="I53" s="45"/>
+      <c r="J53" s="45"/>
+      <c r="K53" s="46"/>
+      <c r="L53" s="46"/>
+      <c r="M53" s="47"/>
+      <c r="N53" s="48"/>
     </row>
     <row r="54" spans="2:14" ht="14.25">
-      <c r="B54" s="46"/>
-      <c r="C54" s="46"/>
-      <c r="D54" s="47"/>
-      <c r="E54" s="47"/>
-      <c r="F54" s="47"/>
-      <c r="G54" s="47"/>
-      <c r="H54" s="48"/>
-      <c r="I54" s="47"/>
-      <c r="J54" s="47"/>
-      <c r="K54" s="48"/>
-      <c r="L54" s="48"/>
-      <c r="M54" s="49"/>
-      <c r="N54" s="50"/>
+      <c r="B54" s="44"/>
+      <c r="C54" s="44"/>
+      <c r="D54" s="45"/>
+      <c r="E54" s="45"/>
+      <c r="F54" s="45"/>
+      <c r="G54" s="45"/>
+      <c r="H54" s="46"/>
+      <c r="I54" s="45"/>
+      <c r="J54" s="45"/>
+      <c r="K54" s="46"/>
+      <c r="L54" s="46"/>
+      <c r="M54" s="47"/>
+      <c r="N54" s="48"/>
     </row>
     <row r="55" spans="2:14" ht="15">
-      <c r="B55" s="42"/>
-      <c r="C55" s="42"/>
-      <c r="D55" s="45"/>
-      <c r="E55" s="47"/>
-      <c r="F55" s="47"/>
-      <c r="G55" s="47"/>
-      <c r="H55" s="48"/>
-      <c r="I55" s="47"/>
-      <c r="J55" s="47"/>
-      <c r="K55" s="48"/>
-      <c r="L55" s="42"/>
-      <c r="M55" s="45"/>
-      <c r="N55" s="50"/>
+      <c r="B55" s="40"/>
+      <c r="C55" s="40"/>
+      <c r="D55" s="43"/>
+      <c r="E55" s="45"/>
+      <c r="F55" s="45"/>
+      <c r="G55" s="45"/>
+      <c r="H55" s="46"/>
+      <c r="I55" s="45"/>
+      <c r="J55" s="45"/>
+      <c r="K55" s="46"/>
+      <c r="L55" s="40"/>
+      <c r="M55" s="43"/>
+      <c r="N55" s="48"/>
     </row>
     <row r="56" spans="2:14" ht="14.25">
-      <c r="B56" s="46"/>
-      <c r="C56" s="46"/>
-      <c r="D56" s="47"/>
-      <c r="E56" s="47"/>
-      <c r="F56" s="47"/>
-      <c r="G56" s="47"/>
-      <c r="H56" s="48"/>
-      <c r="I56" s="47"/>
-      <c r="J56" s="47"/>
-      <c r="K56" s="48"/>
-      <c r="L56" s="48"/>
-      <c r="M56" s="49"/>
-      <c r="N56" s="50"/>
+      <c r="B56" s="44"/>
+      <c r="C56" s="44"/>
+      <c r="D56" s="45"/>
+      <c r="E56" s="45"/>
+      <c r="F56" s="45"/>
+      <c r="G56" s="45"/>
+      <c r="H56" s="46"/>
+      <c r="I56" s="45"/>
+      <c r="J56" s="45"/>
+      <c r="K56" s="46"/>
+      <c r="L56" s="46"/>
+      <c r="M56" s="47"/>
+      <c r="N56" s="48"/>
     </row>
     <row r="57" spans="2:14" ht="15">
-      <c r="B57" s="42"/>
-      <c r="C57" s="42"/>
-      <c r="D57" s="45"/>
-      <c r="E57" s="47"/>
-      <c r="F57" s="47"/>
-      <c r="G57" s="47"/>
-      <c r="H57" s="48"/>
-      <c r="I57" s="47"/>
-      <c r="J57" s="47"/>
-      <c r="K57" s="48"/>
-      <c r="L57" s="42"/>
-      <c r="M57" s="45"/>
-      <c r="N57" s="50"/>
+      <c r="B57" s="40"/>
+      <c r="C57" s="40"/>
+      <c r="D57" s="43"/>
+      <c r="E57" s="45"/>
+      <c r="F57" s="45"/>
+      <c r="G57" s="45"/>
+      <c r="H57" s="46"/>
+      <c r="I57" s="45"/>
+      <c r="J57" s="45"/>
+      <c r="K57" s="46"/>
+      <c r="L57" s="40"/>
+      <c r="M57" s="43"/>
+      <c r="N57" s="48"/>
     </row>
     <row r="58" spans="2:14" ht="15">
-      <c r="B58" s="42"/>
-      <c r="C58" s="42"/>
-      <c r="D58" s="45"/>
-      <c r="E58" s="47"/>
-      <c r="F58" s="47"/>
-      <c r="G58" s="47"/>
-      <c r="H58" s="48"/>
-      <c r="I58" s="47"/>
-      <c r="J58" s="47"/>
-      <c r="K58" s="48"/>
-      <c r="L58" s="42"/>
-      <c r="M58" s="45"/>
-      <c r="N58" s="50"/>
+      <c r="B58" s="40"/>
+      <c r="C58" s="40"/>
+      <c r="D58" s="43"/>
+      <c r="E58" s="45"/>
+      <c r="F58" s="45"/>
+      <c r="G58" s="45"/>
+      <c r="H58" s="46"/>
+      <c r="I58" s="45"/>
+      <c r="J58" s="45"/>
+      <c r="K58" s="46"/>
+      <c r="L58" s="40"/>
+      <c r="M58" s="43"/>
+      <c r="N58" s="48"/>
     </row>
     <row r="59" spans="2:14" ht="15">
-      <c r="B59" s="42"/>
-      <c r="C59" s="42"/>
-      <c r="D59" s="45"/>
-      <c r="E59" s="47"/>
-      <c r="F59" s="47"/>
-      <c r="G59" s="47"/>
-      <c r="H59" s="48"/>
-      <c r="I59" s="47"/>
-      <c r="J59" s="47"/>
-      <c r="K59" s="48"/>
-      <c r="L59" s="42"/>
-      <c r="M59" s="45"/>
-      <c r="N59" s="50"/>
+      <c r="B59" s="40"/>
+      <c r="C59" s="40"/>
+      <c r="D59" s="43"/>
+      <c r="E59" s="45"/>
+      <c r="F59" s="45"/>
+      <c r="G59" s="45"/>
+      <c r="H59" s="46"/>
+      <c r="I59" s="45"/>
+      <c r="J59" s="45"/>
+      <c r="K59" s="46"/>
+      <c r="L59" s="40"/>
+      <c r="M59" s="43"/>
+      <c r="N59" s="48"/>
     </row>
     <row r="60" spans="2:14" ht="14.25">
-      <c r="B60" s="115"/>
-      <c r="C60" s="115"/>
-      <c r="D60" s="116"/>
-      <c r="E60" s="47"/>
-      <c r="F60" s="47"/>
-      <c r="G60" s="47"/>
-      <c r="H60" s="48"/>
-      <c r="I60" s="47"/>
-      <c r="J60" s="47"/>
-      <c r="K60" s="48"/>
-      <c r="L60" s="48"/>
-      <c r="M60" s="49"/>
-      <c r="N60" s="50"/>
+      <c r="B60" s="121"/>
+      <c r="C60" s="121"/>
+      <c r="D60" s="122"/>
+      <c r="E60" s="45"/>
+      <c r="F60" s="45"/>
+      <c r="G60" s="45"/>
+      <c r="H60" s="46"/>
+      <c r="I60" s="45"/>
+      <c r="J60" s="45"/>
+      <c r="K60" s="46"/>
+      <c r="L60" s="46"/>
+      <c r="M60" s="47"/>
+      <c r="N60" s="48"/>
     </row>
     <row r="61" spans="2:14" ht="15">
-      <c r="B61" s="42"/>
-      <c r="C61" s="42"/>
-      <c r="D61" s="45"/>
-      <c r="E61" s="47"/>
-      <c r="F61" s="47"/>
-      <c r="G61" s="47"/>
-      <c r="H61" s="48"/>
-      <c r="I61" s="47"/>
-      <c r="J61" s="47"/>
-      <c r="K61" s="48"/>
-      <c r="L61" s="42"/>
-      <c r="M61" s="45"/>
-      <c r="N61" s="50"/>
+      <c r="B61" s="40"/>
+      <c r="C61" s="40"/>
+      <c r="D61" s="43"/>
+      <c r="E61" s="45"/>
+      <c r="F61" s="45"/>
+      <c r="G61" s="45"/>
+      <c r="H61" s="46"/>
+      <c r="I61" s="45"/>
+      <c r="J61" s="45"/>
+      <c r="K61" s="46"/>
+      <c r="L61" s="40"/>
+      <c r="M61" s="43"/>
+      <c r="N61" s="48"/>
     </row>
     <row r="62" spans="2:14" ht="15">
-      <c r="B62" s="42"/>
-      <c r="C62" s="42"/>
-      <c r="D62" s="45"/>
-      <c r="E62" s="47"/>
-      <c r="F62" s="47"/>
-      <c r="G62" s="47"/>
-      <c r="H62" s="48"/>
-      <c r="I62" s="47"/>
-      <c r="J62" s="47"/>
-      <c r="K62" s="48"/>
-      <c r="L62" s="42"/>
-      <c r="M62" s="45"/>
-      <c r="N62" s="50"/>
+      <c r="B62" s="40"/>
+      <c r="C62" s="40"/>
+      <c r="D62" s="43"/>
+      <c r="E62" s="45"/>
+      <c r="F62" s="45"/>
+      <c r="G62" s="45"/>
+      <c r="H62" s="46"/>
+      <c r="I62" s="45"/>
+      <c r="J62" s="45"/>
+      <c r="K62" s="46"/>
+      <c r="L62" s="40"/>
+      <c r="M62" s="43"/>
+      <c r="N62" s="48"/>
     </row>
     <row r="63" spans="2:14" ht="14.25">
-      <c r="B63" s="115"/>
-      <c r="C63" s="115"/>
-      <c r="D63" s="116"/>
-      <c r="E63" s="47"/>
-      <c r="F63" s="47"/>
-      <c r="G63" s="47"/>
-      <c r="H63" s="48"/>
-      <c r="I63" s="47"/>
-      <c r="J63" s="47"/>
-      <c r="K63" s="48"/>
-      <c r="L63" s="48"/>
-      <c r="M63" s="49"/>
-      <c r="N63" s="50"/>
+      <c r="B63" s="121"/>
+      <c r="C63" s="121"/>
+      <c r="D63" s="122"/>
+      <c r="E63" s="45"/>
+      <c r="F63" s="45"/>
+      <c r="G63" s="45"/>
+      <c r="H63" s="46"/>
+      <c r="I63" s="45"/>
+      <c r="J63" s="45"/>
+      <c r="K63" s="46"/>
+      <c r="L63" s="46"/>
+      <c r="M63" s="47"/>
+      <c r="N63" s="48"/>
     </row>
     <row r="64" spans="2:14" ht="14.25">
-      <c r="B64" s="46"/>
-      <c r="C64" s="46"/>
-      <c r="D64" s="47"/>
-      <c r="E64" s="47"/>
-      <c r="F64" s="47"/>
-      <c r="G64" s="47"/>
-      <c r="H64" s="48"/>
-      <c r="I64" s="47"/>
-      <c r="J64" s="47"/>
-      <c r="K64" s="48"/>
-      <c r="L64" s="48"/>
-      <c r="M64" s="49"/>
-      <c r="N64" s="50"/>
+      <c r="B64" s="44"/>
+      <c r="C64" s="44"/>
+      <c r="D64" s="45"/>
+      <c r="E64" s="45"/>
+      <c r="F64" s="45"/>
+      <c r="G64" s="45"/>
+      <c r="H64" s="46"/>
+      <c r="I64" s="45"/>
+      <c r="J64" s="45"/>
+      <c r="K64" s="46"/>
+      <c r="L64" s="46"/>
+      <c r="M64" s="47"/>
+      <c r="N64" s="48"/>
     </row>
     <row r="65" spans="2:14" ht="14.25">
-      <c r="B65" s="46"/>
-      <c r="C65" s="46"/>
-      <c r="D65" s="47"/>
-      <c r="E65" s="47"/>
-      <c r="F65" s="47"/>
-      <c r="G65" s="47"/>
-      <c r="H65" s="48"/>
-      <c r="I65" s="47"/>
-      <c r="J65" s="47"/>
-      <c r="K65" s="48"/>
-      <c r="L65" s="48"/>
-      <c r="M65" s="49"/>
-      <c r="N65" s="50"/>
+      <c r="B65" s="44"/>
+      <c r="C65" s="44"/>
+      <c r="D65" s="45"/>
+      <c r="E65" s="45"/>
+      <c r="F65" s="45"/>
+      <c r="G65" s="45"/>
+      <c r="H65" s="46"/>
+      <c r="I65" s="45"/>
+      <c r="J65" s="45"/>
+      <c r="K65" s="46"/>
+      <c r="L65" s="46"/>
+      <c r="M65" s="47"/>
+      <c r="N65" s="48"/>
     </row>
     <row r="66" spans="2:14" ht="14.25">
-      <c r="B66" s="46"/>
-      <c r="C66" s="46"/>
-      <c r="D66" s="47"/>
-      <c r="E66" s="47"/>
-      <c r="F66" s="47"/>
-      <c r="G66" s="47"/>
-      <c r="H66" s="48"/>
-      <c r="I66" s="47"/>
-      <c r="J66" s="47"/>
-      <c r="K66" s="48"/>
-      <c r="L66" s="48"/>
-      <c r="M66" s="49"/>
-      <c r="N66" s="50"/>
+      <c r="B66" s="44"/>
+      <c r="C66" s="44"/>
+      <c r="D66" s="45"/>
+      <c r="E66" s="45"/>
+      <c r="F66" s="45"/>
+      <c r="G66" s="45"/>
+      <c r="H66" s="46"/>
+      <c r="I66" s="45"/>
+      <c r="J66" s="45"/>
+      <c r="K66" s="46"/>
+      <c r="L66" s="46"/>
+      <c r="M66" s="47"/>
+      <c r="N66" s="48"/>
     </row>
     <row r="67" spans="2:14" ht="14.25">
-      <c r="B67" s="46"/>
-      <c r="C67" s="46"/>
-      <c r="D67" s="47"/>
-      <c r="E67" s="47"/>
-      <c r="F67" s="47"/>
-      <c r="G67" s="47"/>
-      <c r="H67" s="48"/>
-      <c r="I67" s="47"/>
-      <c r="J67" s="47"/>
-      <c r="K67" s="48"/>
-      <c r="L67" s="48"/>
-      <c r="M67" s="49"/>
-      <c r="N67" s="50"/>
+      <c r="B67" s="44"/>
+      <c r="C67" s="44"/>
+      <c r="D67" s="45"/>
+      <c r="E67" s="45"/>
+      <c r="F67" s="45"/>
+      <c r="G67" s="45"/>
+      <c r="H67" s="46"/>
+      <c r="I67" s="45"/>
+      <c r="J67" s="45"/>
+      <c r="K67" s="46"/>
+      <c r="L67" s="46"/>
+      <c r="M67" s="47"/>
+      <c r="N67" s="48"/>
     </row>
     <row r="68" spans="2:14" ht="14.25">
-      <c r="B68" s="46"/>
-      <c r="C68" s="46"/>
-      <c r="D68" s="47"/>
-      <c r="E68" s="47"/>
-      <c r="F68" s="47"/>
-      <c r="G68" s="47"/>
-      <c r="H68" s="48"/>
-      <c r="I68" s="47"/>
-      <c r="J68" s="47"/>
-      <c r="K68" s="48"/>
-      <c r="L68" s="48"/>
-      <c r="M68" s="49"/>
-      <c r="N68" s="50"/>
+      <c r="B68" s="44"/>
+      <c r="C68" s="44"/>
+      <c r="D68" s="45"/>
+      <c r="E68" s="45"/>
+      <c r="F68" s="45"/>
+      <c r="G68" s="45"/>
+      <c r="H68" s="46"/>
+      <c r="I68" s="45"/>
+      <c r="J68" s="45"/>
+      <c r="K68" s="46"/>
+      <c r="L68" s="46"/>
+      <c r="M68" s="47"/>
+      <c r="N68" s="48"/>
     </row>
     <row r="69" spans="2:14" ht="15">
-      <c r="B69" s="137"/>
-      <c r="C69" s="137"/>
-      <c r="D69" s="137"/>
-      <c r="E69" s="47"/>
-      <c r="F69" s="47"/>
-      <c r="G69" s="47"/>
-      <c r="H69" s="48"/>
-      <c r="I69" s="47"/>
-      <c r="J69" s="47"/>
-      <c r="K69" s="48"/>
-      <c r="L69" s="48"/>
-      <c r="M69" s="49"/>
-      <c r="N69" s="50"/>
+      <c r="B69" s="143"/>
+      <c r="C69" s="143"/>
+      <c r="D69" s="143"/>
+      <c r="E69" s="45"/>
+      <c r="F69" s="45"/>
+      <c r="G69" s="45"/>
+      <c r="H69" s="46"/>
+      <c r="I69" s="45"/>
+      <c r="J69" s="45"/>
+      <c r="K69" s="46"/>
+      <c r="L69" s="46"/>
+      <c r="M69" s="47"/>
+      <c r="N69" s="48"/>
     </row>
     <row r="70" spans="2:14" ht="14.25">
-      <c r="B70" s="46"/>
-      <c r="C70" s="46"/>
-      <c r="D70" s="47"/>
-      <c r="E70" s="47"/>
-      <c r="F70" s="47"/>
-      <c r="G70" s="47"/>
-      <c r="H70" s="48"/>
-      <c r="I70" s="47"/>
-      <c r="J70" s="47"/>
-      <c r="K70" s="48"/>
-      <c r="L70" s="48"/>
-      <c r="M70" s="49"/>
-      <c r="N70" s="50"/>
+      <c r="B70" s="44"/>
+      <c r="C70" s="44"/>
+      <c r="D70" s="45"/>
+      <c r="E70" s="45"/>
+      <c r="F70" s="45"/>
+      <c r="G70" s="45"/>
+      <c r="H70" s="46"/>
+      <c r="I70" s="45"/>
+      <c r="J70" s="45"/>
+      <c r="K70" s="46"/>
+      <c r="L70" s="46"/>
+      <c r="M70" s="47"/>
+      <c r="N70" s="48"/>
     </row>
     <row r="71" spans="2:14" ht="15">
-      <c r="B71" s="53"/>
-      <c r="C71" s="53"/>
-      <c r="D71" s="52"/>
-      <c r="E71" s="47"/>
-      <c r="F71" s="47"/>
-      <c r="G71" s="54"/>
-      <c r="H71" s="48"/>
-      <c r="I71" s="47"/>
-      <c r="J71" s="54"/>
-      <c r="K71" s="48"/>
-      <c r="L71" s="48"/>
-      <c r="M71" s="49"/>
-      <c r="N71" s="49"/>
+      <c r="B71" s="51"/>
+      <c r="C71" s="51"/>
+      <c r="D71" s="50"/>
+      <c r="E71" s="45"/>
+      <c r="F71" s="45"/>
+      <c r="G71" s="52"/>
+      <c r="H71" s="46"/>
+      <c r="I71" s="45"/>
+      <c r="J71" s="52"/>
+      <c r="K71" s="46"/>
+      <c r="L71" s="46"/>
+      <c r="M71" s="47"/>
+      <c r="N71" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="30">

</xml_diff>